<commit_message>
Streamlined the pipelines to be error-free.
</commit_message>
<xml_diff>
--- a/DATA/collate_cultivar_data/data/Smoothed_kcp_trend_vs_datetime.xlsx
+++ b/DATA/collate_cultivar_data/data/Smoothed_kcp_trend_vs_datetime.xlsx
@@ -402,7 +402,7 @@
         <v>42917</v>
       </c>
       <c r="B2">
-        <v>0.08549950000000001</v>
+        <v>0.1093286</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -410,7 +410,7 @@
         <v>42918</v>
       </c>
       <c r="B3">
-        <v>0.08549950000000001</v>
+        <v>0.1094491</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -418,7 +418,7 @@
         <v>42919</v>
       </c>
       <c r="B4">
-        <v>0.08549950000000001</v>
+        <v>0.1095677</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -426,7 +426,7 @@
         <v>42920</v>
       </c>
       <c r="B5">
-        <v>0.08549950000000001</v>
+        <v>0.1096842</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -434,7 +434,7 @@
         <v>42921</v>
       </c>
       <c r="B6">
-        <v>0.08549950000000001</v>
+        <v>0.1097986</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -442,7 +442,7 @@
         <v>42922</v>
       </c>
       <c r="B7">
-        <v>0.08549950000000001</v>
+        <v>0.1099107</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -450,7 +450,7 @@
         <v>42923</v>
       </c>
       <c r="B8">
-        <v>0.08549950000000001</v>
+        <v>0.1100204</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -458,7 +458,7 @@
         <v>42924</v>
       </c>
       <c r="B9">
-        <v>0.08549950000000001</v>
+        <v>0.1101278</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -466,7 +466,7 @@
         <v>42925</v>
       </c>
       <c r="B10">
-        <v>0.08549950000000001</v>
+        <v>0.1102327</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -474,7 +474,7 @@
         <v>42926</v>
       </c>
       <c r="B11">
-        <v>0.08549950000000001</v>
+        <v>0.1103351</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -482,7 +482,7 @@
         <v>42927</v>
       </c>
       <c r="B12">
-        <v>0.08549950000000001</v>
+        <v>0.1104351</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -490,7 +490,7 @@
         <v>42928</v>
       </c>
       <c r="B13">
-        <v>0.08549950000000001</v>
+        <v>0.1105325</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -498,7 +498,7 @@
         <v>42929</v>
       </c>
       <c r="B14">
-        <v>0.08549950000000001</v>
+        <v>0.1106275</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -506,7 +506,7 @@
         <v>42930</v>
       </c>
       <c r="B15">
-        <v>0.08549950000000001</v>
+        <v>0.11072</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -514,7 +514,7 @@
         <v>42931</v>
       </c>
       <c r="B16">
-        <v>0.08549950000000001</v>
+        <v>0.1108102</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -522,7 +522,7 @@
         <v>42932</v>
       </c>
       <c r="B17">
-        <v>0.08549950000000001</v>
+        <v>0.1108981</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -530,7 +530,7 @@
         <v>42933</v>
       </c>
       <c r="B18">
-        <v>0.08549950000000001</v>
+        <v>0.1109837</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -538,7 +538,7 @@
         <v>42934</v>
       </c>
       <c r="B19">
-        <v>0.08549950000000001</v>
+        <v>0.1110673</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -546,7 +546,7 @@
         <v>42935</v>
       </c>
       <c r="B20">
-        <v>0.08549950000000001</v>
+        <v>0.1111489</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -554,7 +554,7 @@
         <v>42936</v>
       </c>
       <c r="B21">
-        <v>0.08549950000000001</v>
+        <v>0.1112287</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -562,7 +562,7 @@
         <v>42937</v>
       </c>
       <c r="B22">
-        <v>0.08549950000000001</v>
+        <v>0.1113068</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -570,7 +570,7 @@
         <v>42938</v>
       </c>
       <c r="B23">
-        <v>0.08549950000000001</v>
+        <v>0.1113835</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -578,7 +578,7 @@
         <v>42939</v>
       </c>
       <c r="B24">
-        <v>0.08549950000000001</v>
+        <v>0.1114591</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -586,7 +586,7 @@
         <v>42940</v>
       </c>
       <c r="B25">
-        <v>0.08549950000000001</v>
+        <v>0.1115336</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -594,7 +594,7 @@
         <v>42941</v>
       </c>
       <c r="B26">
-        <v>0.08549950000000001</v>
+        <v>0.1116074</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -602,7 +602,7 @@
         <v>42942</v>
       </c>
       <c r="B27">
-        <v>0.08549950000000001</v>
+        <v>0.1116807</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -610,7 +610,7 @@
         <v>42943</v>
       </c>
       <c r="B28">
-        <v>0.08549950000000001</v>
+        <v>0.1117539</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -618,7 +618,7 @@
         <v>42944</v>
       </c>
       <c r="B29">
-        <v>0.08549950000000001</v>
+        <v>0.1118272</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -626,7 +626,7 @@
         <v>42945</v>
       </c>
       <c r="B30">
-        <v>0.08549950000000001</v>
+        <v>0.111901</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -634,7 +634,7 @@
         <v>42946</v>
       </c>
       <c r="B31">
-        <v>0.08549950000000001</v>
+        <v>0.1119756</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -642,7 +642,7 @@
         <v>42947</v>
       </c>
       <c r="B32">
-        <v>0.08549950000000001</v>
+        <v>0.1120514</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -650,7 +650,7 @@
         <v>42948</v>
       </c>
       <c r="B33">
-        <v>0.08549950000000001</v>
+        <v>0.1121288</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -658,7 +658,7 @@
         <v>42949</v>
       </c>
       <c r="B34">
-        <v>0.08549950000000001</v>
+        <v>0.112208</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -666,7 +666,7 @@
         <v>42950</v>
       </c>
       <c r="B35">
-        <v>0.08549950000000001</v>
+        <v>0.1122896</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -674,7 +674,7 @@
         <v>42951</v>
       </c>
       <c r="B36">
-        <v>0.08549950000000001</v>
+        <v>0.112374</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -682,7 +682,7 @@
         <v>42952</v>
       </c>
       <c r="B37">
-        <v>0.08549950000000001</v>
+        <v>0.1124616</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -690,7 +690,7 @@
         <v>42953</v>
       </c>
       <c r="B38">
-        <v>0.08549950000000001</v>
+        <v>0.1125529</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -698,7 +698,7 @@
         <v>42954</v>
       </c>
       <c r="B39">
-        <v>0.08549950000000001</v>
+        <v>0.1126483</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -706,7 +706,7 @@
         <v>42955</v>
       </c>
       <c r="B40">
-        <v>0.08549950000000001</v>
+        <v>0.1127483</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -714,7 +714,7 @@
         <v>42956</v>
       </c>
       <c r="B41">
-        <v>0.08549950000000001</v>
+        <v>0.1128533</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -722,7 +722,7 @@
         <v>42957</v>
       </c>
       <c r="B42">
-        <v>0.08549950000000001</v>
+        <v>0.112964</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -730,7 +730,7 @@
         <v>42958</v>
       </c>
       <c r="B43">
-        <v>0.08549950000000001</v>
+        <v>0.1130807</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -738,7 +738,7 @@
         <v>42959</v>
       </c>
       <c r="B44">
-        <v>0.08549950000000001</v>
+        <v>0.1132041</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -746,7 +746,7 @@
         <v>42960</v>
       </c>
       <c r="B45">
-        <v>0.08549950000000001</v>
+        <v>0.1133346</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -754,7 +754,7 @@
         <v>42961</v>
       </c>
       <c r="B46">
-        <v>0.08549950000000001</v>
+        <v>0.1134729</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -762,7 +762,7 @@
         <v>42962</v>
       </c>
       <c r="B47">
-        <v>0.08549950000000001</v>
+        <v>0.1136194</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -770,7 +770,7 @@
         <v>42963</v>
       </c>
       <c r="B48">
-        <v>0.08549950000000001</v>
+        <v>0.1137747</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -778,7 +778,7 @@
         <v>42964</v>
       </c>
       <c r="B49">
-        <v>0.08549950000000001</v>
+        <v>0.1139395</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -786,7 +786,7 @@
         <v>42965</v>
       </c>
       <c r="B50">
-        <v>0.08549950000000001</v>
+        <v>0.1141143</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -794,7 +794,7 @@
         <v>42966</v>
       </c>
       <c r="B51">
-        <v>0.08549950000000001</v>
+        <v>0.1142998</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -802,7 +802,7 @@
         <v>42967</v>
       </c>
       <c r="B52">
-        <v>0.08549950000000001</v>
+        <v>0.1144965</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -810,7 +810,7 @@
         <v>42968</v>
       </c>
       <c r="B53">
-        <v>0.08549950000000001</v>
+        <v>0.114705</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -818,7 +818,7 @@
         <v>42969</v>
       </c>
       <c r="B54">
-        <v>0.08549950000000001</v>
+        <v>0.1149261</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -826,7 +826,7 @@
         <v>42970</v>
       </c>
       <c r="B55">
-        <v>0.0855216</v>
+        <v>0.1151604</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -834,7 +834,7 @@
         <v>42971</v>
       </c>
       <c r="B56">
-        <v>0.08565440000000001</v>
+        <v>0.1154086</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -842,7 +842,7 @@
         <v>42972</v>
       </c>
       <c r="B57">
-        <v>0.0858959</v>
+        <v>0.1156713</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -850,7 +850,7 @@
         <v>42973</v>
       </c>
       <c r="B58">
-        <v>0.0862443</v>
+        <v>0.1159492</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -858,7 +858,7 @@
         <v>42974</v>
       </c>
       <c r="B59">
-        <v>0.0866975</v>
+        <v>0.1162431</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -866,7 +866,7 @@
         <v>42975</v>
       </c>
       <c r="B60">
-        <v>0.0872535</v>
+        <v>0.1165537</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -874,7 +874,7 @@
         <v>42976</v>
       </c>
       <c r="B61">
-        <v>0.0879104</v>
+        <v>0.1168818</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -882,7 +882,7 @@
         <v>42977</v>
       </c>
       <c r="B62">
-        <v>0.08866640000000001</v>
+        <v>0.1172281</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -890,7 +890,7 @@
         <v>42978</v>
       </c>
       <c r="B63">
-        <v>0.0895193</v>
+        <v>0.1175934</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -898,7 +898,7 @@
         <v>42979</v>
       </c>
       <c r="B64">
-        <v>0.0904674</v>
+        <v>0.1179785</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -906,7 +906,7 @@
         <v>42980</v>
       </c>
       <c r="B65">
-        <v>0.0915088</v>
+        <v>0.1183843</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -914,7 +914,7 @@
         <v>42981</v>
       </c>
       <c r="B66">
-        <v>0.0926415</v>
+        <v>0.1188115</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -922,7 +922,7 @@
         <v>42982</v>
       </c>
       <c r="B67">
-        <v>0.09386369999999999</v>
+        <v>0.1192612</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -930,7 +930,7 @@
         <v>42983</v>
       </c>
       <c r="B68">
-        <v>0.09517349999999999</v>
+        <v>0.1197341</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -938,7 +938,7 @@
         <v>42984</v>
       </c>
       <c r="B69">
-        <v>0.0965691</v>
+        <v>0.1202312</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -946,7 +946,7 @@
         <v>42985</v>
       </c>
       <c r="B70">
-        <v>0.0980486</v>
+        <v>0.1207535</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -954,7 +954,7 @@
         <v>42986</v>
       </c>
       <c r="B71">
-        <v>0.0996102</v>
+        <v>0.1213018</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -962,7 +962,7 @@
         <v>42987</v>
       </c>
       <c r="B72">
-        <v>0.1012521</v>
+        <v>0.1218773</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -970,7 +970,7 @@
         <v>42988</v>
       </c>
       <c r="B73">
-        <v>0.1029724</v>
+        <v>0.1224809</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -978,7 +978,7 @@
         <v>42989</v>
       </c>
       <c r="B74">
-        <v>0.1047695</v>
+        <v>0.1231138</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -986,7 +986,7 @@
         <v>42990</v>
       </c>
       <c r="B75">
-        <v>0.1066414</v>
+        <v>0.1237769</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -994,7 +994,7 @@
         <v>42991</v>
       </c>
       <c r="B76">
-        <v>0.1085865</v>
+        <v>0.1244715</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -1002,7 +1002,7 @@
         <v>42992</v>
       </c>
       <c r="B77">
-        <v>0.110603</v>
+        <v>0.1251986</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -1010,7 +1010,7 @@
         <v>42993</v>
       </c>
       <c r="B78">
-        <v>0.1126891</v>
+        <v>0.1259595</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -1018,7 +1018,7 @@
         <v>42994</v>
       </c>
       <c r="B79">
-        <v>0.1148432</v>
+        <v>0.1267554</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -1026,7 +1026,7 @@
         <v>42995</v>
       </c>
       <c r="B80">
-        <v>0.1170634</v>
+        <v>0.1275875</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -1034,7 +1034,7 @@
         <v>42996</v>
       </c>
       <c r="B81">
-        <v>0.119348</v>
+        <v>0.1284572</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -1042,7 +1042,7 @@
         <v>42997</v>
       </c>
       <c r="B82">
-        <v>0.1216955</v>
+        <v>0.1293658</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -1050,7 +1050,7 @@
         <v>42998</v>
       </c>
       <c r="B83">
-        <v>0.124104</v>
+        <v>0.1303146</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -1058,7 +1058,7 @@
         <v>42999</v>
       </c>
       <c r="B84">
-        <v>0.126572</v>
+        <v>0.131305</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -1066,7 +1066,7 @@
         <v>43000</v>
       </c>
       <c r="B85">
-        <v>0.1290978</v>
+        <v>0.1323386</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -1074,7 +1074,7 @@
         <v>43001</v>
       </c>
       <c r="B86">
-        <v>0.1316796</v>
+        <v>0.1334167</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -1082,7 +1082,7 @@
         <v>43002</v>
       </c>
       <c r="B87">
-        <v>0.1343159</v>
+        <v>0.1345408</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -1090,7 +1090,7 @@
         <v>43003</v>
       </c>
       <c r="B88">
-        <v>0.1370051</v>
+        <v>0.1357126</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -1098,7 +1098,7 @@
         <v>43004</v>
       </c>
       <c r="B89">
-        <v>0.1397455</v>
+        <v>0.1369335</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -1106,7 +1106,7 @@
         <v>43005</v>
       </c>
       <c r="B90">
-        <v>0.1425355</v>
+        <v>0.1382052</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -1114,7 +1114,7 @@
         <v>43006</v>
       </c>
       <c r="B91">
-        <v>0.1453736</v>
+        <v>0.1395294</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -1122,7 +1122,7 @@
         <v>43007</v>
       </c>
       <c r="B92">
-        <v>0.1482581</v>
+        <v>0.1409076</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -1130,7 +1130,7 @@
         <v>43008</v>
       </c>
       <c r="B93">
-        <v>0.1511875</v>
+        <v>0.1423416</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -1138,7 +1138,7 @@
         <v>43009</v>
       </c>
       <c r="B94">
-        <v>0.1541603</v>
+        <v>0.1438331</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -1146,7 +1146,7 @@
         <v>43010</v>
       </c>
       <c r="B95">
-        <v>0.1571749</v>
+        <v>0.1453837</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -1154,7 +1154,7 @@
         <v>43011</v>
       </c>
       <c r="B96">
-        <v>0.1602297</v>
+        <v>0.1469953</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -1162,7 +1162,7 @@
         <v>43012</v>
       </c>
       <c r="B97">
-        <v>0.1633233</v>
+        <v>0.1486695</v>
       </c>
     </row>
     <row r="98" spans="1:2">
@@ -1170,7 +1170,7 @@
         <v>43013</v>
       </c>
       <c r="B98">
-        <v>0.1664542</v>
+        <v>0.1504082</v>
       </c>
     </row>
     <row r="99" spans="1:2">
@@ -1178,7 +1178,7 @@
         <v>43014</v>
       </c>
       <c r="B99">
-        <v>0.1696208</v>
+        <v>0.152213</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -1186,7 +1186,7 @@
         <v>43015</v>
       </c>
       <c r="B100">
-        <v>0.1728216</v>
+        <v>0.1540856</v>
       </c>
     </row>
     <row r="101" spans="1:2">
@@ -1194,7 +1194,7 @@
         <v>43016</v>
       </c>
       <c r="B101">
-        <v>0.1760553</v>
+        <v>0.1560278</v>
       </c>
     </row>
     <row r="102" spans="1:2">
@@ -1202,7 +1202,7 @@
         <v>43017</v>
       </c>
       <c r="B102">
-        <v>0.1793203</v>
+        <v>0.1580411</v>
       </c>
     </row>
     <row r="103" spans="1:2">
@@ -1210,7 +1210,7 @@
         <v>43018</v>
       </c>
       <c r="B103">
-        <v>0.1826152</v>
+        <v>0.1601274</v>
       </c>
     </row>
     <row r="104" spans="1:2">
@@ -1218,7 +1218,7 @@
         <v>43019</v>
       </c>
       <c r="B104">
-        <v>0.1859386</v>
+        <v>0.1622881</v>
       </c>
     </row>
     <row r="105" spans="1:2">
@@ -1226,7 +1226,7 @@
         <v>43020</v>
       </c>
       <c r="B105">
-        <v>0.1892889</v>
+        <v>0.1645247</v>
       </c>
     </row>
     <row r="106" spans="1:2">
@@ -1234,7 +1234,7 @@
         <v>43021</v>
       </c>
       <c r="B106">
-        <v>0.1926649</v>
+        <v>0.1668387</v>
       </c>
     </row>
     <row r="107" spans="1:2">
@@ -1242,7 +1242,7 @@
         <v>43022</v>
       </c>
       <c r="B107">
-        <v>0.1960652</v>
+        <v>0.1692316</v>
       </c>
     </row>
     <row r="108" spans="1:2">
@@ -1250,7 +1250,7 @@
         <v>43023</v>
       </c>
       <c r="B108">
-        <v>0.1994882</v>
+        <v>0.1717044</v>
       </c>
     </row>
     <row r="109" spans="1:2">
@@ -1258,7 +1258,7 @@
         <v>43024</v>
       </c>
       <c r="B109">
-        <v>0.2029327</v>
+        <v>0.1742585</v>
       </c>
     </row>
     <row r="110" spans="1:2">
@@ -1266,7 +1266,7 @@
         <v>43025</v>
       </c>
       <c r="B110">
-        <v>0.2063973</v>
+        <v>0.1768949</v>
       </c>
     </row>
     <row r="111" spans="1:2">
@@ -1274,7 +1274,7 @@
         <v>43026</v>
       </c>
       <c r="B111">
-        <v>0.2098807</v>
+        <v>0.1796145</v>
       </c>
     </row>
     <row r="112" spans="1:2">
@@ -1282,7 +1282,7 @@
         <v>43027</v>
       </c>
       <c r="B112">
-        <v>0.2133814</v>
+        <v>0.182418</v>
       </c>
     </row>
     <row r="113" spans="1:2">
@@ -1290,7 +1290,7 @@
         <v>43028</v>
       </c>
       <c r="B113">
-        <v>0.2168983</v>
+        <v>0.185306</v>
       </c>
     </row>
     <row r="114" spans="1:2">
@@ -1298,7 +1298,7 @@
         <v>43029</v>
       </c>
       <c r="B114">
-        <v>0.2204298</v>
+        <v>0.188279</v>
       </c>
     </row>
     <row r="115" spans="1:2">
@@ -1306,7 +1306,7 @@
         <v>43030</v>
       </c>
       <c r="B115">
-        <v>0.2239749</v>
+        <v>0.1913372</v>
       </c>
     </row>
     <row r="116" spans="1:2">
@@ -1314,7 +1314,7 @@
         <v>43031</v>
       </c>
       <c r="B116">
-        <v>0.2275321</v>
+        <v>0.1944805</v>
       </c>
     </row>
     <row r="117" spans="1:2">
@@ -1322,7 +1322,7 @@
         <v>43032</v>
       </c>
       <c r="B117">
-        <v>0.2311002</v>
+        <v>0.1977089</v>
       </c>
     </row>
     <row r="118" spans="1:2">
@@ -1330,7 +1330,7 @@
         <v>43033</v>
       </c>
       <c r="B118">
-        <v>0.2346778</v>
+        <v>0.2010218</v>
       </c>
     </row>
     <row r="119" spans="1:2">
@@ -1338,7 +1338,7 @@
         <v>43034</v>
       </c>
       <c r="B119">
-        <v>0.2382639</v>
+        <v>0.2044187</v>
       </c>
     </row>
     <row r="120" spans="1:2">
@@ -1346,7 +1346,7 @@
         <v>43035</v>
       </c>
       <c r="B120">
-        <v>0.241857</v>
+        <v>0.2078984</v>
       </c>
     </row>
     <row r="121" spans="1:2">
@@ -1354,7 +1354,7 @@
         <v>43036</v>
       </c>
       <c r="B121">
-        <v>0.245456</v>
+        <v>0.2114599</v>
       </c>
     </row>
     <row r="122" spans="1:2">
@@ -1362,7 +1362,7 @@
         <v>43037</v>
       </c>
       <c r="B122">
-        <v>0.2490597</v>
+        <v>0.2151017</v>
       </c>
     </row>
     <row r="123" spans="1:2">
@@ -1370,7 +1370,7 @@
         <v>43038</v>
       </c>
       <c r="B123">
-        <v>0.2526669</v>
+        <v>0.218822</v>
       </c>
     </row>
     <row r="124" spans="1:2">
@@ -1378,7 +1378,7 @@
         <v>43039</v>
       </c>
       <c r="B124">
-        <v>0.2562762</v>
+        <v>0.2226188</v>
       </c>
     </row>
     <row r="125" spans="1:2">
@@ -1386,7 +1386,7 @@
         <v>43040</v>
       </c>
       <c r="B125">
-        <v>0.2598867</v>
+        <v>0.2264897</v>
       </c>
     </row>
     <row r="126" spans="1:2">
@@ -1394,7 +1394,7 @@
         <v>43041</v>
       </c>
       <c r="B126">
-        <v>0.263497</v>
+        <v>0.2304322</v>
       </c>
     </row>
     <row r="127" spans="1:2">
@@ -1402,7 +1402,7 @@
         <v>43042</v>
       </c>
       <c r="B127">
-        <v>0.267106</v>
+        <v>0.2344433</v>
       </c>
     </row>
     <row r="128" spans="1:2">
@@ -1410,7 +1410,7 @@
         <v>43043</v>
       </c>
       <c r="B128">
-        <v>0.2707127</v>
+        <v>0.2385199</v>
       </c>
     </row>
     <row r="129" spans="1:2">
@@ -1418,7 +1418,7 @@
         <v>43044</v>
       </c>
       <c r="B129">
-        <v>0.2743157</v>
+        <v>0.2426585</v>
       </c>
     </row>
     <row r="130" spans="1:2">
@@ -1426,7 +1426,7 @@
         <v>43045</v>
       </c>
       <c r="B130">
-        <v>0.2779141</v>
+        <v>0.2468553</v>
       </c>
     </row>
     <row r="131" spans="1:2">
@@ -1434,7 +1434,7 @@
         <v>43046</v>
       </c>
       <c r="B131">
-        <v>0.2815067</v>
+        <v>0.2511066</v>
       </c>
     </row>
     <row r="132" spans="1:2">
@@ -1442,7 +1442,7 @@
         <v>43047</v>
       </c>
       <c r="B132">
-        <v>0.2850924</v>
+        <v>0.2554079</v>
       </c>
     </row>
     <row r="133" spans="1:2">
@@ -1450,7 +1450,7 @@
         <v>43048</v>
       </c>
       <c r="B133">
-        <v>0.28867</v>
+        <v>0.259755</v>
       </c>
     </row>
     <row r="134" spans="1:2">
@@ -1458,7 +1458,7 @@
         <v>43049</v>
       </c>
       <c r="B134">
-        <v>0.2922387</v>
+        <v>0.2641432</v>
       </c>
     </row>
     <row r="135" spans="1:2">
@@ -1466,7 +1466,7 @@
         <v>43050</v>
       </c>
       <c r="B135">
-        <v>0.2957971</v>
+        <v>0.2685676</v>
       </c>
     </row>
     <row r="136" spans="1:2">
@@ -1474,7 +1474,7 @@
         <v>43051</v>
       </c>
       <c r="B136">
-        <v>0.2993444</v>
+        <v>0.2730235</v>
       </c>
     </row>
     <row r="137" spans="1:2">
@@ -1482,7 +1482,7 @@
         <v>43052</v>
       </c>
       <c r="B137">
-        <v>0.3028794</v>
+        <v>0.2775057</v>
       </c>
     </row>
     <row r="138" spans="1:2">
@@ -1490,7 +1490,7 @@
         <v>43053</v>
       </c>
       <c r="B138">
-        <v>0.3064012</v>
+        <v>0.2820089</v>
       </c>
     </row>
     <row r="139" spans="1:2">
@@ -1498,7 +1498,7 @@
         <v>43054</v>
       </c>
       <c r="B139">
-        <v>0.3099087</v>
+        <v>0.2865281</v>
       </c>
     </row>
     <row r="140" spans="1:2">
@@ -1506,7 +1506,7 @@
         <v>43055</v>
       </c>
       <c r="B140">
-        <v>0.3134009</v>
+        <v>0.2910579</v>
       </c>
     </row>
     <row r="141" spans="1:2">
@@ -1514,7 +1514,7 @@
         <v>43056</v>
       </c>
       <c r="B141">
-        <v>0.3168768</v>
+        <v>0.2955929</v>
       </c>
     </row>
     <row r="142" spans="1:2">
@@ -1522,7 +1522,7 @@
         <v>43057</v>
       </c>
       <c r="B142">
-        <v>0.3203354</v>
+        <v>0.300128</v>
       </c>
     </row>
     <row r="143" spans="1:2">
@@ -1530,7 +1530,7 @@
         <v>43058</v>
       </c>
       <c r="B143">
-        <v>0.3237758</v>
+        <v>0.3046579</v>
       </c>
     </row>
     <row r="144" spans="1:2">
@@ -1538,7 +1538,7 @@
         <v>43059</v>
       </c>
       <c r="B144">
-        <v>0.327197</v>
+        <v>0.3091773</v>
       </c>
     </row>
     <row r="145" spans="1:2">
@@ -1546,7 +1546,7 @@
         <v>43060</v>
       </c>
       <c r="B145">
-        <v>0.330598</v>
+        <v>0.3136813</v>
       </c>
     </row>
     <row r="146" spans="1:2">
@@ -1554,7 +1554,7 @@
         <v>43061</v>
       </c>
       <c r="B146">
-        <v>0.333978</v>
+        <v>0.3181649</v>
       </c>
     </row>
     <row r="147" spans="1:2">
@@ -1562,7 +1562,7 @@
         <v>43062</v>
       </c>
       <c r="B147">
-        <v>0.3373359</v>
+        <v>0.3226233</v>
       </c>
     </row>
     <row r="148" spans="1:2">
@@ -1570,7 +1570,7 @@
         <v>43063</v>
       </c>
       <c r="B148">
-        <v>0.3406709</v>
+        <v>0.3270519</v>
       </c>
     </row>
     <row r="149" spans="1:2">
@@ -1578,7 +1578,7 @@
         <v>43064</v>
       </c>
       <c r="B149">
-        <v>0.3439821</v>
+        <v>0.3314461</v>
       </c>
     </row>
     <row r="150" spans="1:2">
@@ -1586,7 +1586,7 @@
         <v>43065</v>
       </c>
       <c r="B150">
-        <v>0.3472686</v>
+        <v>0.335802</v>
       </c>
     </row>
     <row r="151" spans="1:2">
@@ -1594,7 +1594,7 @@
         <v>43066</v>
       </c>
       <c r="B151">
-        <v>0.3505295</v>
+        <v>0.3401153</v>
       </c>
     </row>
     <row r="152" spans="1:2">
@@ -1602,7 +1602,7 @@
         <v>43067</v>
       </c>
       <c r="B152">
-        <v>0.3537639</v>
+        <v>0.3443824</v>
       </c>
     </row>
     <row r="153" spans="1:2">
@@ -1610,7 +1610,7 @@
         <v>43068</v>
       </c>
       <c r="B153">
-        <v>0.3569711</v>
+        <v>0.3485997</v>
       </c>
     </row>
     <row r="154" spans="1:2">
@@ -1618,7 +1618,7 @@
         <v>43069</v>
       </c>
       <c r="B154">
-        <v>0.3601501</v>
+        <v>0.352764</v>
       </c>
     </row>
     <row r="155" spans="1:2">
@@ -1626,7 +1626,7 @@
         <v>43070</v>
       </c>
       <c r="B155">
-        <v>0.3633001</v>
+        <v>0.3568724</v>
       </c>
     </row>
     <row r="156" spans="1:2">
@@ -1634,7 +1634,7 @@
         <v>43071</v>
       </c>
       <c r="B156">
-        <v>0.3664203</v>
+        <v>0.360922</v>
       </c>
     </row>
     <row r="157" spans="1:2">
@@ -1642,7 +1642,7 @@
         <v>43072</v>
       </c>
       <c r="B157">
-        <v>0.36951</v>
+        <v>0.3649104</v>
       </c>
     </row>
     <row r="158" spans="1:2">
@@ -1650,7 +1650,7 @@
         <v>43073</v>
       </c>
       <c r="B158">
-        <v>0.3725682</v>
+        <v>0.3688355</v>
       </c>
     </row>
     <row r="159" spans="1:2">
@@ -1658,7 +1658,7 @@
         <v>43074</v>
       </c>
       <c r="B159">
-        <v>0.3755943</v>
+        <v>0.3726953</v>
       </c>
     </row>
     <row r="160" spans="1:2">
@@ -1666,7 +1666,7 @@
         <v>43075</v>
       </c>
       <c r="B160">
-        <v>0.3785874</v>
+        <v>0.3764881</v>
       </c>
     </row>
     <row r="161" spans="1:2">
@@ -1674,7 +1674,7 @@
         <v>43076</v>
       </c>
       <c r="B161">
-        <v>0.3815469</v>
+        <v>0.3802124</v>
       </c>
     </row>
     <row r="162" spans="1:2">
@@ -1682,7 +1682,7 @@
         <v>43077</v>
       </c>
       <c r="B162">
-        <v>0.3844718</v>
+        <v>0.3838672</v>
       </c>
     </row>
     <row r="163" spans="1:2">
@@ -1690,7 +1690,7 @@
         <v>43078</v>
       </c>
       <c r="B163">
-        <v>0.3873617</v>
+        <v>0.3874515</v>
       </c>
     </row>
     <row r="164" spans="1:2">
@@ -1698,7 +1698,7 @@
         <v>43079</v>
       </c>
       <c r="B164">
-        <v>0.3902156</v>
+        <v>0.3909644</v>
       </c>
     </row>
     <row r="165" spans="1:2">
@@ -1706,7 +1706,7 @@
         <v>43080</v>
       </c>
       <c r="B165">
-        <v>0.3930329</v>
+        <v>0.3944056</v>
       </c>
     </row>
     <row r="166" spans="1:2">
@@ -1714,7 +1714,7 @@
         <v>43081</v>
       </c>
       <c r="B166">
-        <v>0.3958129</v>
+        <v>0.3977746</v>
       </c>
     </row>
     <row r="167" spans="1:2">
@@ -1722,7 +1722,7 @@
         <v>43082</v>
       </c>
       <c r="B167">
-        <v>0.3985549</v>
+        <v>0.4010713</v>
       </c>
     </row>
     <row r="168" spans="1:2">
@@ -1730,7 +1730,7 @@
         <v>43083</v>
       </c>
       <c r="B168">
-        <v>0.4012583</v>
+        <v>0.4042957</v>
       </c>
     </row>
     <row r="169" spans="1:2">
@@ -1738,7 +1738,7 @@
         <v>43084</v>
       </c>
       <c r="B169">
-        <v>0.4039223</v>
+        <v>0.407448</v>
       </c>
     </row>
     <row r="170" spans="1:2">
@@ -1746,7 +1746,7 @@
         <v>43085</v>
       </c>
       <c r="B170">
-        <v>0.4065464</v>
+        <v>0.4105285</v>
       </c>
     </row>
     <row r="171" spans="1:2">
@@ -1754,7 +1754,7 @@
         <v>43086</v>
       </c>
       <c r="B171">
-        <v>0.4091298</v>
+        <v>0.4135376</v>
       </c>
     </row>
     <row r="172" spans="1:2">
@@ -1762,7 +1762,7 @@
         <v>43087</v>
       </c>
       <c r="B172">
-        <v>0.411672</v>
+        <v>0.416476</v>
       </c>
     </row>
     <row r="173" spans="1:2">
@@ -1770,7 +1770,7 @@
         <v>43088</v>
       </c>
       <c r="B173">
-        <v>0.4141723</v>
+        <v>0.4193442</v>
       </c>
     </row>
     <row r="174" spans="1:2">
@@ -1778,7 +1778,7 @@
         <v>43089</v>
       </c>
       <c r="B174">
-        <v>0.4166302</v>
+        <v>0.422143</v>
       </c>
     </row>
     <row r="175" spans="1:2">
@@ -1786,7 +1786,7 @@
         <v>43090</v>
       </c>
       <c r="B175">
-        <v>0.419045</v>
+        <v>0.4248733</v>
       </c>
     </row>
     <row r="176" spans="1:2">
@@ -1794,7 +1794,7 @@
         <v>43091</v>
       </c>
       <c r="B176">
-        <v>0.4214162</v>
+        <v>0.4275358</v>
       </c>
     </row>
     <row r="177" spans="1:2">
@@ -1802,7 +1802,7 @@
         <v>43092</v>
       </c>
       <c r="B177">
-        <v>0.4237432</v>
+        <v>0.4301317</v>
       </c>
     </row>
     <row r="178" spans="1:2">
@@ -1810,7 +1810,7 @@
         <v>43093</v>
       </c>
       <c r="B178">
-        <v>0.4260254</v>
+        <v>0.4326618</v>
       </c>
     </row>
     <row r="179" spans="1:2">
@@ -1818,7 +1818,7 @@
         <v>43094</v>
       </c>
       <c r="B179">
-        <v>0.4282624</v>
+        <v>0.4351272</v>
       </c>
     </row>
     <row r="180" spans="1:2">
@@ -1826,7 +1826,7 @@
         <v>43095</v>
       </c>
       <c r="B180">
-        <v>0.4304535</v>
+        <v>0.437529</v>
       </c>
     </row>
     <row r="181" spans="1:2">
@@ -1834,7 +1834,7 @@
         <v>43096</v>
       </c>
       <c r="B181">
-        <v>0.4325983</v>
+        <v>0.4398682</v>
       </c>
     </row>
     <row r="182" spans="1:2">
@@ -1842,7 +1842,7 @@
         <v>43097</v>
       </c>
       <c r="B182">
-        <v>0.4346962</v>
+        <v>0.4421459</v>
       </c>
     </row>
     <row r="183" spans="1:2">
@@ -1850,7 +1850,7 @@
         <v>43098</v>
       </c>
       <c r="B183">
-        <v>0.4367467</v>
+        <v>0.4443633</v>
       </c>
     </row>
     <row r="184" spans="1:2">
@@ -1858,7 +1858,7 @@
         <v>43099</v>
       </c>
       <c r="B184">
-        <v>0.4387495</v>
+        <v>0.4465213</v>
       </c>
     </row>
     <row r="185" spans="1:2">
@@ -1866,7 +1866,7 @@
         <v>43100</v>
       </c>
       <c r="B185">
-        <v>0.4407039</v>
+        <v>0.4486211</v>
       </c>
     </row>
     <row r="186" spans="1:2">
@@ -1874,7 +1874,7 @@
         <v>43101</v>
       </c>
       <c r="B186">
-        <v>0.4426095</v>
+        <v>0.4506638</v>
       </c>
     </row>
     <row r="187" spans="1:2">
@@ -1882,7 +1882,7 @@
         <v>43102</v>
       </c>
       <c r="B187">
-        <v>0.444466</v>
+        <v>0.4526504</v>
       </c>
     </row>
     <row r="188" spans="1:2">
@@ -1890,7 +1890,7 @@
         <v>43103</v>
       </c>
       <c r="B188">
-        <v>0.4462727</v>
+        <v>0.4545819</v>
       </c>
     </row>
     <row r="189" spans="1:2">
@@ -1898,7 +1898,7 @@
         <v>43104</v>
       </c>
       <c r="B189">
-        <v>0.4480295</v>
+        <v>0.4564593</v>
       </c>
     </row>
     <row r="190" spans="1:2">
@@ -1906,7 +1906,7 @@
         <v>43105</v>
       </c>
       <c r="B190">
-        <v>0.4497357</v>
+        <v>0.4582836</v>
       </c>
     </row>
     <row r="191" spans="1:2">
@@ -1914,7 +1914,7 @@
         <v>43106</v>
       </c>
       <c r="B191">
-        <v>0.451391</v>
+        <v>0.4600558</v>
       </c>
     </row>
     <row r="192" spans="1:2">
@@ -1922,7 +1922,7 @@
         <v>43107</v>
       </c>
       <c r="B192">
-        <v>0.4529951</v>
+        <v>0.4617768</v>
       </c>
     </row>
     <row r="193" spans="1:2">
@@ -1930,7 +1930,7 @@
         <v>43108</v>
       </c>
       <c r="B193">
-        <v>0.4545475</v>
+        <v>0.4634473</v>
       </c>
     </row>
     <row r="194" spans="1:2">
@@ -1938,7 +1938,7 @@
         <v>43109</v>
       </c>
       <c r="B194">
-        <v>0.4560479</v>
+        <v>0.4650683</v>
       </c>
     </row>
     <row r="195" spans="1:2">
@@ -1946,7 +1946,7 @@
         <v>43110</v>
       </c>
       <c r="B195">
-        <v>0.4574959</v>
+        <v>0.4666405</v>
       </c>
     </row>
     <row r="196" spans="1:2">
@@ -1954,7 +1954,7 @@
         <v>43111</v>
       </c>
       <c r="B196">
-        <v>0.4588912</v>
+        <v>0.4681647</v>
       </c>
     </row>
     <row r="197" spans="1:2">
@@ -1962,7 +1962,7 @@
         <v>43112</v>
       </c>
       <c r="B197">
-        <v>0.4602334</v>
+        <v>0.4696416</v>
       </c>
     </row>
     <row r="198" spans="1:2">
@@ -1970,7 +1970,7 @@
         <v>43113</v>
       </c>
       <c r="B198">
-        <v>0.4615223</v>
+        <v>0.4710718</v>
       </c>
     </row>
     <row r="199" spans="1:2">
@@ -1978,7 +1978,7 @@
         <v>43114</v>
       </c>
       <c r="B199">
-        <v>0.4627575</v>
+        <v>0.4724559</v>
       </c>
     </row>
     <row r="200" spans="1:2">
@@ -1986,7 +1986,7 @@
         <v>43115</v>
       </c>
       <c r="B200">
-        <v>0.4639388</v>
+        <v>0.4737944</v>
       </c>
     </row>
     <row r="201" spans="1:2">
@@ -1994,7 +1994,7 @@
         <v>43116</v>
       </c>
       <c r="B201">
-        <v>0.4650658</v>
+        <v>0.4750879</v>
       </c>
     </row>
     <row r="202" spans="1:2">
@@ -2002,7 +2002,7 @@
         <v>43117</v>
       </c>
       <c r="B202">
-        <v>0.4661383</v>
+        <v>0.4763367</v>
       </c>
     </row>
     <row r="203" spans="1:2">
@@ -2010,7 +2010,7 @@
         <v>43118</v>
       </c>
       <c r="B203">
-        <v>0.4671561</v>
+        <v>0.4775414</v>
       </c>
     </row>
     <row r="204" spans="1:2">
@@ -2018,7 +2018,7 @@
         <v>43119</v>
       </c>
       <c r="B204">
-        <v>0.4681188</v>
+        <v>0.4787022</v>
       </c>
     </row>
     <row r="205" spans="1:2">
@@ -2026,7 +2026,7 @@
         <v>43120</v>
       </c>
       <c r="B205">
-        <v>0.4690263</v>
+        <v>0.4798193</v>
       </c>
     </row>
     <row r="206" spans="1:2">
@@ -2034,7 +2034,7 @@
         <v>43121</v>
       </c>
       <c r="B206">
-        <v>0.4698783</v>
+        <v>0.4808931</v>
       </c>
     </row>
     <row r="207" spans="1:2">
@@ -2042,7 +2042,7 @@
         <v>43122</v>
       </c>
       <c r="B207">
-        <v>0.4706746</v>
+        <v>0.4819236</v>
       </c>
     </row>
     <row r="208" spans="1:2">
@@ -2050,7 +2050,7 @@
         <v>43123</v>
       </c>
       <c r="B208">
-        <v>0.4714151</v>
+        <v>0.482911</v>
       </c>
     </row>
     <row r="209" spans="1:2">
@@ -2058,7 +2058,7 @@
         <v>43124</v>
       </c>
       <c r="B209">
-        <v>0.4720994</v>
+        <v>0.4838553</v>
       </c>
     </row>
     <row r="210" spans="1:2">
@@ -2066,7 +2066,7 @@
         <v>43125</v>
       </c>
       <c r="B210">
-        <v>0.4727276</v>
+        <v>0.4847566</v>
       </c>
     </row>
     <row r="211" spans="1:2">
@@ -2074,7 +2074,7 @@
         <v>43126</v>
       </c>
       <c r="B211">
-        <v>0.4732993</v>
+        <v>0.4856146</v>
       </c>
     </row>
     <row r="212" spans="1:2">
@@ -2082,7 +2082,7 @@
         <v>43127</v>
       </c>
       <c r="B212">
-        <v>0.4738145</v>
+        <v>0.4864294</v>
       </c>
     </row>
     <row r="213" spans="1:2">
@@ -2090,7 +2090,7 @@
         <v>43128</v>
       </c>
       <c r="B213">
-        <v>0.474273</v>
+        <v>0.4872007</v>
       </c>
     </row>
     <row r="214" spans="1:2">
@@ -2098,7 +2098,7 @@
         <v>43129</v>
       </c>
       <c r="B214">
-        <v>0.4746746</v>
+        <v>0.4879282</v>
       </c>
     </row>
     <row r="215" spans="1:2">
@@ -2106,7 +2106,7 @@
         <v>43130</v>
       </c>
       <c r="B215">
-        <v>0.4750193</v>
+        <v>0.4886117</v>
       </c>
     </row>
     <row r="216" spans="1:2">
@@ -2114,7 +2114,7 @@
         <v>43131</v>
       </c>
       <c r="B216">
-        <v>0.475307</v>
+        <v>0.4892507</v>
       </c>
     </row>
     <row r="217" spans="1:2">
@@ -2122,7 +2122,7 @@
         <v>43132</v>
       </c>
       <c r="B217">
-        <v>0.4755376</v>
+        <v>0.489845</v>
       </c>
     </row>
     <row r="218" spans="1:2">
@@ -2130,7 +2130,7 @@
         <v>43133</v>
       </c>
       <c r="B218">
-        <v>0.4757109</v>
+        <v>0.4903939</v>
       </c>
     </row>
     <row r="219" spans="1:2">
@@ -2138,7 +2138,7 @@
         <v>43134</v>
       </c>
       <c r="B219">
-        <v>0.475827</v>
+        <v>0.4908969</v>
       </c>
     </row>
     <row r="220" spans="1:2">
@@ -2146,7 +2146,7 @@
         <v>43135</v>
       </c>
       <c r="B220">
-        <v>0.4758857</v>
+        <v>0.4913535</v>
       </c>
     </row>
     <row r="221" spans="1:2">
@@ -2154,7 +2154,7 @@
         <v>43136</v>
       </c>
       <c r="B221">
-        <v>0.4758871</v>
+        <v>0.491763</v>
       </c>
     </row>
     <row r="222" spans="1:2">
@@ -2162,7 +2162,7 @@
         <v>43137</v>
       </c>
       <c r="B222">
-        <v>0.475831</v>
+        <v>0.4921248</v>
       </c>
     </row>
     <row r="223" spans="1:2">
@@ -2170,7 +2170,7 @@
         <v>43138</v>
       </c>
       <c r="B223">
-        <v>0.4757175</v>
+        <v>0.4924382</v>
       </c>
     </row>
     <row r="224" spans="1:2">
@@ -2178,7 +2178,7 @@
         <v>43139</v>
       </c>
       <c r="B224">
-        <v>0.4755466</v>
+        <v>0.4927023</v>
       </c>
     </row>
     <row r="225" spans="1:2">
@@ -2186,7 +2186,7 @@
         <v>43140</v>
       </c>
       <c r="B225">
-        <v>0.4753182</v>
+        <v>0.4929165</v>
       </c>
     </row>
     <row r="226" spans="1:2">
@@ -2194,7 +2194,7 @@
         <v>43141</v>
       </c>
       <c r="B226">
-        <v>0.4750324</v>
+        <v>0.4930799</v>
       </c>
     </row>
     <row r="227" spans="1:2">
@@ -2202,7 +2202,7 @@
         <v>43142</v>
       </c>
       <c r="B227">
-        <v>0.4746892</v>
+        <v>0.4931916</v>
       </c>
     </row>
     <row r="228" spans="1:2">
@@ -2210,7 +2210,7 @@
         <v>43143</v>
       </c>
       <c r="B228">
-        <v>0.4742887</v>
+        <v>0.4932509</v>
       </c>
     </row>
     <row r="229" spans="1:2">
@@ -2218,7 +2218,7 @@
         <v>43144</v>
       </c>
       <c r="B229">
-        <v>0.4738309</v>
+        <v>0.4932568</v>
       </c>
     </row>
     <row r="230" spans="1:2">
@@ -2226,7 +2226,7 @@
         <v>43145</v>
       </c>
       <c r="B230">
-        <v>0.4733158</v>
+        <v>0.4932086</v>
       </c>
     </row>
     <row r="231" spans="1:2">
@@ -2234,7 +2234,7 @@
         <v>43146</v>
       </c>
       <c r="B231">
-        <v>0.4727436</v>
+        <v>0.4931054</v>
       </c>
     </row>
     <row r="232" spans="1:2">
@@ -2242,7 +2242,7 @@
         <v>43147</v>
       </c>
       <c r="B232">
-        <v>0.4721143</v>
+        <v>0.4929463</v>
       </c>
     </row>
     <row r="233" spans="1:2">
@@ -2250,7 +2250,7 @@
         <v>43148</v>
       </c>
       <c r="B233">
-        <v>0.471428</v>
+        <v>0.4927307</v>
       </c>
     </row>
     <row r="234" spans="1:2">
@@ -2258,7 +2258,7 @@
         <v>43149</v>
       </c>
       <c r="B234">
-        <v>0.4706848</v>
+        <v>0.4924576</v>
       </c>
     </row>
     <row r="235" spans="1:2">
@@ -2266,7 +2266,7 @@
         <v>43150</v>
       </c>
       <c r="B235">
-        <v>0.4698849</v>
+        <v>0.4921265</v>
       </c>
     </row>
     <row r="236" spans="1:2">
@@ -2274,7 +2274,7 @@
         <v>43151</v>
       </c>
       <c r="B236">
-        <v>0.4690284</v>
+        <v>0.4917367</v>
       </c>
     </row>
     <row r="237" spans="1:2">
@@ -2282,7 +2282,7 @@
         <v>43152</v>
       </c>
       <c r="B237">
-        <v>0.4681155</v>
+        <v>0.4912876</v>
       </c>
     </row>
     <row r="238" spans="1:2">
@@ -2290,7 +2290,7 @@
         <v>43153</v>
       </c>
       <c r="B238">
-        <v>0.4671462</v>
+        <v>0.4907788</v>
       </c>
     </row>
     <row r="239" spans="1:2">
@@ -2298,7 +2298,7 @@
         <v>43154</v>
       </c>
       <c r="B239">
-        <v>0.4661208</v>
+        <v>0.4902097</v>
       </c>
     </row>
     <row r="240" spans="1:2">
@@ -2306,7 +2306,7 @@
         <v>43155</v>
       </c>
       <c r="B240">
-        <v>0.4650394</v>
+        <v>0.4895803</v>
       </c>
     </row>
     <row r="241" spans="1:2">
@@ -2314,7 +2314,7 @@
         <v>43156</v>
       </c>
       <c r="B241">
-        <v>0.4639023</v>
+        <v>0.4888902</v>
       </c>
     </row>
     <row r="242" spans="1:2">
@@ -2322,7 +2322,7 @@
         <v>43157</v>
       </c>
       <c r="B242">
-        <v>0.4627096</v>
+        <v>0.4881395</v>
       </c>
     </row>
     <row r="243" spans="1:2">
@@ -2330,7 +2330,7 @@
         <v>43158</v>
       </c>
       <c r="B243">
-        <v>0.4614616</v>
+        <v>0.4873283</v>
       </c>
     </row>
     <row r="244" spans="1:2">
@@ -2338,7 +2338,7 @@
         <v>43159</v>
       </c>
       <c r="B244">
-        <v>0.4601585</v>
+        <v>0.4864568</v>
       </c>
     </row>
     <row r="245" spans="1:2">
@@ -2346,7 +2346,7 @@
         <v>43160</v>
       </c>
       <c r="B245">
-        <v>0.4588005</v>
+        <v>0.4855254</v>
       </c>
     </row>
     <row r="246" spans="1:2">
@@ -2354,7 +2354,7 @@
         <v>43161</v>
       </c>
       <c r="B246">
-        <v>0.4573879</v>
+        <v>0.4845347</v>
       </c>
     </row>
     <row r="247" spans="1:2">
@@ -2362,7 +2362,7 @@
         <v>43162</v>
       </c>
       <c r="B247">
-        <v>0.455921</v>
+        <v>0.4834856</v>
       </c>
     </row>
     <row r="248" spans="1:2">
@@ -2370,7 +2370,7 @@
         <v>43163</v>
       </c>
       <c r="B248">
-        <v>0.4544</v>
+        <v>0.4823789</v>
       </c>
     </row>
     <row r="249" spans="1:2">
@@ -2378,7 +2378,7 @@
         <v>43164</v>
       </c>
       <c r="B249">
-        <v>0.4528252</v>
+        <v>0.4812157</v>
       </c>
     </row>
     <row r="250" spans="1:2">
@@ -2386,7 +2386,7 @@
         <v>43165</v>
       </c>
       <c r="B250">
-        <v>0.451197</v>
+        <v>0.4799975</v>
       </c>
     </row>
     <row r="251" spans="1:2">
@@ -2394,7 +2394,7 @@
         <v>43166</v>
       </c>
       <c r="B251">
-        <v>0.4495155</v>
+        <v>0.4787257</v>
       </c>
     </row>
     <row r="252" spans="1:2">
@@ -2402,7 +2402,7 @@
         <v>43167</v>
       </c>
       <c r="B252">
-        <v>0.4477813</v>
+        <v>0.4774021</v>
       </c>
     </row>
     <row r="253" spans="1:2">
@@ -2410,7 +2410,7 @@
         <v>43168</v>
       </c>
       <c r="B253">
-        <v>0.4459945</v>
+        <v>0.4760285</v>
       </c>
     </row>
     <row r="254" spans="1:2">
@@ -2418,7 +2418,7 @@
         <v>43169</v>
       </c>
       <c r="B254">
-        <v>0.4441556</v>
+        <v>0.4746071</v>
       </c>
     </row>
     <row r="255" spans="1:2">
@@ -2426,7 +2426,7 @@
         <v>43170</v>
       </c>
       <c r="B255">
-        <v>0.4422649</v>
+        <v>0.4731401</v>
       </c>
     </row>
     <row r="256" spans="1:2">
@@ -2434,7 +2434,7 @@
         <v>43171</v>
       </c>
       <c r="B256">
-        <v>0.4403227</v>
+        <v>0.4716299</v>
       </c>
     </row>
     <row r="257" spans="1:2">
@@ -2442,7 +2442,7 @@
         <v>43172</v>
       </c>
       <c r="B257">
-        <v>0.4383296</v>
+        <v>0.4700793</v>
       </c>
     </row>
     <row r="258" spans="1:2">
@@ -2450,7 +2450,7 @@
         <v>43173</v>
       </c>
       <c r="B258">
-        <v>0.4362858</v>
+        <v>0.4684909</v>
       </c>
     </row>
     <row r="259" spans="1:2">
@@ -2458,7 +2458,7 @@
         <v>43174</v>
       </c>
       <c r="B259">
-        <v>0.4341917</v>
+        <v>0.4668677</v>
       </c>
     </row>
     <row r="260" spans="1:2">
@@ -2466,7 +2466,7 @@
         <v>43175</v>
       </c>
       <c r="B260">
-        <v>0.4320478</v>
+        <v>0.4652126</v>
       </c>
     </row>
     <row r="261" spans="1:2">
@@ -2474,7 +2474,7 @@
         <v>43176</v>
       </c>
       <c r="B261">
-        <v>0.4298546</v>
+        <v>0.4635289</v>
       </c>
     </row>
     <row r="262" spans="1:2">
@@ -2482,7 +2482,7 @@
         <v>43177</v>
       </c>
       <c r="B262">
-        <v>0.4276124</v>
+        <v>0.4618197</v>
       </c>
     </row>
     <row r="263" spans="1:2">
@@ -2490,7 +2490,7 @@
         <v>43178</v>
       </c>
       <c r="B263">
-        <v>0.4253217</v>
+        <v>0.4600883</v>
       </c>
     </row>
     <row r="264" spans="1:2">
@@ -2498,7 +2498,7 @@
         <v>43179</v>
       </c>
       <c r="B264">
-        <v>0.4229831</v>
+        <v>0.4583381</v>
       </c>
     </row>
     <row r="265" spans="1:2">
@@ -2506,7 +2506,7 @@
         <v>43180</v>
       </c>
       <c r="B265">
-        <v>0.4205968</v>
+        <v>0.4565725</v>
       </c>
     </row>
     <row r="266" spans="1:2">
@@ -2514,7 +2514,7 @@
         <v>43181</v>
       </c>
       <c r="B266">
-        <v>0.4181636</v>
+        <v>0.4547948</v>
       </c>
     </row>
     <row r="267" spans="1:2">
@@ -2522,7 +2522,7 @@
         <v>43182</v>
       </c>
       <c r="B267">
-        <v>0.4156838</v>
+        <v>0.4530084</v>
       </c>
     </row>
     <row r="268" spans="1:2">
@@ -2530,7 +2530,7 @@
         <v>43183</v>
       </c>
       <c r="B268">
-        <v>0.4131579</v>
+        <v>0.4512168</v>
       </c>
     </row>
     <row r="269" spans="1:2">
@@ -2538,7 +2538,7 @@
         <v>43184</v>
       </c>
       <c r="B269">
-        <v>0.4105866</v>
+        <v>0.4494231</v>
       </c>
     </row>
     <row r="270" spans="1:2">
@@ -2546,7 +2546,7 @@
         <v>43185</v>
       </c>
       <c r="B270">
-        <v>0.4079703</v>
+        <v>0.4476307</v>
       </c>
     </row>
     <row r="271" spans="1:2">
@@ -2554,7 +2554,7 @@
         <v>43186</v>
       </c>
       <c r="B271">
-        <v>0.4053096</v>
+        <v>0.4458427</v>
       </c>
     </row>
     <row r="272" spans="1:2">
@@ -2562,7 +2562,7 @@
         <v>43187</v>
       </c>
       <c r="B272">
-        <v>0.4026051</v>
+        <v>0.4440622</v>
       </c>
     </row>
     <row r="273" spans="1:2">
@@ -2570,7 +2570,7 @@
         <v>43188</v>
       </c>
       <c r="B273">
-        <v>0.3998572</v>
+        <v>0.4422921</v>
       </c>
     </row>
     <row r="274" spans="1:2">
@@ -2578,7 +2578,7 @@
         <v>43189</v>
       </c>
       <c r="B274">
-        <v>0.3970667</v>
+        <v>0.4405353</v>
       </c>
     </row>
     <row r="275" spans="1:2">
@@ -2586,7 +2586,7 @@
         <v>43190</v>
       </c>
       <c r="B275">
-        <v>0.3942341</v>
+        <v>0.4387945</v>
       </c>
     </row>
     <row r="276" spans="1:2">
@@ -2594,7 +2594,7 @@
         <v>43191</v>
       </c>
       <c r="B276">
-        <v>0.3913601</v>
+        <v>0.4370722</v>
       </c>
     </row>
     <row r="277" spans="1:2">
@@ -2602,7 +2602,7 @@
         <v>43192</v>
       </c>
       <c r="B277">
-        <v>0.3884451</v>
+        <v>0.4353708</v>
       </c>
     </row>
     <row r="278" spans="1:2">
@@ -2610,7 +2610,7 @@
         <v>43193</v>
       </c>
       <c r="B278">
-        <v>0.38549</v>
+        <v>0.4336926</v>
       </c>
     </row>
     <row r="279" spans="1:2">
@@ -2618,7 +2618,7 @@
         <v>43194</v>
       </c>
       <c r="B279">
-        <v>0.3824953</v>
+        <v>0.4320396</v>
       </c>
     </row>
     <row r="280" spans="1:2">
@@ -2626,7 +2626,7 @@
         <v>43195</v>
       </c>
       <c r="B280">
-        <v>0.3794616</v>
+        <v>0.4304136</v>
       </c>
     </row>
     <row r="281" spans="1:2">
@@ -2634,7 +2634,7 @@
         <v>43196</v>
       </c>
       <c r="B281">
-        <v>0.3763897</v>
+        <v>0.4288166</v>
       </c>
     </row>
     <row r="282" spans="1:2">
@@ -2642,7 +2642,7 @@
         <v>43197</v>
       </c>
       <c r="B282">
-        <v>0.3732803</v>
+        <v>0.4272499</v>
       </c>
     </row>
     <row r="283" spans="1:2">
@@ -2650,7 +2650,7 @@
         <v>43198</v>
       </c>
       <c r="B283">
-        <v>0.3701339</v>
+        <v>0.425715</v>
       </c>
     </row>
     <row r="284" spans="1:2">
@@ -2658,7 +2658,7 @@
         <v>43199</v>
       </c>
       <c r="B284">
-        <v>0.3669514</v>
+        <v>0.4242132</v>
       </c>
     </row>
     <row r="285" spans="1:2">
@@ -2666,7 +2666,7 @@
         <v>43200</v>
       </c>
       <c r="B285">
-        <v>0.3637335</v>
+        <v>0.4227453</v>
       </c>
     </row>
     <row r="286" spans="1:2">
@@ -2674,7 +2674,7 @@
         <v>43201</v>
       </c>
       <c r="B286">
-        <v>0.3604808</v>
+        <v>0.4213125</v>
       </c>
     </row>
     <row r="287" spans="1:2">
@@ -2682,7 +2682,7 @@
         <v>43202</v>
       </c>
       <c r="B287">
-        <v>0.3571941</v>
+        <v>0.4199153</v>
       </c>
     </row>
     <row r="288" spans="1:2">
@@ -2690,7 +2690,7 @@
         <v>43203</v>
       </c>
       <c r="B288">
-        <v>0.3538743</v>
+        <v>0.4185545</v>
       </c>
     </row>
     <row r="289" spans="1:2">
@@ -2698,7 +2698,7 @@
         <v>43204</v>
       </c>
       <c r="B289">
-        <v>0.3505219</v>
+        <v>0.4172304</v>
       </c>
     </row>
     <row r="290" spans="1:2">
@@ -2706,7 +2706,7 @@
         <v>43205</v>
       </c>
       <c r="B290">
-        <v>0.3471379</v>
+        <v>0.4159434</v>
       </c>
     </row>
     <row r="291" spans="1:2">
@@ -2714,7 +2714,7 @@
         <v>43206</v>
       </c>
       <c r="B291">
-        <v>0.3437229</v>
+        <v>0.4146936</v>
       </c>
     </row>
     <row r="292" spans="1:2">
@@ -2722,7 +2722,7 @@
         <v>43207</v>
       </c>
       <c r="B292">
-        <v>0.3402779</v>
+        <v>0.4134812</v>
       </c>
     </row>
     <row r="293" spans="1:2">
@@ -2730,7 +2730,7 @@
         <v>43208</v>
       </c>
       <c r="B293">
-        <v>0.3368036</v>
+        <v>0.412306</v>
       </c>
     </row>
     <row r="294" spans="1:2">
@@ -2738,7 +2738,7 @@
         <v>43209</v>
       </c>
       <c r="B294">
-        <v>0.3333008</v>
+        <v>0.4111681</v>
       </c>
     </row>
     <row r="295" spans="1:2">
@@ -2746,7 +2746,7 @@
         <v>43210</v>
       </c>
       <c r="B295">
-        <v>0.3297704</v>
+        <v>0.4100671</v>
       </c>
     </row>
     <row r="296" spans="1:2">
@@ -2754,7 +2754,7 @@
         <v>43211</v>
       </c>
       <c r="B296">
-        <v>0.3262133</v>
+        <v>0.4090027</v>
       </c>
     </row>
     <row r="297" spans="1:2">
@@ -2762,7 +2762,7 @@
         <v>43212</v>
       </c>
       <c r="B297">
-        <v>0.3226302</v>
+        <v>0.4079746</v>
       </c>
     </row>
     <row r="298" spans="1:2">
@@ -2770,7 +2770,7 @@
         <v>43213</v>
       </c>
       <c r="B298">
-        <v>0.319022</v>
+        <v>0.4069822</v>
       </c>
     </row>
     <row r="299" spans="1:2">
@@ -2778,7 +2778,7 @@
         <v>43214</v>
       </c>
       <c r="B299">
-        <v>0.3153897</v>
+        <v>0.4060251</v>
       </c>
     </row>
     <row r="300" spans="1:2">
@@ -2786,7 +2786,7 @@
         <v>43215</v>
       </c>
       <c r="B300">
-        <v>0.3117342</v>
+        <v>0.4051027</v>
       </c>
     </row>
     <row r="301" spans="1:2">
@@ -2794,7 +2794,7 @@
         <v>43216</v>
       </c>
       <c r="B301">
-        <v>0.3080562</v>
+        <v>0.4042143</v>
       </c>
     </row>
     <row r="302" spans="1:2">
@@ -2802,7 +2802,7 @@
         <v>43217</v>
       </c>
       <c r="B302">
-        <v>0.3043569</v>
+        <v>0.4033593</v>
       </c>
     </row>
     <row r="303" spans="1:2">
@@ -2810,7 +2810,7 @@
         <v>43218</v>
       </c>
       <c r="B303">
-        <v>0.300637</v>
+        <v>0.402537</v>
       </c>
     </row>
     <row r="304" spans="1:2">
@@ -2818,7 +2818,7 @@
         <v>43219</v>
       </c>
       <c r="B304">
-        <v>0.2968976</v>
+        <v>0.4017466</v>
       </c>
     </row>
     <row r="305" spans="1:2">
@@ -2826,7 +2826,7 @@
         <v>43220</v>
       </c>
       <c r="B305">
-        <v>0.2931395</v>
+        <v>0.4009874</v>
       </c>
     </row>
     <row r="306" spans="1:2">
@@ -2834,7 +2834,7 @@
         <v>43221</v>
       </c>
       <c r="B306">
-        <v>0.2893639</v>
+        <v>0.4002586</v>
       </c>
     </row>
     <row r="307" spans="1:2">
@@ -2842,7 +2842,7 @@
         <v>43222</v>
       </c>
       <c r="B307">
-        <v>0.2855715</v>
+        <v>0.3995594</v>
       </c>
     </row>
     <row r="308" spans="1:2">
@@ -2850,7 +2850,7 @@
         <v>43223</v>
       </c>
       <c r="B308">
-        <v>0.2817635</v>
+        <v>0.398889</v>
       </c>
     </row>
     <row r="309" spans="1:2">
@@ -2858,7 +2858,7 @@
         <v>43224</v>
       </c>
       <c r="B309">
-        <v>0.2779408</v>
+        <v>0.3982466</v>
       </c>
     </row>
     <row r="310" spans="1:2">
@@ -2866,7 +2866,7 @@
         <v>43225</v>
       </c>
       <c r="B310">
-        <v>0.2741045</v>
+        <v>0.3976314</v>
       </c>
     </row>
     <row r="311" spans="1:2">
@@ -2874,7 +2874,7 @@
         <v>43226</v>
       </c>
       <c r="B311">
-        <v>0.2702555</v>
+        <v>0.3970425</v>
       </c>
     </row>
     <row r="312" spans="1:2">
@@ -2882,7 +2882,7 @@
         <v>43227</v>
       </c>
       <c r="B312">
-        <v>0.2663949</v>
+        <v>0.3964792</v>
       </c>
     </row>
     <row r="313" spans="1:2">
@@ -2890,7 +2890,7 @@
         <v>43228</v>
       </c>
       <c r="B313">
-        <v>0.2625238</v>
+        <v>0.3959406</v>
       </c>
     </row>
     <row r="314" spans="1:2">
@@ -2898,7 +2898,7 @@
         <v>43229</v>
       </c>
       <c r="B314">
-        <v>0.2586432</v>
+        <v>0.3954259</v>
       </c>
     </row>
     <row r="315" spans="1:2">
@@ -2906,7 +2906,7 @@
         <v>43230</v>
       </c>
       <c r="B315">
-        <v>0.2547542</v>
+        <v>0.3949343</v>
       </c>
     </row>
     <row r="316" spans="1:2">
@@ -2914,7 +2914,7 @@
         <v>43231</v>
       </c>
       <c r="B316">
-        <v>0.2508579</v>
+        <v>0.3944651</v>
       </c>
     </row>
     <row r="317" spans="1:2">
@@ -2922,7 +2922,7 @@
         <v>43232</v>
       </c>
       <c r="B317">
-        <v>0.2469554</v>
+        <v>0.3940175</v>
       </c>
     </row>
     <row r="318" spans="1:2">
@@ -2930,7 +2930,7 @@
         <v>43233</v>
       </c>
       <c r="B318">
-        <v>0.2430478</v>
+        <v>0.3935906</v>
       </c>
     </row>
     <row r="319" spans="1:2">
@@ -2938,7 +2938,7 @@
         <v>43234</v>
       </c>
       <c r="B319">
-        <v>0.2391361</v>
+        <v>0.3931839</v>
       </c>
     </row>
     <row r="320" spans="1:2">
@@ -2946,7 +2946,7 @@
         <v>43235</v>
       </c>
       <c r="B320">
-        <v>0.2352217</v>
+        <v>0.3927965</v>
       </c>
     </row>
     <row r="321" spans="1:2">
@@ -2954,7 +2954,7 @@
         <v>43236</v>
       </c>
       <c r="B321">
-        <v>0.2313055</v>
+        <v>0.3924277</v>
       </c>
     </row>
     <row r="322" spans="1:2">
@@ -2962,7 +2962,7 @@
         <v>43237</v>
       </c>
       <c r="B322">
-        <v>0.2273887</v>
+        <v>0.3920768</v>
       </c>
     </row>
     <row r="323" spans="1:2">
@@ -2970,7 +2970,7 @@
         <v>43238</v>
       </c>
       <c r="B323">
-        <v>0.2234726</v>
+        <v>0.3917432</v>
       </c>
     </row>
     <row r="324" spans="1:2">
@@ -2978,7 +2978,7 @@
         <v>43239</v>
       </c>
       <c r="B324">
-        <v>0.2195582</v>
+        <v>0.3914262</v>
       </c>
     </row>
     <row r="325" spans="1:2">
@@ -2986,7 +2986,7 @@
         <v>43240</v>
       </c>
       <c r="B325">
-        <v>0.2156469</v>
+        <v>0.3911252</v>
       </c>
     </row>
     <row r="326" spans="1:2">
@@ -2994,7 +2994,7 @@
         <v>43241</v>
       </c>
       <c r="B326">
-        <v>0.2117397</v>
+        <v>0.3908395</v>
       </c>
     </row>
     <row r="327" spans="1:2">
@@ -3002,7 +3002,7 @@
         <v>43242</v>
       </c>
       <c r="B327">
-        <v>0.207838</v>
+        <v>0.3905686</v>
       </c>
     </row>
     <row r="328" spans="1:2">
@@ -3010,7 +3010,7 @@
         <v>43243</v>
       </c>
       <c r="B328">
-        <v>0.2039429</v>
+        <v>0.3903118</v>
       </c>
     </row>
     <row r="329" spans="1:2">
@@ -3018,7 +3018,7 @@
         <v>43244</v>
       </c>
       <c r="B329">
-        <v>0.2000557</v>
+        <v>0.3900686</v>
       </c>
     </row>
     <row r="330" spans="1:2">
@@ -3026,7 +3026,7 @@
         <v>43245</v>
       </c>
       <c r="B330">
-        <v>0.1961776</v>
+        <v>0.3898384</v>
       </c>
     </row>
     <row r="331" spans="1:2">
@@ -3034,7 +3034,7 @@
         <v>43246</v>
       </c>
       <c r="B331">
-        <v>0.1923099</v>
+        <v>0.3896207</v>
       </c>
     </row>
     <row r="332" spans="1:2">
@@ -3042,7 +3042,7 @@
         <v>43247</v>
       </c>
       <c r="B332">
-        <v>0.1884539</v>
+        <v>0.389415</v>
       </c>
     </row>
     <row r="333" spans="1:2">
@@ -3050,7 +3050,7 @@
         <v>43248</v>
       </c>
       <c r="B333">
-        <v>0.1846108</v>
+        <v>0.3892208</v>
       </c>
     </row>
     <row r="334" spans="1:2">
@@ -3058,7 +3058,7 @@
         <v>43249</v>
       </c>
       <c r="B334">
-        <v>0.180782</v>
+        <v>0.3890375</v>
       </c>
     </row>
     <row r="335" spans="1:2">
@@ -3066,7 +3066,7 @@
         <v>43250</v>
       </c>
       <c r="B335">
-        <v>0.1769688</v>
+        <v>0.3888649</v>
       </c>
     </row>
     <row r="336" spans="1:2">
@@ -3074,7 +3074,7 @@
         <v>43251</v>
       </c>
       <c r="B336">
-        <v>0.1731725</v>
+        <v>0.3887023</v>
       </c>
     </row>
     <row r="337" spans="1:2">
@@ -3082,7 +3082,7 @@
         <v>43252</v>
       </c>
       <c r="B337">
-        <v>0.1693944</v>
+        <v>0.3885494</v>
       </c>
     </row>
     <row r="338" spans="1:2">
@@ -3090,7 +3090,7 @@
         <v>43253</v>
       </c>
       <c r="B338">
-        <v>0.1656358</v>
+        <v>0.3884057</v>
       </c>
     </row>
     <row r="339" spans="1:2">
@@ -3098,7 +3098,7 @@
         <v>43254</v>
       </c>
       <c r="B339">
-        <v>0.1618983</v>
+        <v>0.3882709</v>
       </c>
     </row>
     <row r="340" spans="1:2">
@@ -3106,7 +3106,7 @@
         <v>43255</v>
       </c>
       <c r="B340">
-        <v>0.158183</v>
+        <v>0.3881446</v>
       </c>
     </row>
     <row r="341" spans="1:2">
@@ -3114,7 +3114,7 @@
         <v>43256</v>
       </c>
       <c r="B341">
-        <v>0.1544914</v>
+        <v>0.3880263</v>
       </c>
     </row>
     <row r="342" spans="1:2">
@@ -3122,7 +3122,7 @@
         <v>43257</v>
       </c>
       <c r="B342">
-        <v>0.1508249</v>
+        <v>0.3879158</v>
       </c>
     </row>
     <row r="343" spans="1:2">
@@ -3130,7 +3130,7 @@
         <v>43258</v>
       </c>
       <c r="B343">
-        <v>0.1471849</v>
+        <v>0.3878127</v>
       </c>
     </row>
     <row r="344" spans="1:2">
@@ -3138,7 +3138,7 @@
         <v>43259</v>
       </c>
       <c r="B344">
-        <v>0.1435729</v>
+        <v>0.3877166</v>
       </c>
     </row>
     <row r="345" spans="1:2">
@@ -3146,7 +3146,7 @@
         <v>43260</v>
       </c>
       <c r="B345">
-        <v>0.1399901</v>
+        <v>0.3876272</v>
       </c>
     </row>
     <row r="346" spans="1:2">
@@ -3154,7 +3154,7 @@
         <v>43261</v>
       </c>
       <c r="B346">
-        <v>0.1364382</v>
+        <v>0.3875443</v>
       </c>
     </row>
     <row r="347" spans="1:2">
@@ -3162,7 +3162,7 @@
         <v>43262</v>
       </c>
       <c r="B347">
-        <v>0.1329185</v>
+        <v>0.3874676</v>
       </c>
     </row>
     <row r="348" spans="1:2">
@@ -3170,7 +3170,7 @@
         <v>43263</v>
       </c>
       <c r="B348">
-        <v>0.1294325</v>
+        <v>0.3873966</v>
       </c>
     </row>
     <row r="349" spans="1:2">
@@ -3178,7 +3178,7 @@
         <v>43264</v>
       </c>
       <c r="B349">
-        <v>0.1259817</v>
+        <v>0.3873313</v>
       </c>
     </row>
     <row r="350" spans="1:2">
@@ -3186,7 +3186,7 @@
         <v>43265</v>
       </c>
       <c r="B350">
-        <v>0.1225676</v>
+        <v>0.3872712</v>
       </c>
     </row>
     <row r="351" spans="1:2">
@@ -3194,7 +3194,7 @@
         <v>43266</v>
       </c>
       <c r="B351">
-        <v>0.1191916</v>
+        <v>0.3872163</v>
       </c>
     </row>
     <row r="352" spans="1:2">
@@ -3202,7 +3202,7 @@
         <v>43267</v>
       </c>
       <c r="B352">
-        <v>0.1158553</v>
+        <v>0.3871661</v>
       </c>
     </row>
     <row r="353" spans="1:2">
@@ -3210,7 +3210,7 @@
         <v>43268</v>
       </c>
       <c r="B353">
-        <v>0.1125603</v>
+        <v>0.3871206</v>
       </c>
     </row>
     <row r="354" spans="1:2">
@@ -3218,7 +3218,7 @@
         <v>43269</v>
       </c>
       <c r="B354">
-        <v>0.109308</v>
+        <v>0.3870794</v>
       </c>
     </row>
     <row r="355" spans="1:2">
@@ -3226,7 +3226,7 @@
         <v>43270</v>
       </c>
       <c r="B355">
-        <v>0.1061001</v>
+        <v>0.3870423</v>
       </c>
     </row>
     <row r="356" spans="1:2">
@@ -3234,7 +3234,7 @@
         <v>43271</v>
       </c>
       <c r="B356">
-        <v>0.1029379</v>
+        <v>0.3870092</v>
       </c>
     </row>
     <row r="357" spans="1:2">
@@ -3242,7 +3242,7 @@
         <v>43272</v>
       </c>
       <c r="B357">
-        <v>0.0998233</v>
+        <v>0.3869798</v>
       </c>
     </row>
     <row r="358" spans="1:2">
@@ -3250,7 +3250,7 @@
         <v>43273</v>
       </c>
       <c r="B358">
-        <v>0.0967576</v>
+        <v>0.386954</v>
       </c>
     </row>
     <row r="359" spans="1:2">
@@ -3258,7 +3258,7 @@
         <v>43274</v>
       </c>
       <c r="B359">
-        <v>0.0937426</v>
+        <v>0.3869315</v>
       </c>
     </row>
     <row r="360" spans="1:2">
@@ -3266,7 +3266,7 @@
         <v>43275</v>
       </c>
       <c r="B360">
-        <v>0.0907799</v>
+        <v>0.3869123</v>
       </c>
     </row>
     <row r="361" spans="1:2">
@@ -3274,7 +3274,7 @@
         <v>43276</v>
       </c>
       <c r="B361">
-        <v>0.0878709</v>
+        <v>0.386896</v>
       </c>
     </row>
     <row r="362" spans="1:2">
@@ -3282,7 +3282,7 @@
         <v>43277</v>
       </c>
       <c r="B362">
-        <v>0.0850175</v>
+        <v>0.3868826</v>
       </c>
     </row>
     <row r="363" spans="1:2">
@@ -3290,7 +3290,7 @@
         <v>43278</v>
       </c>
       <c r="B363">
-        <v>0.08222119999999999</v>
+        <v>0.386872</v>
       </c>
     </row>
     <row r="364" spans="1:2">
@@ -3298,7 +3298,7 @@
         <v>43279</v>
       </c>
       <c r="B364">
-        <v>0.0794837</v>
+        <v>0.3868638</v>
       </c>
     </row>
     <row r="365" spans="1:2">
@@ -3306,7 +3306,7 @@
         <v>43280</v>
       </c>
       <c r="B365">
-        <v>0.0768066</v>
+        <v>0.3868581</v>
       </c>
     </row>
     <row r="366" spans="1:2">
@@ -3314,7 +3314,7 @@
         <v>43281</v>
       </c>
       <c r="B366">
-        <v>0.0741917</v>
+        <v>0.3868546</v>
       </c>
     </row>
     <row r="367" spans="1:2">
@@ -3322,7 +3322,7 @@
         <v>43282</v>
       </c>
       <c r="B367">
-        <v>0.0716406</v>
+        <v>0.3868533</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Round 1 of cleaning all the code.
</commit_message>
<xml_diff>
--- a/DATA/collate_cultivar_data/data/Smoothed_kcp_trend_vs_datetime.xlsx
+++ b/DATA/collate_cultivar_data/data/Smoothed_kcp_trend_vs_datetime.xlsx
@@ -402,7 +402,7 @@
         <v>42917</v>
       </c>
       <c r="B2">
-        <v>0.0769446</v>
+        <v>0.09059</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -410,7 +410,7 @@
         <v>42918</v>
       </c>
       <c r="B3">
-        <v>0.0769446</v>
+        <v>0.09059</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -418,7 +418,7 @@
         <v>42919</v>
       </c>
       <c r="B4">
-        <v>0.0769446</v>
+        <v>0.09059</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -426,7 +426,7 @@
         <v>42920</v>
       </c>
       <c r="B5">
-        <v>0.0769446</v>
+        <v>0.09059</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -434,7 +434,7 @@
         <v>42921</v>
       </c>
       <c r="B6">
-        <v>0.0769446</v>
+        <v>0.09059</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -442,7 +442,7 @@
         <v>42922</v>
       </c>
       <c r="B7">
-        <v>0.0769446</v>
+        <v>0.09059</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -450,7 +450,7 @@
         <v>42923</v>
       </c>
       <c r="B8">
-        <v>0.0769446</v>
+        <v>0.09059</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -458,7 +458,7 @@
         <v>42924</v>
       </c>
       <c r="B9">
-        <v>0.0769446</v>
+        <v>0.09059</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -466,7 +466,7 @@
         <v>42925</v>
       </c>
       <c r="B10">
-        <v>0.0769446</v>
+        <v>0.09059</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -474,7 +474,7 @@
         <v>42926</v>
       </c>
       <c r="B11">
-        <v>0.0769446</v>
+        <v>0.09059</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -482,7 +482,7 @@
         <v>42927</v>
       </c>
       <c r="B12">
-        <v>0.0769446</v>
+        <v>0.09059</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -490,7 +490,7 @@
         <v>42928</v>
       </c>
       <c r="B13">
-        <v>0.0769446</v>
+        <v>0.09059</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -498,7 +498,7 @@
         <v>42929</v>
       </c>
       <c r="B14">
-        <v>0.0769446</v>
+        <v>0.09059</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -506,7 +506,7 @@
         <v>42930</v>
       </c>
       <c r="B15">
-        <v>0.0769446</v>
+        <v>0.09059</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -514,7 +514,7 @@
         <v>42931</v>
       </c>
       <c r="B16">
-        <v>0.0769446</v>
+        <v>0.09059</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -522,7 +522,7 @@
         <v>42932</v>
       </c>
       <c r="B17">
-        <v>0.0769446</v>
+        <v>0.09059</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -530,7 +530,7 @@
         <v>42933</v>
       </c>
       <c r="B18">
-        <v>0.0769446</v>
+        <v>0.09059</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -538,7 +538,7 @@
         <v>42934</v>
       </c>
       <c r="B19">
-        <v>0.0769446</v>
+        <v>0.09059</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -546,7 +546,7 @@
         <v>42935</v>
       </c>
       <c r="B20">
-        <v>0.0769446</v>
+        <v>0.09059</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -554,7 +554,7 @@
         <v>42936</v>
       </c>
       <c r="B21">
-        <v>0.0769446</v>
+        <v>0.09059</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -562,7 +562,7 @@
         <v>42937</v>
       </c>
       <c r="B22">
-        <v>0.0769446</v>
+        <v>0.09059</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -570,7 +570,7 @@
         <v>42938</v>
       </c>
       <c r="B23">
-        <v>0.0769446</v>
+        <v>0.09059</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -578,7 +578,7 @@
         <v>42939</v>
       </c>
       <c r="B24">
-        <v>0.0769446</v>
+        <v>0.09059</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -586,7 +586,7 @@
         <v>42940</v>
       </c>
       <c r="B25">
-        <v>0.0769446</v>
+        <v>0.09059</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -594,7 +594,7 @@
         <v>42941</v>
       </c>
       <c r="B26">
-        <v>0.0769446</v>
+        <v>0.09059</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -602,7 +602,7 @@
         <v>42942</v>
       </c>
       <c r="B27">
-        <v>0.0769446</v>
+        <v>0.09059</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -610,7 +610,7 @@
         <v>42943</v>
       </c>
       <c r="B28">
-        <v>0.0769446</v>
+        <v>0.09059</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -618,7 +618,7 @@
         <v>42944</v>
       </c>
       <c r="B29">
-        <v>0.0769446</v>
+        <v>0.09059</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -626,7 +626,7 @@
         <v>42945</v>
       </c>
       <c r="B30">
-        <v>0.0769446</v>
+        <v>0.09059</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -634,7 +634,7 @@
         <v>42946</v>
       </c>
       <c r="B31">
-        <v>0.0769446</v>
+        <v>0.09059</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -642,7 +642,7 @@
         <v>42947</v>
       </c>
       <c r="B32">
-        <v>0.0769446</v>
+        <v>0.09059</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -650,7 +650,7 @@
         <v>42948</v>
       </c>
       <c r="B33">
-        <v>0.0769446</v>
+        <v>0.09059</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -658,7 +658,7 @@
         <v>42949</v>
       </c>
       <c r="B34">
-        <v>0.0769446</v>
+        <v>0.09059</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -666,7 +666,7 @@
         <v>42950</v>
       </c>
       <c r="B35">
-        <v>0.0769446</v>
+        <v>0.09059</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -674,7 +674,7 @@
         <v>42951</v>
       </c>
       <c r="B36">
-        <v>0.0769446</v>
+        <v>0.09059</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -682,7 +682,7 @@
         <v>42952</v>
       </c>
       <c r="B37">
-        <v>0.0769446</v>
+        <v>0.09059</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -690,7 +690,7 @@
         <v>42953</v>
       </c>
       <c r="B38">
-        <v>0.0769446</v>
+        <v>0.09059</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -698,7 +698,7 @@
         <v>42954</v>
       </c>
       <c r="B39">
-        <v>0.0769446</v>
+        <v>0.09059</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -706,7 +706,7 @@
         <v>42955</v>
       </c>
       <c r="B40">
-        <v>0.0769446</v>
+        <v>0.09059</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -714,7 +714,7 @@
         <v>42956</v>
       </c>
       <c r="B41">
-        <v>0.0769446</v>
+        <v>0.09059</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -722,7 +722,7 @@
         <v>42957</v>
       </c>
       <c r="B42">
-        <v>0.0769446</v>
+        <v>0.09059</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -730,7 +730,7 @@
         <v>42958</v>
       </c>
       <c r="B43">
-        <v>0.0769446</v>
+        <v>0.09059</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -738,7 +738,7 @@
         <v>42959</v>
       </c>
       <c r="B44">
-        <v>0.0769446</v>
+        <v>0.09059</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -746,7 +746,7 @@
         <v>42960</v>
       </c>
       <c r="B45">
-        <v>0.0769446</v>
+        <v>0.09059</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -754,7 +754,7 @@
         <v>42961</v>
       </c>
       <c r="B46">
-        <v>0.0769446</v>
+        <v>0.09059</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -762,7 +762,7 @@
         <v>42962</v>
       </c>
       <c r="B47">
-        <v>0.0769446</v>
+        <v>0.09059</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -770,7 +770,7 @@
         <v>42963</v>
       </c>
       <c r="B48">
-        <v>0.0769446</v>
+        <v>0.09059</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -778,7 +778,7 @@
         <v>42964</v>
       </c>
       <c r="B49">
-        <v>0.0769446</v>
+        <v>0.09059</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -786,7 +786,7 @@
         <v>42965</v>
       </c>
       <c r="B50">
-        <v>0.0769446</v>
+        <v>0.09059</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -794,7 +794,7 @@
         <v>42966</v>
       </c>
       <c r="B51">
-        <v>0.0769446</v>
+        <v>0.09059</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -802,7 +802,7 @@
         <v>42967</v>
       </c>
       <c r="B52">
-        <v>0.0769446</v>
+        <v>0.09059</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -810,7 +810,7 @@
         <v>42968</v>
       </c>
       <c r="B53">
-        <v>0.0769446</v>
+        <v>0.09059</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -818,7 +818,7 @@
         <v>42969</v>
       </c>
       <c r="B54">
-        <v>0.0769724</v>
+        <v>0.09059</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -826,7 +826,7 @@
         <v>42970</v>
       </c>
       <c r="B55">
-        <v>0.0770969</v>
+        <v>0.09059</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -834,7 +834,7 @@
         <v>42971</v>
       </c>
       <c r="B56">
-        <v>0.077317</v>
+        <v>0.09059</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -842,7 +842,7 @@
         <v>42972</v>
       </c>
       <c r="B57">
-        <v>0.0776314</v>
+        <v>0.09059</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -850,7 +850,7 @@
         <v>42973</v>
       </c>
       <c r="B58">
-        <v>0.07803880000000001</v>
+        <v>0.09059</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -858,7 +858,7 @@
         <v>42974</v>
       </c>
       <c r="B59">
-        <v>0.078538</v>
+        <v>0.09064270000000001</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -866,7 +866,7 @@
         <v>42975</v>
       </c>
       <c r="B60">
-        <v>0.0791279</v>
+        <v>0.0907843</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -874,7 +874,7 @@
         <v>42976</v>
       </c>
       <c r="B61">
-        <v>0.07980710000000001</v>
+        <v>0.09101339999999999</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -882,7 +882,7 @@
         <v>42977</v>
       </c>
       <c r="B62">
-        <v>0.08057449999999999</v>
+        <v>0.0913288</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -890,7 +890,7 @@
         <v>42978</v>
       </c>
       <c r="B63">
-        <v>0.0814288</v>
+        <v>0.0917293</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -898,7 +898,7 @@
         <v>42979</v>
       </c>
       <c r="B64">
-        <v>0.08236880000000001</v>
+        <v>0.0922137</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -906,7 +906,7 @@
         <v>42980</v>
       </c>
       <c r="B65">
-        <v>0.0833933</v>
+        <v>0.0927809</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -914,7 +914,7 @@
         <v>42981</v>
       </c>
       <c r="B66">
-        <v>0.0845011</v>
+        <v>0.0934295</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -922,7 +922,7 @@
         <v>42982</v>
       </c>
       <c r="B67">
-        <v>0.085691</v>
+        <v>0.0941583</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -930,7 +930,7 @@
         <v>42983</v>
       </c>
       <c r="B68">
-        <v>0.0869617</v>
+        <v>0.0949663</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -938,7 +938,7 @@
         <v>42984</v>
       </c>
       <c r="B69">
-        <v>0.0883121</v>
+        <v>0.0958521</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -946,7 +946,7 @@
         <v>42985</v>
       </c>
       <c r="B70">
-        <v>0.0897408</v>
+        <v>0.0968146</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -954,7 +954,7 @@
         <v>42986</v>
       </c>
       <c r="B71">
-        <v>0.0912468</v>
+        <v>0.0978526</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -962,7 +962,7 @@
         <v>42987</v>
       </c>
       <c r="B72">
-        <v>0.0928288</v>
+        <v>0.09896480000000001</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -970,7 +970,7 @@
         <v>42988</v>
       </c>
       <c r="B73">
-        <v>0.0944856</v>
+        <v>0.1001502</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -978,7 +978,7 @@
         <v>42989</v>
       </c>
       <c r="B74">
-        <v>0.09621589999999999</v>
+        <v>0.1014074</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -986,7 +986,7 @@
         <v>42990</v>
       </c>
       <c r="B75">
-        <v>0.0980186</v>
+        <v>0.1027354</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -994,7 +994,7 @@
         <v>42991</v>
       </c>
       <c r="B76">
-        <v>0.0998926</v>
+        <v>0.1041329</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -1002,7 +1002,7 @@
         <v>42992</v>
       </c>
       <c r="B77">
-        <v>0.1018364</v>
+        <v>0.1055988</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -1010,7 +1010,7 @@
         <v>42993</v>
       </c>
       <c r="B78">
-        <v>0.1038491</v>
+        <v>0.1071319</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -1018,7 +1018,7 @@
         <v>42994</v>
       </c>
       <c r="B79">
-        <v>0.1059293</v>
+        <v>0.108731</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -1026,7 +1026,7 @@
         <v>42995</v>
       </c>
       <c r="B80">
-        <v>0.1080759</v>
+        <v>0.110395</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -1034,7 +1034,7 @@
         <v>42996</v>
       </c>
       <c r="B81">
-        <v>0.1102877</v>
+        <v>0.1121226</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -1042,7 +1042,7 @@
         <v>42997</v>
       </c>
       <c r="B82">
-        <v>0.1125634</v>
+        <v>0.1139127</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -1050,7 +1050,7 @@
         <v>42998</v>
       </c>
       <c r="B83">
-        <v>0.114902</v>
+        <v>0.1157642</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -1058,7 +1058,7 @@
         <v>42999</v>
       </c>
       <c r="B84">
-        <v>0.1173021</v>
+        <v>0.1176758</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -1066,7 +1066,7 @@
         <v>43000</v>
       </c>
       <c r="B85">
-        <v>0.1197626</v>
+        <v>0.1196465</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -1074,7 +1074,7 @@
         <v>43001</v>
       </c>
       <c r="B86">
-        <v>0.1222824</v>
+        <v>0.1216751</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -1082,7 +1082,7 @@
         <v>43002</v>
       </c>
       <c r="B87">
-        <v>0.1248601</v>
+        <v>0.1237604</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -1090,7 +1090,7 @@
         <v>43003</v>
       </c>
       <c r="B88">
-        <v>0.1274947</v>
+        <v>0.1259013</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -1098,7 +1098,7 @@
         <v>43004</v>
       </c>
       <c r="B89">
-        <v>0.1301849</v>
+        <v>0.1280966</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -1106,7 +1106,7 @@
         <v>43005</v>
       </c>
       <c r="B90">
-        <v>0.1329296</v>
+        <v>0.1303452</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -1114,7 +1114,7 @@
         <v>43006</v>
       </c>
       <c r="B91">
-        <v>0.1357276</v>
+        <v>0.132646</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -1122,7 +1122,7 @@
         <v>43007</v>
       </c>
       <c r="B92">
-        <v>0.1385776</v>
+        <v>0.1349978</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -1130,7 +1130,7 @@
         <v>43008</v>
       </c>
       <c r="B93">
-        <v>0.1414786</v>
+        <v>0.1373994</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -1138,7 +1138,7 @@
         <v>43009</v>
       </c>
       <c r="B94">
-        <v>0.1444293</v>
+        <v>0.1398498</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -1146,7 +1146,7 @@
         <v>43010</v>
       </c>
       <c r="B95">
-        <v>0.1474285</v>
+        <v>0.1423478</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -1154,7 +1154,7 @@
         <v>43011</v>
       </c>
       <c r="B96">
-        <v>0.1504752</v>
+        <v>0.1448923</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -1162,7 +1162,7 @@
         <v>43012</v>
       </c>
       <c r="B97">
-        <v>0.153568</v>
+        <v>0.1474821</v>
       </c>
     </row>
     <row r="98" spans="1:2">
@@ -1170,7 +1170,7 @@
         <v>43013</v>
       </c>
       <c r="B98">
-        <v>0.1567058</v>
+        <v>0.1501162</v>
       </c>
     </row>
     <row r="99" spans="1:2">
@@ -1178,7 +1178,7 @@
         <v>43014</v>
       </c>
       <c r="B99">
-        <v>0.1598875</v>
+        <v>0.1527934</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -1186,7 +1186,7 @@
         <v>43015</v>
       </c>
       <c r="B100">
-        <v>0.1631119</v>
+        <v>0.1555127</v>
       </c>
     </row>
     <row r="101" spans="1:2">
@@ -1194,7 +1194,7 @@
         <v>43016</v>
       </c>
       <c r="B101">
-        <v>0.1663778</v>
+        <v>0.1582728</v>
       </c>
     </row>
     <row r="102" spans="1:2">
@@ -1202,7 +1202,7 @@
         <v>43017</v>
       </c>
       <c r="B102">
-        <v>0.169684</v>
+        <v>0.1610727</v>
       </c>
     </row>
     <row r="103" spans="1:2">
@@ -1210,7 +1210,7 @@
         <v>43018</v>
       </c>
       <c r="B103">
-        <v>0.1730295</v>
+        <v>0.1639113</v>
       </c>
     </row>
     <row r="104" spans="1:2">
@@ -1218,7 +1218,7 @@
         <v>43019</v>
       </c>
       <c r="B104">
-        <v>0.1764129</v>
+        <v>0.1667874</v>
       </c>
     </row>
     <row r="105" spans="1:2">
@@ -1226,7 +1226,7 @@
         <v>43020</v>
       </c>
       <c r="B105">
-        <v>0.1798331</v>
+        <v>0.1697</v>
       </c>
     </row>
     <row r="106" spans="1:2">
@@ -1234,7 +1234,7 @@
         <v>43021</v>
       </c>
       <c r="B106">
-        <v>0.1832891</v>
+        <v>0.172648</v>
       </c>
     </row>
     <row r="107" spans="1:2">
@@ -1242,7 +1242,7 @@
         <v>43022</v>
       </c>
       <c r="B107">
-        <v>0.1867795</v>
+        <v>0.1756303</v>
       </c>
     </row>
     <row r="108" spans="1:2">
@@ -1250,7 +1250,7 @@
         <v>43023</v>
       </c>
       <c r="B108">
-        <v>0.1903033</v>
+        <v>0.1786457</v>
       </c>
     </row>
     <row r="109" spans="1:2">
@@ -1258,7 +1258,7 @@
         <v>43024</v>
       </c>
       <c r="B109">
-        <v>0.1938593</v>
+        <v>0.1816932</v>
       </c>
     </row>
     <row r="110" spans="1:2">
@@ -1266,7 +1266,7 @@
         <v>43025</v>
       </c>
       <c r="B110">
-        <v>0.1974463</v>
+        <v>0.1847718</v>
       </c>
     </row>
     <row r="111" spans="1:2">
@@ -1274,7 +1274,7 @@
         <v>43026</v>
       </c>
       <c r="B111">
-        <v>0.2010633</v>
+        <v>0.1878802</v>
       </c>
     </row>
     <row r="112" spans="1:2">
@@ -1282,7 +1282,7 @@
         <v>43027</v>
       </c>
       <c r="B112">
-        <v>0.2047089</v>
+        <v>0.1910175</v>
       </c>
     </row>
     <row r="113" spans="1:2">
@@ -1290,7 +1290,7 @@
         <v>43028</v>
       </c>
       <c r="B113">
-        <v>0.2083821</v>
+        <v>0.1941825</v>
       </c>
     </row>
     <row r="114" spans="1:2">
@@ -1298,7 +1298,7 @@
         <v>43029</v>
       </c>
       <c r="B114">
-        <v>0.2120817</v>
+        <v>0.1973742</v>
       </c>
     </row>
     <row r="115" spans="1:2">
@@ -1306,7 +1306,7 @@
         <v>43030</v>
       </c>
       <c r="B115">
-        <v>0.2158066</v>
+        <v>0.2005915</v>
       </c>
     </row>
     <row r="116" spans="1:2">
@@ -1314,7 +1314,7 @@
         <v>43031</v>
       </c>
       <c r="B116">
-        <v>0.2195556</v>
+        <v>0.2038333</v>
       </c>
     </row>
     <row r="117" spans="1:2">
@@ -1322,7 +1322,7 @@
         <v>43032</v>
       </c>
       <c r="B117">
-        <v>0.2233276</v>
+        <v>0.2070985</v>
       </c>
     </row>
     <row r="118" spans="1:2">
@@ -1330,7 +1330,7 @@
         <v>43033</v>
       </c>
       <c r="B118">
-        <v>0.2271214</v>
+        <v>0.2103862</v>
       </c>
     </row>
     <row r="119" spans="1:2">
@@ -1338,7 +1338,7 @@
         <v>43034</v>
       </c>
       <c r="B119">
-        <v>0.2309359</v>
+        <v>0.2136952</v>
       </c>
     </row>
     <row r="120" spans="1:2">
@@ -1346,7 +1346,7 @@
         <v>43035</v>
       </c>
       <c r="B120">
-        <v>0.2347699</v>
+        <v>0.2170244</v>
       </c>
     </row>
     <row r="121" spans="1:2">
@@ -1354,7 +1354,7 @@
         <v>43036</v>
       </c>
       <c r="B121">
-        <v>0.2386223</v>
+        <v>0.2203729</v>
       </c>
     </row>
     <row r="122" spans="1:2">
@@ -1362,7 +1362,7 @@
         <v>43037</v>
       </c>
       <c r="B122">
-        <v>0.2424919</v>
+        <v>0.2237395</v>
       </c>
     </row>
     <row r="123" spans="1:2">
@@ -1370,7 +1370,7 @@
         <v>43038</v>
       </c>
       <c r="B123">
-        <v>0.2463776</v>
+        <v>0.2271231</v>
       </c>
     </row>
     <row r="124" spans="1:2">
@@ -1378,7 +1378,7 @@
         <v>43039</v>
       </c>
       <c r="B124">
-        <v>0.2502783</v>
+        <v>0.2305229</v>
       </c>
     </row>
     <row r="125" spans="1:2">
@@ -1386,7 +1386,7 @@
         <v>43040</v>
       </c>
       <c r="B125">
-        <v>0.2541928</v>
+        <v>0.2339376</v>
       </c>
     </row>
     <row r="126" spans="1:2">
@@ -1394,7 +1394,7 @@
         <v>43041</v>
       </c>
       <c r="B126">
-        <v>0.25812</v>
+        <v>0.2373663</v>
       </c>
     </row>
     <row r="127" spans="1:2">
@@ -1402,7 +1402,7 @@
         <v>43042</v>
       </c>
       <c r="B127">
-        <v>0.2620587</v>
+        <v>0.2408079</v>
       </c>
     </row>
     <row r="128" spans="1:2">
@@ -1410,7 +1410,7 @@
         <v>43043</v>
       </c>
       <c r="B128">
-        <v>0.2660079</v>
+        <v>0.2442613</v>
       </c>
     </row>
     <row r="129" spans="1:2">
@@ -1418,7 +1418,7 @@
         <v>43044</v>
       </c>
       <c r="B129">
-        <v>0.2699664</v>
+        <v>0.2477256</v>
       </c>
     </row>
     <row r="130" spans="1:2">
@@ -1426,7 +1426,7 @@
         <v>43045</v>
       </c>
       <c r="B130">
-        <v>0.273933</v>
+        <v>0.2511997</v>
       </c>
     </row>
     <row r="131" spans="1:2">
@@ -1434,7 +1434,7 @@
         <v>43046</v>
       </c>
       <c r="B131">
-        <v>0.2779066</v>
+        <v>0.2546826</v>
       </c>
     </row>
     <row r="132" spans="1:2">
@@ -1442,7 +1442,7 @@
         <v>43047</v>
       </c>
       <c r="B132">
-        <v>0.2818861</v>
+        <v>0.2581732</v>
       </c>
     </row>
     <row r="133" spans="1:2">
@@ -1450,7 +1450,7 @@
         <v>43048</v>
       </c>
       <c r="B133">
-        <v>0.2858704</v>
+        <v>0.2616706</v>
       </c>
     </row>
     <row r="134" spans="1:2">
@@ -1458,7 +1458,7 @@
         <v>43049</v>
       </c>
       <c r="B134">
-        <v>0.2898584</v>
+        <v>0.2651736</v>
       </c>
     </row>
     <row r="135" spans="1:2">
@@ -1466,7 +1466,7 @@
         <v>43050</v>
       </c>
       <c r="B135">
-        <v>0.2938488</v>
+        <v>0.2686813</v>
       </c>
     </row>
     <row r="136" spans="1:2">
@@ -1474,7 +1474,7 @@
         <v>43051</v>
       </c>
       <c r="B136">
-        <v>0.2978407</v>
+        <v>0.2721926</v>
       </c>
     </row>
     <row r="137" spans="1:2">
@@ -1482,7 +1482,7 @@
         <v>43052</v>
       </c>
       <c r="B137">
-        <v>0.3018328</v>
+        <v>0.2757066</v>
       </c>
     </row>
     <row r="138" spans="1:2">
@@ -1490,7 +1490,7 @@
         <v>43053</v>
       </c>
       <c r="B138">
-        <v>0.3058241</v>
+        <v>0.2792222</v>
       </c>
     </row>
     <row r="139" spans="1:2">
@@ -1498,7 +1498,7 @@
         <v>43054</v>
       </c>
       <c r="B139">
-        <v>0.3098134</v>
+        <v>0.2827384</v>
       </c>
     </row>
     <row r="140" spans="1:2">
@@ -1506,7 +1506,7 @@
         <v>43055</v>
       </c>
       <c r="B140">
-        <v>0.3137996</v>
+        <v>0.2862542</v>
       </c>
     </row>
     <row r="141" spans="1:2">
@@ -1514,7 +1514,7 @@
         <v>43056</v>
       </c>
       <c r="B141">
-        <v>0.3177816</v>
+        <v>0.2897687</v>
       </c>
     </row>
     <row r="142" spans="1:2">
@@ -1522,7 +1522,7 @@
         <v>43057</v>
       </c>
       <c r="B142">
-        <v>0.3217583</v>
+        <v>0.2932807</v>
       </c>
     </row>
     <row r="143" spans="1:2">
@@ -1530,7 +1530,7 @@
         <v>43058</v>
       </c>
       <c r="B143">
-        <v>0.3257286</v>
+        <v>0.2967894</v>
       </c>
     </row>
     <row r="144" spans="1:2">
@@ -1538,7 +1538,7 @@
         <v>43059</v>
       </c>
       <c r="B144">
-        <v>0.3296913</v>
+        <v>0.3002937</v>
       </c>
     </row>
     <row r="145" spans="1:2">
@@ -1546,7 +1546,7 @@
         <v>43060</v>
       </c>
       <c r="B145">
-        <v>0.3336454</v>
+        <v>0.3037925</v>
       </c>
     </row>
     <row r="146" spans="1:2">
@@ -1554,7 +1554,7 @@
         <v>43061</v>
       </c>
       <c r="B146">
-        <v>0.3375897</v>
+        <v>0.3072851</v>
       </c>
     </row>
     <row r="147" spans="1:2">
@@ -1562,7 +1562,7 @@
         <v>43062</v>
       </c>
       <c r="B147">
-        <v>0.3415232</v>
+        <v>0.3107702</v>
       </c>
     </row>
     <row r="148" spans="1:2">
@@ -1570,7 +1570,7 @@
         <v>43063</v>
       </c>
       <c r="B148">
-        <v>0.3454446</v>
+        <v>0.314247</v>
       </c>
     </row>
     <row r="149" spans="1:2">
@@ -1578,7 +1578,7 @@
         <v>43064</v>
       </c>
       <c r="B149">
-        <v>0.349353</v>
+        <v>0.3177145</v>
       </c>
     </row>
     <row r="150" spans="1:2">
@@ -1586,7 +1586,7 @@
         <v>43065</v>
       </c>
       <c r="B150">
-        <v>0.3532472</v>
+        <v>0.3211717</v>
       </c>
     </row>
     <row r="151" spans="1:2">
@@ -1594,7 +1594,7 @@
         <v>43066</v>
       </c>
       <c r="B151">
-        <v>0.3571261</v>
+        <v>0.3246176</v>
       </c>
     </row>
     <row r="152" spans="1:2">
@@ -1602,7 +1602,7 @@
         <v>43067</v>
       </c>
       <c r="B152">
-        <v>0.3609886</v>
+        <v>0.3280512</v>
       </c>
     </row>
     <row r="153" spans="1:2">
@@ -1610,7 +1610,7 @@
         <v>43068</v>
       </c>
       <c r="B153">
-        <v>0.3648336</v>
+        <v>0.3314716</v>
       </c>
     </row>
     <row r="154" spans="1:2">
@@ -1618,7 +1618,7 @@
         <v>43069</v>
       </c>
       <c r="B154">
-        <v>0.36866</v>
+        <v>0.3348779</v>
       </c>
     </row>
     <row r="155" spans="1:2">
@@ -1626,7 +1626,7 @@
         <v>43070</v>
       </c>
       <c r="B155">
-        <v>0.3724668</v>
+        <v>0.3382689</v>
       </c>
     </row>
     <row r="156" spans="1:2">
@@ -1634,7 +1634,7 @@
         <v>43071</v>
       </c>
       <c r="B156">
-        <v>0.3762527</v>
+        <v>0.3416439</v>
       </c>
     </row>
     <row r="157" spans="1:2">
@@ -1642,7 +1642,7 @@
         <v>43072</v>
       </c>
       <c r="B157">
-        <v>0.3800168</v>
+        <v>0.3450017</v>
       </c>
     </row>
     <row r="158" spans="1:2">
@@ -1650,7 +1650,7 @@
         <v>43073</v>
       </c>
       <c r="B158">
-        <v>0.3837579</v>
+        <v>0.3483415</v>
       </c>
     </row>
     <row r="159" spans="1:2">
@@ -1658,7 +1658,7 @@
         <v>43074</v>
       </c>
       <c r="B159">
-        <v>0.3874749</v>
+        <v>0.3516623</v>
       </c>
     </row>
     <row r="160" spans="1:2">
@@ -1666,7 +1666,7 @@
         <v>43075</v>
       </c>
       <c r="B160">
-        <v>0.3911667</v>
+        <v>0.3549632</v>
       </c>
     </row>
     <row r="161" spans="1:2">
@@ -1674,7 +1674,7 @@
         <v>43076</v>
       </c>
       <c r="B161">
-        <v>0.3948324</v>
+        <v>0.3582431</v>
       </c>
     </row>
     <row r="162" spans="1:2">
@@ -1682,7 +1682,7 @@
         <v>43077</v>
       </c>
       <c r="B162">
-        <v>0.3984706</v>
+        <v>0.3615013</v>
       </c>
     </row>
     <row r="163" spans="1:2">
@@ -1690,7 +1690,7 @@
         <v>43078</v>
       </c>
       <c r="B163">
-        <v>0.4020805</v>
+        <v>0.3647366</v>
       </c>
     </row>
     <row r="164" spans="1:2">
@@ -1698,7 +1698,7 @@
         <v>43079</v>
       </c>
       <c r="B164">
-        <v>0.4056608</v>
+        <v>0.3679482</v>
       </c>
     </row>
     <row r="165" spans="1:2">
@@ -1706,7 +1706,7 @@
         <v>43080</v>
       </c>
       <c r="B165">
-        <v>0.4092106</v>
+        <v>0.3711351</v>
       </c>
     </row>
     <row r="166" spans="1:2">
@@ -1714,7 +1714,7 @@
         <v>43081</v>
       </c>
       <c r="B166">
-        <v>0.4127287</v>
+        <v>0.3742965</v>
       </c>
     </row>
     <row r="167" spans="1:2">
@@ -1722,7 +1722,7 @@
         <v>43082</v>
       </c>
       <c r="B167">
-        <v>0.416214</v>
+        <v>0.3774313</v>
       </c>
     </row>
     <row r="168" spans="1:2">
@@ -1730,7 +1730,7 @@
         <v>43083</v>
       </c>
       <c r="B168">
-        <v>0.4196655</v>
+        <v>0.3805386</v>
       </c>
     </row>
     <row r="169" spans="1:2">
@@ -1738,7 +1738,7 @@
         <v>43084</v>
       </c>
       <c r="B169">
-        <v>0.423082</v>
+        <v>0.3836175</v>
       </c>
     </row>
     <row r="170" spans="1:2">
@@ -1746,7 +1746,7 @@
         <v>43085</v>
       </c>
       <c r="B170">
-        <v>0.4264626</v>
+        <v>0.3866671</v>
       </c>
     </row>
     <row r="171" spans="1:2">
@@ -1754,7 +1754,7 @@
         <v>43086</v>
       </c>
       <c r="B171">
-        <v>0.4298061</v>
+        <v>0.3896865</v>
       </c>
     </row>
     <row r="172" spans="1:2">
@@ -1762,7 +1762,7 @@
         <v>43087</v>
       </c>
       <c r="B172">
-        <v>0.4331115</v>
+        <v>0.3926747</v>
       </c>
     </row>
     <row r="173" spans="1:2">
@@ -1770,7 +1770,7 @@
         <v>43088</v>
       </c>
       <c r="B173">
-        <v>0.4363776</v>
+        <v>0.3956309</v>
       </c>
     </row>
     <row r="174" spans="1:2">
@@ -1778,7 +1778,7 @@
         <v>43089</v>
       </c>
       <c r="B174">
-        <v>0.4396035</v>
+        <v>0.398554</v>
       </c>
     </row>
     <row r="175" spans="1:2">
@@ -1786,7 +1786,7 @@
         <v>43090</v>
       </c>
       <c r="B175">
-        <v>0.442788</v>
+        <v>0.4014433</v>
       </c>
     </row>
     <row r="176" spans="1:2">
@@ -1794,7 +1794,7 @@
         <v>43091</v>
       </c>
       <c r="B176">
-        <v>0.4459301</v>
+        <v>0.4042977</v>
       </c>
     </row>
     <row r="177" spans="1:2">
@@ -1802,7 +1802,7 @@
         <v>43092</v>
       </c>
       <c r="B177">
-        <v>0.4490287</v>
+        <v>0.4071164</v>
       </c>
     </row>
     <row r="178" spans="1:2">
@@ -1810,7 +1810,7 @@
         <v>43093</v>
       </c>
       <c r="B178">
-        <v>0.4520827</v>
+        <v>0.4098985</v>
       </c>
     </row>
     <row r="179" spans="1:2">
@@ -1818,7 +1818,7 @@
         <v>43094</v>
       </c>
       <c r="B179">
-        <v>0.4550911</v>
+        <v>0.4126431</v>
       </c>
     </row>
     <row r="180" spans="1:2">
@@ -1826,7 +1826,7 @@
         <v>43095</v>
       </c>
       <c r="B180">
-        <v>0.4580527</v>
+        <v>0.4153493</v>
       </c>
     </row>
     <row r="181" spans="1:2">
@@ -1834,7 +1834,7 @@
         <v>43096</v>
       </c>
       <c r="B181">
-        <v>0.4609667</v>
+        <v>0.4180161</v>
       </c>
     </row>
     <row r="182" spans="1:2">
@@ -1842,7 +1842,7 @@
         <v>43097</v>
       </c>
       <c r="B182">
-        <v>0.4638318</v>
+        <v>0.4206428</v>
       </c>
     </row>
     <row r="183" spans="1:2">
@@ -1850,7 +1850,7 @@
         <v>43098</v>
       </c>
       <c r="B183">
-        <v>0.4666471</v>
+        <v>0.4232283</v>
       </c>
     </row>
     <row r="184" spans="1:2">
@@ -1858,7 +1858,7 @@
         <v>43099</v>
       </c>
       <c r="B184">
-        <v>0.4694114</v>
+        <v>0.4257719</v>
       </c>
     </row>
     <row r="185" spans="1:2">
@@ -1866,7 +1866,7 @@
         <v>43100</v>
       </c>
       <c r="B185">
-        <v>0.4721237</v>
+        <v>0.4282726</v>
       </c>
     </row>
     <row r="186" spans="1:2">
@@ -1874,7 +1874,7 @@
         <v>43101</v>
       </c>
       <c r="B186">
-        <v>0.474783</v>
+        <v>0.4307296</v>
       </c>
     </row>
     <row r="187" spans="1:2">
@@ -1882,7 +1882,7 @@
         <v>43102</v>
       </c>
       <c r="B187">
-        <v>0.4773882</v>
+        <v>0.433142</v>
       </c>
     </row>
     <row r="188" spans="1:2">
@@ -1890,7 +1890,7 @@
         <v>43103</v>
       </c>
       <c r="B188">
-        <v>0.4799382</v>
+        <v>0.4355089</v>
       </c>
     </row>
     <row r="189" spans="1:2">
@@ -1898,7 +1898,7 @@
         <v>43104</v>
       </c>
       <c r="B189">
-        <v>0.482432</v>
+        <v>0.4378293</v>
       </c>
     </row>
     <row r="190" spans="1:2">
@@ -1906,7 +1906,7 @@
         <v>43105</v>
       </c>
       <c r="B190">
-        <v>0.4848685</v>
+        <v>0.4401026</v>
       </c>
     </row>
     <row r="191" spans="1:2">
@@ -1914,7 +1914,7 @@
         <v>43106</v>
       </c>
       <c r="B191">
-        <v>0.4872468</v>
+        <v>0.4423277</v>
       </c>
     </row>
     <row r="192" spans="1:2">
@@ -1922,7 +1922,7 @@
         <v>43107</v>
       </c>
       <c r="B192">
-        <v>0.4895657</v>
+        <v>0.4445039</v>
       </c>
     </row>
     <row r="193" spans="1:2">
@@ -1930,7 +1930,7 @@
         <v>43108</v>
       </c>
       <c r="B193">
-        <v>0.4918242</v>
+        <v>0.4466303</v>
       </c>
     </row>
     <row r="194" spans="1:2">
@@ -1938,7 +1938,7 @@
         <v>43109</v>
       </c>
       <c r="B194">
-        <v>0.4940212</v>
+        <v>0.4487059</v>
       </c>
     </row>
     <row r="195" spans="1:2">
@@ -1946,7 +1946,7 @@
         <v>43110</v>
       </c>
       <c r="B195">
-        <v>0.4961558</v>
+        <v>0.45073</v>
       </c>
     </row>
     <row r="196" spans="1:2">
@@ -1954,7 +1954,7 @@
         <v>43111</v>
       </c>
       <c r="B196">
-        <v>0.4982269</v>
+        <v>0.4527017</v>
       </c>
     </row>
     <row r="197" spans="1:2">
@@ -1962,7 +1962,7 @@
         <v>43112</v>
       </c>
       <c r="B197">
-        <v>0.5002333</v>
+        <v>0.4546202</v>
       </c>
     </row>
     <row r="198" spans="1:2">
@@ -1970,7 +1970,7 @@
         <v>43113</v>
       </c>
       <c r="B198">
-        <v>0.5021742</v>
+        <v>0.4564845</v>
       </c>
     </row>
     <row r="199" spans="1:2">
@@ -1978,7 +1978,7 @@
         <v>43114</v>
       </c>
       <c r="B199">
-        <v>0.5040484</v>
+        <v>0.4582939</v>
       </c>
     </row>
     <row r="200" spans="1:2">
@@ -1986,7 +1986,7 @@
         <v>43115</v>
       </c>
       <c r="B200">
-        <v>0.5058549</v>
+        <v>0.4600475</v>
       </c>
     </row>
     <row r="201" spans="1:2">
@@ -1994,7 +1994,7 @@
         <v>43116</v>
       </c>
       <c r="B201">
-        <v>0.5075927</v>
+        <v>0.4617445</v>
       </c>
     </row>
     <row r="202" spans="1:2">
@@ -2002,7 +2002,7 @@
         <v>43117</v>
       </c>
       <c r="B202">
-        <v>0.5092607</v>
+        <v>0.463384</v>
       </c>
     </row>
     <row r="203" spans="1:2">
@@ -2010,7 +2010,7 @@
         <v>43118</v>
       </c>
       <c r="B203">
-        <v>0.510858</v>
+        <v>0.4649652</v>
       </c>
     </row>
     <row r="204" spans="1:2">
@@ -2018,7 +2018,7 @@
         <v>43119</v>
       </c>
       <c r="B204">
-        <v>0.5123834</v>
+        <v>0.4664873</v>
       </c>
     </row>
     <row r="205" spans="1:2">
@@ -2026,7 +2026,7 @@
         <v>43120</v>
       </c>
       <c r="B205">
-        <v>0.513836</v>
+        <v>0.4679494</v>
       </c>
     </row>
     <row r="206" spans="1:2">
@@ -2034,7 +2034,7 @@
         <v>43121</v>
       </c>
       <c r="B206">
-        <v>0.5152147</v>
+        <v>0.4693507</v>
       </c>
     </row>
     <row r="207" spans="1:2">
@@ -2042,7 +2042,7 @@
         <v>43122</v>
       </c>
       <c r="B207">
-        <v>0.5165185</v>
+        <v>0.4706904</v>
       </c>
     </row>
     <row r="208" spans="1:2">
@@ -2050,7 +2050,7 @@
         <v>43123</v>
       </c>
       <c r="B208">
-        <v>0.5177463</v>
+        <v>0.4719677</v>
       </c>
     </row>
     <row r="209" spans="1:2">
@@ -2058,7 +2058,7 @@
         <v>43124</v>
       </c>
       <c r="B209">
-        <v>0.5188971999999999</v>
+        <v>0.4731817</v>
       </c>
     </row>
     <row r="210" spans="1:2">
@@ -2066,7 +2066,7 @@
         <v>43125</v>
       </c>
       <c r="B210">
-        <v>0.5199702</v>
+        <v>0.4743316</v>
       </c>
     </row>
     <row r="211" spans="1:2">
@@ -2074,7 +2074,7 @@
         <v>43126</v>
       </c>
       <c r="B211">
-        <v>0.5209641</v>
+        <v>0.4754167</v>
       </c>
     </row>
     <row r="212" spans="1:2">
@@ -2082,7 +2082,7 @@
         <v>43127</v>
       </c>
       <c r="B212">
-        <v>0.521878</v>
+        <v>0.4764361</v>
       </c>
     </row>
     <row r="213" spans="1:2">
@@ -2090,7 +2090,7 @@
         <v>43128</v>
       </c>
       <c r="B213">
-        <v>0.5227108</v>
+        <v>0.477389</v>
       </c>
     </row>
     <row r="214" spans="1:2">
@@ -2098,7 +2098,7 @@
         <v>43129</v>
       </c>
       <c r="B214">
-        <v>0.5234616</v>
+        <v>0.4782745</v>
       </c>
     </row>
     <row r="215" spans="1:2">
@@ -2106,7 +2106,7 @@
         <v>43130</v>
       </c>
       <c r="B215">
-        <v>0.5241293</v>
+        <v>0.479092</v>
       </c>
     </row>
     <row r="216" spans="1:2">
@@ -2114,7 +2114,7 @@
         <v>43131</v>
       </c>
       <c r="B216">
-        <v>0.524713</v>
+        <v>0.4798406</v>
       </c>
     </row>
     <row r="217" spans="1:2">
@@ -2122,7 +2122,7 @@
         <v>43132</v>
       </c>
       <c r="B217">
-        <v>0.5252115000000001</v>
+        <v>0.4805195</v>
       </c>
     </row>
     <row r="218" spans="1:2">
@@ -2130,7 +2130,7 @@
         <v>43133</v>
       </c>
       <c r="B218">
-        <v>0.5256239</v>
+        <v>0.4811278</v>
       </c>
     </row>
     <row r="219" spans="1:2">
@@ -2138,7 +2138,7 @@
         <v>43134</v>
       </c>
       <c r="B219">
-        <v>0.5259490999999999</v>
+        <v>0.4816649</v>
       </c>
     </row>
     <row r="220" spans="1:2">
@@ -2146,7 +2146,7 @@
         <v>43135</v>
       </c>
       <c r="B220">
-        <v>0.5261862</v>
+        <v>0.48213</v>
       </c>
     </row>
     <row r="221" spans="1:2">
@@ -2154,7 +2154,7 @@
         <v>43136</v>
       </c>
       <c r="B221">
-        <v>0.5263342</v>
+        <v>0.4825221</v>
       </c>
     </row>
     <row r="222" spans="1:2">
@@ -2162,7 +2162,7 @@
         <v>43137</v>
       </c>
       <c r="B222">
-        <v>0.526392</v>
+        <v>0.4828406</v>
       </c>
     </row>
     <row r="223" spans="1:2">
@@ -2170,7 +2170,7 @@
         <v>43138</v>
       </c>
       <c r="B223">
-        <v>0.5263587</v>
+        <v>0.4830847</v>
       </c>
     </row>
     <row r="224" spans="1:2">
@@ -2178,7 +2178,7 @@
         <v>43139</v>
       </c>
       <c r="B224">
-        <v>0.5262332</v>
+        <v>0.4832537</v>
       </c>
     </row>
     <row r="225" spans="1:2">
@@ -2186,7 +2186,7 @@
         <v>43140</v>
       </c>
       <c r="B225">
-        <v>0.5260145000000001</v>
+        <v>0.4833466</v>
       </c>
     </row>
     <row r="226" spans="1:2">
@@ -2194,7 +2194,7 @@
         <v>43141</v>
       </c>
       <c r="B226">
-        <v>0.5257016</v>
+        <v>0.4833628</v>
       </c>
     </row>
     <row r="227" spans="1:2">
@@ -2202,7 +2202,7 @@
         <v>43142</v>
       </c>
       <c r="B227">
-        <v>0.5252936</v>
+        <v>0.4833015</v>
       </c>
     </row>
     <row r="228" spans="1:2">
@@ -2210,7 +2210,7 @@
         <v>43143</v>
       </c>
       <c r="B228">
-        <v>0.5247894</v>
+        <v>0.4831619</v>
       </c>
     </row>
     <row r="229" spans="1:2">
@@ -2218,7 +2218,7 @@
         <v>43144</v>
       </c>
       <c r="B229">
-        <v>0.524188</v>
+        <v>0.4829432</v>
       </c>
     </row>
     <row r="230" spans="1:2">
@@ -2226,7 +2226,7 @@
         <v>43145</v>
       </c>
       <c r="B230">
-        <v>0.5234885</v>
+        <v>0.4826448</v>
       </c>
     </row>
     <row r="231" spans="1:2">
@@ -2234,7 +2234,7 @@
         <v>43146</v>
       </c>
       <c r="B231">
-        <v>0.5226898</v>
+        <v>0.4822657</v>
       </c>
     </row>
     <row r="232" spans="1:2">
@@ -2242,7 +2242,7 @@
         <v>43147</v>
       </c>
       <c r="B232">
-        <v>0.5217908999999999</v>
+        <v>0.4818054</v>
       </c>
     </row>
     <row r="233" spans="1:2">
@@ -2250,7 +2250,7 @@
         <v>43148</v>
       </c>
       <c r="B233">
-        <v>0.5207908999999999</v>
+        <v>0.481263</v>
       </c>
     </row>
     <row r="234" spans="1:2">
@@ -2258,7 +2258,7 @@
         <v>43149</v>
       </c>
       <c r="B234">
-        <v>0.5196888</v>
+        <v>0.4806378</v>
       </c>
     </row>
     <row r="235" spans="1:2">
@@ -2266,7 +2266,7 @@
         <v>43150</v>
       </c>
       <c r="B235">
-        <v>0.5184835</v>
+        <v>0.479929</v>
       </c>
     </row>
     <row r="236" spans="1:2">
@@ -2274,7 +2274,7 @@
         <v>43151</v>
       </c>
       <c r="B236">
-        <v>0.5171741</v>
+        <v>0.4791359</v>
       </c>
     </row>
     <row r="237" spans="1:2">
@@ -2282,7 +2282,7 @@
         <v>43152</v>
       </c>
       <c r="B237">
-        <v>0.5157596</v>
+        <v>0.4782578</v>
       </c>
     </row>
     <row r="238" spans="1:2">
@@ -2290,7 +2290,7 @@
         <v>43153</v>
       </c>
       <c r="B238">
-        <v>0.5142390999999999</v>
+        <v>0.4772938</v>
       </c>
     </row>
     <row r="239" spans="1:2">
@@ -2298,7 +2298,7 @@
         <v>43154</v>
       </c>
       <c r="B239">
-        <v>0.5126114000000001</v>
+        <v>0.4762434</v>
       </c>
     </row>
     <row r="240" spans="1:2">
@@ -2306,7 +2306,7 @@
         <v>43155</v>
       </c>
       <c r="B240">
-        <v>0.5108757</v>
+        <v>0.4751056</v>
       </c>
     </row>
     <row r="241" spans="1:2">
@@ -2314,7 +2314,7 @@
         <v>43156</v>
       </c>
       <c r="B241">
-        <v>0.509031</v>
+        <v>0.4738799</v>
       </c>
     </row>
     <row r="242" spans="1:2">
@@ -2322,7 +2322,7 @@
         <v>43157</v>
       </c>
       <c r="B242">
-        <v>0.5070762</v>
+        <v>0.4725655</v>
       </c>
     </row>
     <row r="243" spans="1:2">
@@ -2330,7 +2330,7 @@
         <v>43158</v>
       </c>
       <c r="B243">
-        <v>0.5050104</v>
+        <v>0.4711616</v>
       </c>
     </row>
     <row r="244" spans="1:2">
@@ -2338,7 +2338,7 @@
         <v>43159</v>
       </c>
       <c r="B244">
-        <v>0.5028327</v>
+        <v>0.4696675</v>
       </c>
     </row>
     <row r="245" spans="1:2">
@@ -2346,7 +2346,7 @@
         <v>43160</v>
       </c>
       <c r="B245">
-        <v>0.500542</v>
+        <v>0.4680826</v>
       </c>
     </row>
     <row r="246" spans="1:2">
@@ -2354,7 +2354,7 @@
         <v>43161</v>
       </c>
       <c r="B246">
-        <v>0.4981374</v>
+        <v>0.466406</v>
       </c>
     </row>
     <row r="247" spans="1:2">
@@ -2362,7 +2362,7 @@
         <v>43162</v>
       </c>
       <c r="B247">
-        <v>0.4956179</v>
+        <v>0.4646372</v>
       </c>
     </row>
     <row r="248" spans="1:2">
@@ -2370,7 +2370,7 @@
         <v>43163</v>
       </c>
       <c r="B248">
-        <v>0.4929825</v>
+        <v>0.4627753</v>
       </c>
     </row>
     <row r="249" spans="1:2">
@@ -2378,7 +2378,7 @@
         <v>43164</v>
       </c>
       <c r="B249">
-        <v>0.4902303</v>
+        <v>0.4608196</v>
       </c>
     </row>
     <row r="250" spans="1:2">
@@ -2386,7 +2386,7 @@
         <v>43165</v>
       </c>
       <c r="B250">
-        <v>0.4873603</v>
+        <v>0.4587695</v>
       </c>
     </row>
     <row r="251" spans="1:2">
@@ -2394,7 +2394,7 @@
         <v>43166</v>
       </c>
       <c r="B251">
-        <v>0.4843714</v>
+        <v>0.4566243</v>
       </c>
     </row>
     <row r="252" spans="1:2">
@@ -2402,7 +2402,7 @@
         <v>43167</v>
       </c>
       <c r="B252">
-        <v>0.4812629</v>
+        <v>0.4543832</v>
       </c>
     </row>
     <row r="253" spans="1:2">
@@ -2410,7 +2410,7 @@
         <v>43168</v>
       </c>
       <c r="B253">
-        <v>0.4780336</v>
+        <v>0.4520455</v>
       </c>
     </row>
     <row r="254" spans="1:2">
@@ -2418,7 +2418,7 @@
         <v>43169</v>
       </c>
       <c r="B254">
-        <v>0.4746827</v>
+        <v>0.4496107</v>
       </c>
     </row>
     <row r="255" spans="1:2">
@@ -2426,7 +2426,7 @@
         <v>43170</v>
       </c>
       <c r="B255">
-        <v>0.4712091</v>
+        <v>0.4470778</v>
       </c>
     </row>
     <row r="256" spans="1:2">
@@ -2434,7 +2434,7 @@
         <v>43171</v>
       </c>
       <c r="B256">
-        <v>0.4676119</v>
+        <v>0.4444464</v>
       </c>
     </row>
     <row r="257" spans="1:2">
@@ -2442,7 +2442,7 @@
         <v>43172</v>
       </c>
       <c r="B257">
-        <v>0.4638902</v>
+        <v>0.4417156</v>
       </c>
     </row>
     <row r="258" spans="1:2">
@@ -2450,7 +2450,7 @@
         <v>43173</v>
       </c>
       <c r="B258">
-        <v>0.4600429</v>
+        <v>0.4388849</v>
       </c>
     </row>
     <row r="259" spans="1:2">
@@ -2458,7 +2458,7 @@
         <v>43174</v>
       </c>
       <c r="B259">
-        <v>0.4560691</v>
+        <v>0.4359534</v>
       </c>
     </row>
     <row r="260" spans="1:2">
@@ -2466,7 +2466,7 @@
         <v>43175</v>
       </c>
       <c r="B260">
-        <v>0.451968</v>
+        <v>0.4329206</v>
       </c>
     </row>
     <row r="261" spans="1:2">
@@ -2474,7 +2474,7 @@
         <v>43176</v>
       </c>
       <c r="B261">
-        <v>0.4477384</v>
+        <v>0.4297858</v>
       </c>
     </row>
     <row r="262" spans="1:2">
@@ -2482,7 +2482,7 @@
         <v>43177</v>
       </c>
       <c r="B262">
-        <v>0.4433795</v>
+        <v>0.4265482</v>
       </c>
     </row>
     <row r="263" spans="1:2">
@@ -2490,7 +2490,7 @@
         <v>43178</v>
       </c>
       <c r="B263">
-        <v>0.4388903</v>
+        <v>0.4232073</v>
       </c>
     </row>
     <row r="264" spans="1:2">
@@ -2498,7 +2498,7 @@
         <v>43179</v>
       </c>
       <c r="B264">
-        <v>0.4342699</v>
+        <v>0.4197623</v>
       </c>
     </row>
     <row r="265" spans="1:2">
@@ -2506,7 +2506,7 @@
         <v>43180</v>
       </c>
       <c r="B265">
-        <v>0.4295173</v>
+        <v>0.4162126</v>
       </c>
     </row>
     <row r="266" spans="1:2">
@@ -2514,7 +2514,7 @@
         <v>43181</v>
       </c>
       <c r="B266">
-        <v>0.4246315</v>
+        <v>0.4125576</v>
       </c>
     </row>
     <row r="267" spans="1:2">
@@ -2522,7 +2522,7 @@
         <v>43182</v>
       </c>
       <c r="B267">
-        <v>0.4196117</v>
+        <v>0.4087965</v>
       </c>
     </row>
     <row r="268" spans="1:2">
@@ -2530,7 +2530,7 @@
         <v>43183</v>
       </c>
       <c r="B268">
-        <v>0.4144568</v>
+        <v>0.4049287</v>
       </c>
     </row>
     <row r="269" spans="1:2">
@@ -2538,7 +2538,7 @@
         <v>43184</v>
       </c>
       <c r="B269">
-        <v>0.4091659</v>
+        <v>0.4009536</v>
       </c>
     </row>
     <row r="270" spans="1:2">
@@ -2546,7 +2546,7 @@
         <v>43185</v>
       </c>
       <c r="B270">
-        <v>0.4037382</v>
+        <v>0.3968704</v>
       </c>
     </row>
     <row r="271" spans="1:2">
@@ -2554,7 +2554,7 @@
         <v>43186</v>
       </c>
       <c r="B271">
-        <v>0.3981725</v>
+        <v>0.3926787</v>
       </c>
     </row>
     <row r="272" spans="1:2">
@@ -2562,7 +2562,7 @@
         <v>43187</v>
       </c>
       <c r="B272">
-        <v>0.3924681</v>
+        <v>0.3883776</v>
       </c>
     </row>
     <row r="273" spans="1:2">
@@ -2570,7 +2570,7 @@
         <v>43188</v>
       </c>
       <c r="B273">
-        <v>0.3866239</v>
+        <v>0.3839666</v>
       </c>
     </row>
     <row r="274" spans="1:2">
@@ -2578,7 +2578,7 @@
         <v>43189</v>
       </c>
       <c r="B274">
-        <v>0.3806391</v>
+        <v>0.379445</v>
       </c>
     </row>
     <row r="275" spans="1:2">
@@ -2586,7 +2586,7 @@
         <v>43190</v>
       </c>
       <c r="B275">
-        <v>0.3745126</v>
+        <v>0.3748122</v>
       </c>
     </row>
     <row r="276" spans="1:2">
@@ -2594,7 +2594,7 @@
         <v>43191</v>
       </c>
       <c r="B276">
-        <v>0.3682436</v>
+        <v>0.3700676</v>
       </c>
     </row>
     <row r="277" spans="1:2">
@@ -2602,7 +2602,7 @@
         <v>43192</v>
       </c>
       <c r="B277">
-        <v>0.3618312</v>
+        <v>0.3652104</v>
       </c>
     </row>
     <row r="278" spans="1:2">
@@ -2610,7 +2610,7 @@
         <v>43193</v>
       </c>
       <c r="B278">
-        <v>0.3552743</v>
+        <v>0.3602402</v>
       </c>
     </row>
     <row r="279" spans="1:2">
@@ -2618,7 +2618,7 @@
         <v>43194</v>
       </c>
       <c r="B279">
-        <v>0.3485721</v>
+        <v>0.3551562</v>
       </c>
     </row>
     <row r="280" spans="1:2">
@@ -2626,7 +2626,7 @@
         <v>43195</v>
       </c>
       <c r="B280">
-        <v>0.3417236</v>
+        <v>0.3499579</v>
       </c>
     </row>
     <row r="281" spans="1:2">
@@ -2634,7 +2634,7 @@
         <v>43196</v>
       </c>
       <c r="B281">
-        <v>0.3347279</v>
+        <v>0.3446446</v>
       </c>
     </row>
     <row r="282" spans="1:2">
@@ -2642,7 +2642,7 @@
         <v>43197</v>
       </c>
       <c r="B282">
-        <v>0.3275841</v>
+        <v>0.3392156</v>
       </c>
     </row>
     <row r="283" spans="1:2">
@@ -2650,7 +2650,7 @@
         <v>43198</v>
       </c>
       <c r="B283">
-        <v>0.3202913</v>
+        <v>0.3336705</v>
       </c>
     </row>
     <row r="284" spans="1:2">
@@ -2658,7 +2658,7 @@
         <v>43199</v>
       </c>
       <c r="B284">
-        <v>0.3128484</v>
+        <v>0.3280085</v>
       </c>
     </row>
     <row r="285" spans="1:2">
@@ -2666,7 +2666,7 @@
         <v>43200</v>
       </c>
       <c r="B285">
-        <v>0.3052547</v>
+        <v>0.3222291</v>
       </c>
     </row>
     <row r="286" spans="1:2">
@@ -2674,7 +2674,7 @@
         <v>43201</v>
       </c>
       <c r="B286">
-        <v>0.2975092</v>
+        <v>0.3163316</v>
       </c>
     </row>
     <row r="287" spans="1:2">
@@ -2682,7 +2682,7 @@
         <v>43202</v>
       </c>
       <c r="B287">
-        <v>0.2896109</v>
+        <v>0.3103154</v>
       </c>
     </row>
     <row r="288" spans="1:2">
@@ -2690,7 +2690,7 @@
         <v>43203</v>
       </c>
       <c r="B288">
-        <v>0.281559</v>
+        <v>0.3041801</v>
       </c>
     </row>
     <row r="289" spans="1:2">
@@ -2698,7 +2698,7 @@
         <v>43204</v>
       </c>
       <c r="B289">
-        <v>0.2733525</v>
+        <v>0.2979248</v>
       </c>
     </row>
     <row r="290" spans="1:2">
@@ -2706,7 +2706,7 @@
         <v>43205</v>
       </c>
       <c r="B290">
-        <v>0.2649906</v>
+        <v>0.2915491</v>
       </c>
     </row>
     <row r="291" spans="1:2">
@@ -2714,7 +2714,7 @@
         <v>43206</v>
       </c>
       <c r="B291">
-        <v>0.2564722</v>
+        <v>0.2850523</v>
       </c>
     </row>
     <row r="292" spans="1:2">
@@ -2722,7 +2722,7 @@
         <v>43207</v>
       </c>
       <c r="B292">
-        <v>0.2477966</v>
+        <v>0.2784339</v>
       </c>
     </row>
     <row r="293" spans="1:2">
@@ -2730,7 +2730,7 @@
         <v>43208</v>
       </c>
       <c r="B293">
-        <v>0.2389627</v>
+        <v>0.2716933</v>
       </c>
     </row>
     <row r="294" spans="1:2">
@@ -2738,7 +2738,7 @@
         <v>43209</v>
       </c>
       <c r="B294">
-        <v>0.2299696</v>
+        <v>0.2648298</v>
       </c>
     </row>
     <row r="295" spans="1:2">
@@ -2746,7 +2746,7 @@
         <v>43210</v>
       </c>
       <c r="B295">
-        <v>0.2208166</v>
+        <v>0.257843</v>
       </c>
     </row>
     <row r="296" spans="1:2">
@@ -2754,7 +2754,7 @@
         <v>43211</v>
       </c>
       <c r="B296">
-        <v>0.2115025</v>
+        <v>0.2507322</v>
       </c>
     </row>
     <row r="297" spans="1:2">
@@ -2762,7 +2762,7 @@
         <v>43212</v>
       </c>
       <c r="B297">
-        <v>0.2020267</v>
+        <v>0.2434968</v>
       </c>
     </row>
     <row r="298" spans="1:2">
@@ -2770,7 +2770,7 @@
         <v>43213</v>
       </c>
       <c r="B298">
-        <v>0.192388</v>
+        <v>0.2361362</v>
       </c>
     </row>
     <row r="299" spans="1:2">
@@ -2778,7 +2778,7 @@
         <v>43214</v>
       </c>
       <c r="B299">
-        <v>0.1825858</v>
+        <v>0.22865</v>
       </c>
     </row>
     <row r="300" spans="1:2">
@@ -2786,7 +2786,7 @@
         <v>43215</v>
       </c>
       <c r="B300">
-        <v>0.1726189</v>
+        <v>0.2210375</v>
       </c>
     </row>
     <row r="301" spans="1:2">
@@ -2794,7 +2794,7 @@
         <v>43216</v>
       </c>
       <c r="B301">
-        <v>0.1624866</v>
+        <v>0.2132982</v>
       </c>
     </row>
     <row r="302" spans="1:2">
@@ -2802,7 +2802,7 @@
         <v>43217</v>
       </c>
       <c r="B302">
-        <v>0.1521879</v>
+        <v>0.2054314</v>
       </c>
     </row>
     <row r="303" spans="1:2">
@@ -2810,7 +2810,7 @@
         <v>43218</v>
       </c>
       <c r="B303">
-        <v>0.1417219</v>
+        <v>0.1974367</v>
       </c>
     </row>
     <row r="304" spans="1:2">
@@ -2818,7 +2818,7 @@
         <v>43219</v>
       </c>
       <c r="B304">
-        <v>0.1310878</v>
+        <v>0.1893135</v>
       </c>
     </row>
     <row r="305" spans="1:2">
@@ -2826,7 +2826,7 @@
         <v>43220</v>
       </c>
       <c r="B305">
-        <v>0.1202847</v>
+        <v>0.1810611</v>
       </c>
     </row>
     <row r="306" spans="1:2">
@@ -2834,7 +2834,7 @@
         <v>43221</v>
       </c>
       <c r="B306">
-        <v>0.1093116</v>
+        <v>0.1726792</v>
       </c>
     </row>
     <row r="307" spans="1:2">
@@ -2842,7 +2842,7 @@
         <v>43222</v>
       </c>
       <c r="B307">
-        <v>0.09816759999999999</v>
+        <v>0.164167</v>
       </c>
     </row>
     <row r="308" spans="1:2">
@@ -2850,7 +2850,7 @@
         <v>43223</v>
       </c>
       <c r="B308">
-        <v>0.0868519</v>
+        <v>0.1555241</v>
       </c>
     </row>
     <row r="309" spans="1:2">
@@ -2858,7 +2858,7 @@
         <v>43224</v>
       </c>
       <c r="B309">
-        <v>0.0753636</v>
+        <v>0.14675</v>
       </c>
     </row>
     <row r="310" spans="1:2">
@@ -2866,7 +2866,7 @@
         <v>43225</v>
       </c>
       <c r="B310">
-        <v>0.0637018</v>
+        <v>0.137844</v>
       </c>
     </row>
     <row r="311" spans="1:2">
@@ -2874,7 +2874,7 @@
         <v>43226</v>
       </c>
       <c r="B311">
-        <v>0.0518656</v>
+        <v>0.1288056</v>
       </c>
     </row>
     <row r="312" spans="1:2">
@@ -2882,7 +2882,7 @@
         <v>43227</v>
       </c>
       <c r="B312">
-        <v>0.0398541</v>
+        <v>0.1196344</v>
       </c>
     </row>
     <row r="313" spans="1:2">
@@ -2890,7 +2890,7 @@
         <v>43228</v>
       </c>
       <c r="B313">
-        <v>0.0276664</v>
+        <v>0.1103297</v>
       </c>
     </row>
     <row r="314" spans="1:2">
@@ -2898,7 +2898,7 @@
         <v>43229</v>
       </c>
       <c r="B314">
-        <v>0.0153017</v>
+        <v>0.1008911</v>
       </c>
     </row>
     <row r="315" spans="1:2">
@@ -2906,7 +2906,7 @@
         <v>43230</v>
       </c>
       <c r="B315">
-        <v>0.0027591</v>
+        <v>0.09131789999999999</v>
       </c>
     </row>
     <row r="316" spans="1:2">
@@ -2914,7 +2914,7 @@
         <v>43231</v>
       </c>
       <c r="B316">
-        <v>0.0027591</v>
+        <v>0.0816098</v>
       </c>
     </row>
     <row r="317" spans="1:2">
@@ -2922,7 +2922,7 @@
         <v>43232</v>
       </c>
       <c r="B317">
-        <v>0.0027591</v>
+        <v>0.0717661</v>
       </c>
     </row>
     <row r="318" spans="1:2">
@@ -2930,7 +2930,7 @@
         <v>43233</v>
       </c>
       <c r="B318">
-        <v>0.0027591</v>
+        <v>0.0617863</v>
       </c>
     </row>
     <row r="319" spans="1:2">
@@ -2938,7 +2938,7 @@
         <v>43234</v>
       </c>
       <c r="B319">
-        <v>0.0027591</v>
+        <v>0.05167</v>
       </c>
     </row>
     <row r="320" spans="1:2">
@@ -2946,7 +2946,7 @@
         <v>43235</v>
       </c>
       <c r="B320">
-        <v>0.0027591</v>
+        <v>0.0414165</v>
       </c>
     </row>
     <row r="321" spans="1:2">
@@ -2954,7 +2954,7 @@
         <v>43236</v>
       </c>
       <c r="B321">
-        <v>0.0027591</v>
+        <v>0.0310255</v>
       </c>
     </row>
     <row r="322" spans="1:2">
@@ -2962,7 +2962,7 @@
         <v>43237</v>
       </c>
       <c r="B322">
-        <v>0.0027591</v>
+        <v>0.0204964</v>
       </c>
     </row>
     <row r="323" spans="1:2">
@@ -2970,7 +2970,7 @@
         <v>43238</v>
       </c>
       <c r="B323">
-        <v>0.0027591</v>
+        <v>0.0098286</v>
       </c>
     </row>
     <row r="324" spans="1:2">
@@ -2978,7 +2978,7 @@
         <v>43239</v>
       </c>
       <c r="B324">
-        <v>0.0027591</v>
+        <v>0.0098286</v>
       </c>
     </row>
     <row r="325" spans="1:2">
@@ -2986,7 +2986,7 @@
         <v>43240</v>
       </c>
       <c r="B325">
-        <v>0.0027591</v>
+        <v>0.0098286</v>
       </c>
     </row>
     <row r="326" spans="1:2">
@@ -2994,7 +2994,7 @@
         <v>43241</v>
       </c>
       <c r="B326">
-        <v>0.0027591</v>
+        <v>0.0098286</v>
       </c>
     </row>
     <row r="327" spans="1:2">
@@ -3002,7 +3002,7 @@
         <v>43242</v>
       </c>
       <c r="B327">
-        <v>0.0027591</v>
+        <v>0.0098286</v>
       </c>
     </row>
     <row r="328" spans="1:2">
@@ -3010,7 +3010,7 @@
         <v>43243</v>
       </c>
       <c r="B328">
-        <v>0.0027591</v>
+        <v>0.0098286</v>
       </c>
     </row>
     <row r="329" spans="1:2">
@@ -3018,7 +3018,7 @@
         <v>43244</v>
       </c>
       <c r="B329">
-        <v>0.0027591</v>
+        <v>0.0098286</v>
       </c>
     </row>
     <row r="330" spans="1:2">
@@ -3026,7 +3026,7 @@
         <v>43245</v>
       </c>
       <c r="B330">
-        <v>0.0027591</v>
+        <v>0.0098286</v>
       </c>
     </row>
     <row r="331" spans="1:2">
@@ -3034,7 +3034,7 @@
         <v>43246</v>
       </c>
       <c r="B331">
-        <v>0.0027591</v>
+        <v>0.0098286</v>
       </c>
     </row>
     <row r="332" spans="1:2">
@@ -3042,7 +3042,7 @@
         <v>43247</v>
       </c>
       <c r="B332">
-        <v>0.0027591</v>
+        <v>0.0098286</v>
       </c>
     </row>
     <row r="333" spans="1:2">
@@ -3050,7 +3050,7 @@
         <v>43248</v>
       </c>
       <c r="B333">
-        <v>0.0027591</v>
+        <v>0.0098286</v>
       </c>
     </row>
     <row r="334" spans="1:2">
@@ -3058,7 +3058,7 @@
         <v>43249</v>
       </c>
       <c r="B334">
-        <v>0.0027591</v>
+        <v>0.0098286</v>
       </c>
     </row>
     <row r="335" spans="1:2">
@@ -3066,7 +3066,7 @@
         <v>43250</v>
       </c>
       <c r="B335">
-        <v>0.0027591</v>
+        <v>0.0098286</v>
       </c>
     </row>
     <row r="336" spans="1:2">
@@ -3074,7 +3074,7 @@
         <v>43251</v>
       </c>
       <c r="B336">
-        <v>0.0027591</v>
+        <v>0.0098286</v>
       </c>
     </row>
     <row r="337" spans="1:2">
@@ -3082,7 +3082,7 @@
         <v>43252</v>
       </c>
       <c r="B337">
-        <v>0.0027591</v>
+        <v>0.0098286</v>
       </c>
     </row>
     <row r="338" spans="1:2">
@@ -3090,7 +3090,7 @@
         <v>43253</v>
       </c>
       <c r="B338">
-        <v>0.0027591</v>
+        <v>0.0098286</v>
       </c>
     </row>
     <row r="339" spans="1:2">
@@ -3098,7 +3098,7 @@
         <v>43254</v>
       </c>
       <c r="B339">
-        <v>0.0027591</v>
+        <v>0.0098286</v>
       </c>
     </row>
     <row r="340" spans="1:2">
@@ -3106,7 +3106,7 @@
         <v>43255</v>
       </c>
       <c r="B340">
-        <v>0.0027591</v>
+        <v>0.0098286</v>
       </c>
     </row>
     <row r="341" spans="1:2">
@@ -3114,7 +3114,7 @@
         <v>43256</v>
       </c>
       <c r="B341">
-        <v>0.0027591</v>
+        <v>0.0098286</v>
       </c>
     </row>
     <row r="342" spans="1:2">
@@ -3122,7 +3122,7 @@
         <v>43257</v>
       </c>
       <c r="B342">
-        <v>0.0027591</v>
+        <v>0.0098286</v>
       </c>
     </row>
     <row r="343" spans="1:2">
@@ -3130,7 +3130,7 @@
         <v>43258</v>
       </c>
       <c r="B343">
-        <v>0.0027591</v>
+        <v>0.0098286</v>
       </c>
     </row>
     <row r="344" spans="1:2">
@@ -3138,7 +3138,7 @@
         <v>43259</v>
       </c>
       <c r="B344">
-        <v>0.0027591</v>
+        <v>0.0098286</v>
       </c>
     </row>
     <row r="345" spans="1:2">
@@ -3146,7 +3146,7 @@
         <v>43260</v>
       </c>
       <c r="B345">
-        <v>0.0027591</v>
+        <v>0.0098286</v>
       </c>
     </row>
     <row r="346" spans="1:2">
@@ -3154,7 +3154,7 @@
         <v>43261</v>
       </c>
       <c r="B346">
-        <v>0.0027591</v>
+        <v>0.0098286</v>
       </c>
     </row>
     <row r="347" spans="1:2">
@@ -3162,7 +3162,7 @@
         <v>43262</v>
       </c>
       <c r="B347">
-        <v>0.0027591</v>
+        <v>0.0098286</v>
       </c>
     </row>
     <row r="348" spans="1:2">
@@ -3170,7 +3170,7 @@
         <v>43263</v>
       </c>
       <c r="B348">
-        <v>0.0027591</v>
+        <v>0.0098286</v>
       </c>
     </row>
     <row r="349" spans="1:2">
@@ -3178,7 +3178,7 @@
         <v>43264</v>
       </c>
       <c r="B349">
-        <v>0.0027591</v>
+        <v>0.0098286</v>
       </c>
     </row>
     <row r="350" spans="1:2">
@@ -3186,7 +3186,7 @@
         <v>43265</v>
       </c>
       <c r="B350">
-        <v>0.0027591</v>
+        <v>0.0098286</v>
       </c>
     </row>
     <row r="351" spans="1:2">
@@ -3194,7 +3194,7 @@
         <v>43266</v>
       </c>
       <c r="B351">
-        <v>0.0027591</v>
+        <v>0.0098286</v>
       </c>
     </row>
     <row r="352" spans="1:2">
@@ -3202,7 +3202,7 @@
         <v>43267</v>
       </c>
       <c r="B352">
-        <v>0.0027591</v>
+        <v>0.0098286</v>
       </c>
     </row>
     <row r="353" spans="1:2">
@@ -3210,7 +3210,7 @@
         <v>43268</v>
       </c>
       <c r="B353">
-        <v>0.0027591</v>
+        <v>0.0098286</v>
       </c>
     </row>
     <row r="354" spans="1:2">
@@ -3218,7 +3218,7 @@
         <v>43269</v>
       </c>
       <c r="B354">
-        <v>0.0027591</v>
+        <v>0.0098286</v>
       </c>
     </row>
     <row r="355" spans="1:2">
@@ -3226,7 +3226,7 @@
         <v>43270</v>
       </c>
       <c r="B355">
-        <v>0.0027591</v>
+        <v>0.0098286</v>
       </c>
     </row>
     <row r="356" spans="1:2">
@@ -3234,7 +3234,7 @@
         <v>43271</v>
       </c>
       <c r="B356">
-        <v>0.0027591</v>
+        <v>0.0098286</v>
       </c>
     </row>
     <row r="357" spans="1:2">
@@ -3242,7 +3242,7 @@
         <v>43272</v>
       </c>
       <c r="B357">
-        <v>0.0027591</v>
+        <v>0.0098286</v>
       </c>
     </row>
     <row r="358" spans="1:2">
@@ -3250,7 +3250,7 @@
         <v>43273</v>
       </c>
       <c r="B358">
-        <v>0.0027591</v>
+        <v>0.0098286</v>
       </c>
     </row>
     <row r="359" spans="1:2">
@@ -3258,7 +3258,7 @@
         <v>43274</v>
       </c>
       <c r="B359">
-        <v>0.0027591</v>
+        <v>0.0098286</v>
       </c>
     </row>
     <row r="360" spans="1:2">
@@ -3266,7 +3266,7 @@
         <v>43275</v>
       </c>
       <c r="B360">
-        <v>0.0027591</v>
+        <v>0.0098286</v>
       </c>
     </row>
     <row r="361" spans="1:2">
@@ -3274,7 +3274,7 @@
         <v>43276</v>
       </c>
       <c r="B361">
-        <v>0.0027591</v>
+        <v>0.0098286</v>
       </c>
     </row>
     <row r="362" spans="1:2">
@@ -3282,7 +3282,7 @@
         <v>43277</v>
       </c>
       <c r="B362">
-        <v>0.0027591</v>
+        <v>0.0098286</v>
       </c>
     </row>
     <row r="363" spans="1:2">
@@ -3290,7 +3290,7 @@
         <v>43278</v>
       </c>
       <c r="B363">
-        <v>0.0027591</v>
+        <v>0.0098286</v>
       </c>
     </row>
     <row r="364" spans="1:2">
@@ -3298,7 +3298,7 @@
         <v>43279</v>
       </c>
       <c r="B364">
-        <v>0.0027591</v>
+        <v>0.0098286</v>
       </c>
     </row>
     <row r="365" spans="1:2">
@@ -3306,7 +3306,7 @@
         <v>43280</v>
       </c>
       <c r="B365">
-        <v>0.0027591</v>
+        <v>0.0098286</v>
       </c>
     </row>
     <row r="366" spans="1:2">
@@ -3314,7 +3314,7 @@
         <v>43281</v>
       </c>
       <c r="B366">
-        <v>0.0027591</v>
+        <v>0.0098286</v>
       </c>
     </row>
     <row r="367" spans="1:2">
@@ -3322,7 +3322,7 @@
         <v>43282</v>
       </c>
       <c r="B367">
-        <v>0.0027591</v>
+        <v>0.0098286</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Code Cleaning Round 2.
</commit_message>
<xml_diff>
--- a/DATA/collate_cultivar_data/data/Smoothed_kcp_trend_vs_datetime.xlsx
+++ b/DATA/collate_cultivar_data/data/Smoothed_kcp_trend_vs_datetime.xlsx
@@ -402,7 +402,7 @@
         <v>42917</v>
       </c>
       <c r="B2">
-        <v>0.09059</v>
+        <v>0.109133</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -410,7 +410,7 @@
         <v>42918</v>
       </c>
       <c r="B3">
-        <v>0.09059</v>
+        <v>0.1092034</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -418,7 +418,7 @@
         <v>42919</v>
       </c>
       <c r="B4">
-        <v>0.09059</v>
+        <v>0.1092763</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -426,7 +426,7 @@
         <v>42920</v>
       </c>
       <c r="B5">
-        <v>0.09059</v>
+        <v>0.1093516</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -434,7 +434,7 @@
         <v>42921</v>
       </c>
       <c r="B6">
-        <v>0.09059</v>
+        <v>0.1094293</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -442,7 +442,7 @@
         <v>42922</v>
       </c>
       <c r="B7">
-        <v>0.09059</v>
+        <v>0.1095091</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -450,7 +450,7 @@
         <v>42923</v>
       </c>
       <c r="B8">
-        <v>0.09059</v>
+        <v>0.109591</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -458,7 +458,7 @@
         <v>42924</v>
       </c>
       <c r="B9">
-        <v>0.09059</v>
+        <v>0.1096748</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -466,7 +466,7 @@
         <v>42925</v>
       </c>
       <c r="B10">
-        <v>0.09059</v>
+        <v>0.1097603</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -474,7 +474,7 @@
         <v>42926</v>
       </c>
       <c r="B11">
-        <v>0.09059</v>
+        <v>0.1098474</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -482,7 +482,7 @@
         <v>42927</v>
       </c>
       <c r="B12">
-        <v>0.09059</v>
+        <v>0.109936</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -490,7 +490,7 @@
         <v>42928</v>
       </c>
       <c r="B13">
-        <v>0.09059</v>
+        <v>0.1100257</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -498,7 +498,7 @@
         <v>42929</v>
       </c>
       <c r="B14">
-        <v>0.09059</v>
+        <v>0.1101164</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -506,7 +506,7 @@
         <v>42930</v>
       </c>
       <c r="B15">
-        <v>0.09059</v>
+        <v>0.1102078</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -514,7 +514,7 @@
         <v>42931</v>
       </c>
       <c r="B16">
-        <v>0.09059</v>
+        <v>0.1102998</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -522,7 +522,7 @@
         <v>42932</v>
       </c>
       <c r="B17">
-        <v>0.09059</v>
+        <v>0.1103921</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -530,7 +530,7 @@
         <v>42933</v>
       </c>
       <c r="B18">
-        <v>0.09059</v>
+        <v>0.1104843</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -538,7 +538,7 @@
         <v>42934</v>
       </c>
       <c r="B19">
-        <v>0.09059</v>
+        <v>0.1105764</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -546,7 +546,7 @@
         <v>42935</v>
       </c>
       <c r="B20">
-        <v>0.09059</v>
+        <v>0.1106678</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -554,7 +554,7 @@
         <v>42936</v>
       </c>
       <c r="B21">
-        <v>0.09059</v>
+        <v>0.1107585</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -562,7 +562,7 @@
         <v>42937</v>
       </c>
       <c r="B22">
-        <v>0.09059</v>
+        <v>0.110848</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -570,7 +570,7 @@
         <v>42938</v>
       </c>
       <c r="B23">
-        <v>0.09059</v>
+        <v>0.1109361</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -578,7 +578,7 @@
         <v>42939</v>
       </c>
       <c r="B24">
-        <v>0.09059</v>
+        <v>0.1110225</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -586,7 +586,7 @@
         <v>42940</v>
       </c>
       <c r="B25">
-        <v>0.09059</v>
+        <v>0.1111068</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -594,7 +594,7 @@
         <v>42941</v>
       </c>
       <c r="B26">
-        <v>0.09059</v>
+        <v>0.1111888</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -602,7 +602,7 @@
         <v>42942</v>
       </c>
       <c r="B27">
-        <v>0.09059</v>
+        <v>0.1112682</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -610,7 +610,7 @@
         <v>42943</v>
       </c>
       <c r="B28">
-        <v>0.09059</v>
+        <v>0.1113446</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -618,7 +618,7 @@
         <v>42944</v>
       </c>
       <c r="B29">
-        <v>0.09059</v>
+        <v>0.1114179</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -626,7 +626,7 @@
         <v>42945</v>
       </c>
       <c r="B30">
-        <v>0.09059</v>
+        <v>0.1114877</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -634,7 +634,7 @@
         <v>42946</v>
       </c>
       <c r="B31">
-        <v>0.09059</v>
+        <v>0.1115537</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -642,7 +642,7 @@
         <v>42947</v>
       </c>
       <c r="B32">
-        <v>0.09059</v>
+        <v>0.1116159</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -650,7 +650,7 @@
         <v>42948</v>
       </c>
       <c r="B33">
-        <v>0.09059</v>
+        <v>0.1116739</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -658,7 +658,7 @@
         <v>42949</v>
       </c>
       <c r="B34">
-        <v>0.09059</v>
+        <v>0.1117276</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -666,7 +666,7 @@
         <v>42950</v>
       </c>
       <c r="B35">
-        <v>0.09059</v>
+        <v>0.111777</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -674,7 +674,7 @@
         <v>42951</v>
       </c>
       <c r="B36">
-        <v>0.09059</v>
+        <v>0.1118218</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -682,7 +682,7 @@
         <v>42952</v>
       </c>
       <c r="B37">
-        <v>0.09059</v>
+        <v>0.1118621</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -690,7 +690,7 @@
         <v>42953</v>
       </c>
       <c r="B38">
-        <v>0.09059</v>
+        <v>0.1118979</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -698,7 +698,7 @@
         <v>42954</v>
       </c>
       <c r="B39">
-        <v>0.09059</v>
+        <v>0.1119293</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -706,7 +706,7 @@
         <v>42955</v>
       </c>
       <c r="B40">
-        <v>0.09059</v>
+        <v>0.1119563</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -714,7 +714,7 @@
         <v>42956</v>
       </c>
       <c r="B41">
-        <v>0.09059</v>
+        <v>0.1119792</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -722,7 +722,7 @@
         <v>42957</v>
       </c>
       <c r="B42">
-        <v>0.09059</v>
+        <v>0.1119982</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -730,7 +730,7 @@
         <v>42958</v>
       </c>
       <c r="B43">
-        <v>0.09059</v>
+        <v>0.1120137</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -738,7 +738,7 @@
         <v>42959</v>
       </c>
       <c r="B44">
-        <v>0.09059</v>
+        <v>0.112026</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -746,7 +746,7 @@
         <v>42960</v>
       </c>
       <c r="B45">
-        <v>0.09059</v>
+        <v>0.1120357</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -754,7 +754,7 @@
         <v>42961</v>
       </c>
       <c r="B46">
-        <v>0.09059</v>
+        <v>0.1120432</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -762,7 +762,7 @@
         <v>42962</v>
       </c>
       <c r="B47">
-        <v>0.09059</v>
+        <v>0.1120491</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -770,7 +770,7 @@
         <v>42963</v>
       </c>
       <c r="B48">
-        <v>0.09059</v>
+        <v>0.1120543</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -778,7 +778,7 @@
         <v>42964</v>
       </c>
       <c r="B49">
-        <v>0.09059</v>
+        <v>0.1120593</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -786,7 +786,7 @@
         <v>42965</v>
       </c>
       <c r="B50">
-        <v>0.09059</v>
+        <v>0.1120651</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -794,7 +794,7 @@
         <v>42966</v>
       </c>
       <c r="B51">
-        <v>0.09059</v>
+        <v>0.1120725</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -802,7 +802,7 @@
         <v>42967</v>
       </c>
       <c r="B52">
-        <v>0.09059</v>
+        <v>0.1120825</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -810,7 +810,7 @@
         <v>42968</v>
       </c>
       <c r="B53">
-        <v>0.09059</v>
+        <v>0.112096</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -818,7 +818,7 @@
         <v>42969</v>
       </c>
       <c r="B54">
-        <v>0.09059</v>
+        <v>0.1121141</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -826,7 +826,7 @@
         <v>42970</v>
       </c>
       <c r="B55">
-        <v>0.09059</v>
+        <v>0.1121379</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -834,7 +834,7 @@
         <v>42971</v>
       </c>
       <c r="B56">
-        <v>0.09059</v>
+        <v>0.1121686</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -842,7 +842,7 @@
         <v>42972</v>
       </c>
       <c r="B57">
-        <v>0.09059</v>
+        <v>0.1122072</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -850,7 +850,7 @@
         <v>42973</v>
       </c>
       <c r="B58">
-        <v>0.09059</v>
+        <v>0.112255</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -858,7 +858,7 @@
         <v>42974</v>
       </c>
       <c r="B59">
-        <v>0.09064270000000001</v>
+        <v>0.1123132</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -866,7 +866,7 @@
         <v>42975</v>
       </c>
       <c r="B60">
-        <v>0.0907843</v>
+        <v>0.1123829</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -874,7 +874,7 @@
         <v>42976</v>
       </c>
       <c r="B61">
-        <v>0.09101339999999999</v>
+        <v>0.1124655</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -882,7 +882,7 @@
         <v>42977</v>
       </c>
       <c r="B62">
-        <v>0.0913288</v>
+        <v>0.112562</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -890,7 +890,7 @@
         <v>42978</v>
       </c>
       <c r="B63">
-        <v>0.0917293</v>
+        <v>0.1126738</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -898,7 +898,7 @@
         <v>42979</v>
       </c>
       <c r="B64">
-        <v>0.0922137</v>
+        <v>0.112802</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -906,7 +906,7 @@
         <v>42980</v>
       </c>
       <c r="B65">
-        <v>0.0927809</v>
+        <v>0.1129479</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -914,7 +914,7 @@
         <v>42981</v>
       </c>
       <c r="B66">
-        <v>0.0934295</v>
+        <v>0.1131126</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -922,7 +922,7 @@
         <v>42982</v>
       </c>
       <c r="B67">
-        <v>0.0941583</v>
+        <v>0.1132973</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -930,7 +930,7 @@
         <v>42983</v>
       </c>
       <c r="B68">
-        <v>0.0949663</v>
+        <v>0.1135032</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -938,7 +938,7 @@
         <v>42984</v>
       </c>
       <c r="B69">
-        <v>0.0958521</v>
+        <v>0.1137314</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -946,7 +946,7 @@
         <v>42985</v>
       </c>
       <c r="B70">
-        <v>0.0968146</v>
+        <v>0.113983</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -954,7 +954,7 @@
         <v>42986</v>
       </c>
       <c r="B71">
-        <v>0.0978526</v>
+        <v>0.1142592</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -962,7 +962,7 @@
         <v>42987</v>
       </c>
       <c r="B72">
-        <v>0.09896480000000001</v>
+        <v>0.1145611</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -970,7 +970,7 @@
         <v>42988</v>
       </c>
       <c r="B73">
-        <v>0.1001502</v>
+        <v>0.1148897</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -978,7 +978,7 @@
         <v>42989</v>
       </c>
       <c r="B74">
-        <v>0.1014074</v>
+        <v>0.1152462</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -986,7 +986,7 @@
         <v>42990</v>
       </c>
       <c r="B75">
-        <v>0.1027354</v>
+        <v>0.1156316</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -994,7 +994,7 @@
         <v>42991</v>
       </c>
       <c r="B76">
-        <v>0.1041329</v>
+        <v>0.1160471</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -1002,7 +1002,7 @@
         <v>42992</v>
       </c>
       <c r="B77">
-        <v>0.1055988</v>
+        <v>0.1164938</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -1010,7 +1010,7 @@
         <v>42993</v>
       </c>
       <c r="B78">
-        <v>0.1071319</v>
+        <v>0.1169728</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -1018,7 +1018,7 @@
         <v>42994</v>
       </c>
       <c r="B79">
-        <v>0.108731</v>
+        <v>0.1174853</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -1026,7 +1026,7 @@
         <v>42995</v>
       </c>
       <c r="B80">
-        <v>0.110395</v>
+        <v>0.1180323</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -1034,7 +1034,7 @@
         <v>42996</v>
       </c>
       <c r="B81">
-        <v>0.1121226</v>
+        <v>0.1186152</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -1042,7 +1042,7 @@
         <v>42997</v>
       </c>
       <c r="B82">
-        <v>0.1139127</v>
+        <v>0.1192351</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -1050,7 +1050,7 @@
         <v>42998</v>
       </c>
       <c r="B83">
-        <v>0.1157642</v>
+        <v>0.1198933</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -1058,7 +1058,7 @@
         <v>42999</v>
       </c>
       <c r="B84">
-        <v>0.1176758</v>
+        <v>0.1205912</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -1066,7 +1066,7 @@
         <v>43000</v>
       </c>
       <c r="B85">
-        <v>0.1196465</v>
+        <v>0.1213301</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -1074,7 +1074,7 @@
         <v>43001</v>
       </c>
       <c r="B86">
-        <v>0.1216751</v>
+        <v>0.1221114</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -1082,7 +1082,7 @@
         <v>43002</v>
       </c>
       <c r="B87">
-        <v>0.1237604</v>
+        <v>0.1229367</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -1090,7 +1090,7 @@
         <v>43003</v>
       </c>
       <c r="B88">
-        <v>0.1259013</v>
+        <v>0.1238074</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -1098,7 +1098,7 @@
         <v>43004</v>
       </c>
       <c r="B89">
-        <v>0.1280966</v>
+        <v>0.1247252</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -1106,7 +1106,7 @@
         <v>43005</v>
       </c>
       <c r="B90">
-        <v>0.1303452</v>
+        <v>0.1256917</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -1114,7 +1114,7 @@
         <v>43006</v>
       </c>
       <c r="B91">
-        <v>0.132646</v>
+        <v>0.1267088</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -1122,7 +1122,7 @@
         <v>43007</v>
       </c>
       <c r="B92">
-        <v>0.1349978</v>
+        <v>0.1277783</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -1130,7 +1130,7 @@
         <v>43008</v>
       </c>
       <c r="B93">
-        <v>0.1373994</v>
+        <v>0.1289021</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -1138,7 +1138,7 @@
         <v>43009</v>
       </c>
       <c r="B94">
-        <v>0.1398498</v>
+        <v>0.1300823</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -1146,7 +1146,7 @@
         <v>43010</v>
       </c>
       <c r="B95">
-        <v>0.1423478</v>
+        <v>0.1313208</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -1154,7 +1154,7 @@
         <v>43011</v>
       </c>
       <c r="B96">
-        <v>0.1448923</v>
+        <v>0.1326198</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -1162,7 +1162,7 @@
         <v>43012</v>
       </c>
       <c r="B97">
-        <v>0.1474821</v>
+        <v>0.1339817</v>
       </c>
     </row>
     <row r="98" spans="1:2">
@@ -1170,7 +1170,7 @@
         <v>43013</v>
       </c>
       <c r="B98">
-        <v>0.1501162</v>
+        <v>0.1354088</v>
       </c>
     </row>
     <row r="99" spans="1:2">
@@ -1178,7 +1178,7 @@
         <v>43014</v>
       </c>
       <c r="B99">
-        <v>0.1527934</v>
+        <v>0.1369034</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -1186,7 +1186,7 @@
         <v>43015</v>
       </c>
       <c r="B100">
-        <v>0.1555127</v>
+        <v>0.138468</v>
       </c>
     </row>
     <row r="101" spans="1:2">
@@ -1194,7 +1194,7 @@
         <v>43016</v>
       </c>
       <c r="B101">
-        <v>0.1582728</v>
+        <v>0.1401052</v>
       </c>
     </row>
     <row r="102" spans="1:2">
@@ -1202,7 +1202,7 @@
         <v>43017</v>
       </c>
       <c r="B102">
-        <v>0.1610727</v>
+        <v>0.1418176</v>
       </c>
     </row>
     <row r="103" spans="1:2">
@@ -1210,7 +1210,7 @@
         <v>43018</v>
       </c>
       <c r="B103">
-        <v>0.1639113</v>
+        <v>0.1436079</v>
       </c>
     </row>
     <row r="104" spans="1:2">
@@ -1218,7 +1218,7 @@
         <v>43019</v>
       </c>
       <c r="B104">
-        <v>0.1667874</v>
+        <v>0.1454788</v>
       </c>
     </row>
     <row r="105" spans="1:2">
@@ -1226,7 +1226,7 @@
         <v>43020</v>
       </c>
       <c r="B105">
-        <v>0.1697</v>
+        <v>0.1474331</v>
       </c>
     </row>
     <row r="106" spans="1:2">
@@ -1234,7 +1234,7 @@
         <v>43021</v>
       </c>
       <c r="B106">
-        <v>0.172648</v>
+        <v>0.1494735</v>
       </c>
     </row>
     <row r="107" spans="1:2">
@@ -1242,7 +1242,7 @@
         <v>43022</v>
       </c>
       <c r="B107">
-        <v>0.1756303</v>
+        <v>0.1516029</v>
       </c>
     </row>
     <row r="108" spans="1:2">
@@ -1250,7 +1250,7 @@
         <v>43023</v>
       </c>
       <c r="B108">
-        <v>0.1786457</v>
+        <v>0.1538239</v>
       </c>
     </row>
     <row r="109" spans="1:2">
@@ -1258,7 +1258,7 @@
         <v>43024</v>
       </c>
       <c r="B109">
-        <v>0.1816932</v>
+        <v>0.1561395</v>
       </c>
     </row>
     <row r="110" spans="1:2">
@@ -1266,7 +1266,7 @@
         <v>43025</v>
       </c>
       <c r="B110">
-        <v>0.1847718</v>
+        <v>0.1585524</v>
       </c>
     </row>
     <row r="111" spans="1:2">
@@ -1274,7 +1274,7 @@
         <v>43026</v>
       </c>
       <c r="B111">
-        <v>0.1878802</v>
+        <v>0.1610651</v>
       </c>
     </row>
     <row r="112" spans="1:2">
@@ -1282,7 +1282,7 @@
         <v>43027</v>
       </c>
       <c r="B112">
-        <v>0.1910175</v>
+        <v>0.1636804</v>
       </c>
     </row>
     <row r="113" spans="1:2">
@@ -1290,7 +1290,7 @@
         <v>43028</v>
       </c>
       <c r="B113">
-        <v>0.1941825</v>
+        <v>0.1664006</v>
       </c>
     </row>
     <row r="114" spans="1:2">
@@ -1298,7 +1298,7 @@
         <v>43029</v>
       </c>
       <c r="B114">
-        <v>0.1973742</v>
+        <v>0.1692282</v>
       </c>
     </row>
     <row r="115" spans="1:2">
@@ -1306,7 +1306,7 @@
         <v>43030</v>
       </c>
       <c r="B115">
-        <v>0.2005915</v>
+        <v>0.1721653</v>
       </c>
     </row>
     <row r="116" spans="1:2">
@@ -1314,7 +1314,7 @@
         <v>43031</v>
       </c>
       <c r="B116">
-        <v>0.2038333</v>
+        <v>0.1752138</v>
       </c>
     </row>
     <row r="117" spans="1:2">
@@ -1322,7 +1322,7 @@
         <v>43032</v>
       </c>
       <c r="B117">
-        <v>0.2070985</v>
+        <v>0.1783756</v>
       </c>
     </row>
     <row r="118" spans="1:2">
@@ -1330,7 +1330,7 @@
         <v>43033</v>
       </c>
       <c r="B118">
-        <v>0.2103862</v>
+        <v>0.1816521</v>
       </c>
     </row>
     <row r="119" spans="1:2">
@@ -1338,7 +1338,7 @@
         <v>43034</v>
       </c>
       <c r="B119">
-        <v>0.2136952</v>
+        <v>0.1850446</v>
       </c>
     </row>
     <row r="120" spans="1:2">
@@ -1346,7 +1346,7 @@
         <v>43035</v>
       </c>
       <c r="B120">
-        <v>0.2170244</v>
+        <v>0.1885539</v>
       </c>
     </row>
     <row r="121" spans="1:2">
@@ -1354,7 +1354,7 @@
         <v>43036</v>
       </c>
       <c r="B121">
-        <v>0.2203729</v>
+        <v>0.1921804</v>
       </c>
     </row>
     <row r="122" spans="1:2">
@@ -1362,7 +1362,7 @@
         <v>43037</v>
       </c>
       <c r="B122">
-        <v>0.2237395</v>
+        <v>0.1959244</v>
       </c>
     </row>
     <row r="123" spans="1:2">
@@ -1370,7 +1370,7 @@
         <v>43038</v>
       </c>
       <c r="B123">
-        <v>0.2271231</v>
+        <v>0.1997855</v>
       </c>
     </row>
     <row r="124" spans="1:2">
@@ -1378,7 +1378,7 @@
         <v>43039</v>
       </c>
       <c r="B124">
-        <v>0.2305229</v>
+        <v>0.2037628</v>
       </c>
     </row>
     <row r="125" spans="1:2">
@@ -1386,7 +1386,7 @@
         <v>43040</v>
       </c>
       <c r="B125">
-        <v>0.2339376</v>
+        <v>0.2078551</v>
       </c>
     </row>
     <row r="126" spans="1:2">
@@ -1394,7 +1394,7 @@
         <v>43041</v>
       </c>
       <c r="B126">
-        <v>0.2373663</v>
+        <v>0.2120607</v>
       </c>
     </row>
     <row r="127" spans="1:2">
@@ -1402,7 +1402,7 @@
         <v>43042</v>
       </c>
       <c r="B127">
-        <v>0.2408079</v>
+        <v>0.216377</v>
       </c>
     </row>
     <row r="128" spans="1:2">
@@ -1410,7 +1410,7 @@
         <v>43043</v>
       </c>
       <c r="B128">
-        <v>0.2442613</v>
+        <v>0.2208012</v>
       </c>
     </row>
     <row r="129" spans="1:2">
@@ -1418,7 +1418,7 @@
         <v>43044</v>
       </c>
       <c r="B129">
-        <v>0.2477256</v>
+        <v>0.2253299</v>
       </c>
     </row>
     <row r="130" spans="1:2">
@@ -1426,7 +1426,7 @@
         <v>43045</v>
       </c>
       <c r="B130">
-        <v>0.2511997</v>
+        <v>0.2299588</v>
       </c>
     </row>
     <row r="131" spans="1:2">
@@ -1434,7 +1434,7 @@
         <v>43046</v>
       </c>
       <c r="B131">
-        <v>0.2546826</v>
+        <v>0.2346832</v>
       </c>
     </row>
     <row r="132" spans="1:2">
@@ -1442,7 +1442,7 @@
         <v>43047</v>
       </c>
       <c r="B132">
-        <v>0.2581732</v>
+        <v>0.239498</v>
       </c>
     </row>
     <row r="133" spans="1:2">
@@ -1450,7 +1450,7 @@
         <v>43048</v>
       </c>
       <c r="B133">
-        <v>0.2616706</v>
+        <v>0.2443972</v>
       </c>
     </row>
     <row r="134" spans="1:2">
@@ -1458,7 +1458,7 @@
         <v>43049</v>
       </c>
       <c r="B134">
-        <v>0.2651736</v>
+        <v>0.2493743</v>
       </c>
     </row>
     <row r="135" spans="1:2">
@@ -1466,7 +1466,7 @@
         <v>43050</v>
       </c>
       <c r="B135">
-        <v>0.2686813</v>
+        <v>0.2544223</v>
       </c>
     </row>
     <row r="136" spans="1:2">
@@ -1474,7 +1474,7 @@
         <v>43051</v>
       </c>
       <c r="B136">
-        <v>0.2721926</v>
+        <v>0.2595338</v>
       </c>
     </row>
     <row r="137" spans="1:2">
@@ -1482,7 +1482,7 @@
         <v>43052</v>
       </c>
       <c r="B137">
-        <v>0.2757066</v>
+        <v>0.2647007</v>
       </c>
     </row>
     <row r="138" spans="1:2">
@@ -1490,7 +1490,7 @@
         <v>43053</v>
       </c>
       <c r="B138">
-        <v>0.2792222</v>
+        <v>0.2699146</v>
       </c>
     </row>
     <row r="139" spans="1:2">
@@ -1498,7 +1498,7 @@
         <v>43054</v>
       </c>
       <c r="B139">
-        <v>0.2827384</v>
+        <v>0.2751667</v>
       </c>
     </row>
     <row r="140" spans="1:2">
@@ -1506,7 +1506,7 @@
         <v>43055</v>
       </c>
       <c r="B140">
-        <v>0.2862542</v>
+        <v>0.2804478</v>
       </c>
     </row>
     <row r="141" spans="1:2">
@@ -1514,7 +1514,7 @@
         <v>43056</v>
       </c>
       <c r="B141">
-        <v>0.2897687</v>
+        <v>0.2857486</v>
       </c>
     </row>
     <row r="142" spans="1:2">
@@ -1522,7 +1522,7 @@
         <v>43057</v>
       </c>
       <c r="B142">
-        <v>0.2932807</v>
+        <v>0.2910593</v>
       </c>
     </row>
     <row r="143" spans="1:2">
@@ -1530,7 +1530,7 @@
         <v>43058</v>
       </c>
       <c r="B143">
-        <v>0.2967894</v>
+        <v>0.2963704</v>
       </c>
     </row>
     <row r="144" spans="1:2">
@@ -1538,7 +1538,7 @@
         <v>43059</v>
       </c>
       <c r="B144">
-        <v>0.3002937</v>
+        <v>0.3016719</v>
       </c>
     </row>
     <row r="145" spans="1:2">
@@ -1546,7 +1546,7 @@
         <v>43060</v>
       </c>
       <c r="B145">
-        <v>0.3037925</v>
+        <v>0.3069541</v>
       </c>
     </row>
     <row r="146" spans="1:2">
@@ -1554,7 +1554,7 @@
         <v>43061</v>
       </c>
       <c r="B146">
-        <v>0.3072851</v>
+        <v>0.3122073</v>
       </c>
     </row>
     <row r="147" spans="1:2">
@@ -1562,7 +1562,7 @@
         <v>43062</v>
       </c>
       <c r="B147">
-        <v>0.3107702</v>
+        <v>0.3174219</v>
       </c>
     </row>
     <row r="148" spans="1:2">
@@ -1570,7 +1570,7 @@
         <v>43063</v>
       </c>
       <c r="B148">
-        <v>0.314247</v>
+        <v>0.3225886</v>
       </c>
     </row>
     <row r="149" spans="1:2">
@@ -1578,7 +1578,7 @@
         <v>43064</v>
       </c>
       <c r="B149">
-        <v>0.3177145</v>
+        <v>0.3276984</v>
       </c>
     </row>
     <row r="150" spans="1:2">
@@ -1586,7 +1586,7 @@
         <v>43065</v>
       </c>
       <c r="B150">
-        <v>0.3211717</v>
+        <v>0.3327426</v>
       </c>
     </row>
     <row r="151" spans="1:2">
@@ -1594,7 +1594,7 @@
         <v>43066</v>
       </c>
       <c r="B151">
-        <v>0.3246176</v>
+        <v>0.337713</v>
       </c>
     </row>
     <row r="152" spans="1:2">
@@ -1602,7 +1602,7 @@
         <v>43067</v>
       </c>
       <c r="B152">
-        <v>0.3280512</v>
+        <v>0.3426017</v>
       </c>
     </row>
     <row r="153" spans="1:2">
@@ -1610,7 +1610,7 @@
         <v>43068</v>
       </c>
       <c r="B153">
-        <v>0.3314716</v>
+        <v>0.3474014</v>
       </c>
     </row>
     <row r="154" spans="1:2">
@@ -1618,7 +1618,7 @@
         <v>43069</v>
       </c>
       <c r="B154">
-        <v>0.3348779</v>
+        <v>0.3521054</v>
       </c>
     </row>
     <row r="155" spans="1:2">
@@ -1626,7 +1626,7 @@
         <v>43070</v>
       </c>
       <c r="B155">
-        <v>0.3382689</v>
+        <v>0.3567075</v>
       </c>
     </row>
     <row r="156" spans="1:2">
@@ -1634,7 +1634,7 @@
         <v>43071</v>
       </c>
       <c r="B156">
-        <v>0.3416439</v>
+        <v>0.3612021</v>
       </c>
     </row>
     <row r="157" spans="1:2">
@@ -1642,7 +1642,7 @@
         <v>43072</v>
       </c>
       <c r="B157">
-        <v>0.3450017</v>
+        <v>0.3655842</v>
       </c>
     </row>
     <row r="158" spans="1:2">
@@ -1650,7 +1650,7 @@
         <v>43073</v>
       </c>
       <c r="B158">
-        <v>0.3483415</v>
+        <v>0.3698496</v>
       </c>
     </row>
     <row r="159" spans="1:2">
@@ -1658,7 +1658,7 @@
         <v>43074</v>
       </c>
       <c r="B159">
-        <v>0.3516623</v>
+        <v>0.3739944</v>
       </c>
     </row>
     <row r="160" spans="1:2">
@@ -1666,7 +1666,7 @@
         <v>43075</v>
       </c>
       <c r="B160">
-        <v>0.3549632</v>
+        <v>0.3780156</v>
       </c>
     </row>
     <row r="161" spans="1:2">
@@ -1674,7 +1674,7 @@
         <v>43076</v>
       </c>
       <c r="B161">
-        <v>0.3582431</v>
+        <v>0.3819107</v>
       </c>
     </row>
     <row r="162" spans="1:2">
@@ -1682,7 +1682,7 @@
         <v>43077</v>
       </c>
       <c r="B162">
-        <v>0.3615013</v>
+        <v>0.3856778</v>
       </c>
     </row>
     <row r="163" spans="1:2">
@@ -1690,7 +1690,7 @@
         <v>43078</v>
       </c>
       <c r="B163">
-        <v>0.3647366</v>
+        <v>0.3893156</v>
       </c>
     </row>
     <row r="164" spans="1:2">
@@ -1698,7 +1698,7 @@
         <v>43079</v>
       </c>
       <c r="B164">
-        <v>0.3679482</v>
+        <v>0.3928234</v>
       </c>
     </row>
     <row r="165" spans="1:2">
@@ -1706,7 +1706,7 @@
         <v>43080</v>
       </c>
       <c r="B165">
-        <v>0.3711351</v>
+        <v>0.3962009</v>
       </c>
     </row>
     <row r="166" spans="1:2">
@@ -1714,7 +1714,7 @@
         <v>43081</v>
       </c>
       <c r="B166">
-        <v>0.3742965</v>
+        <v>0.3994484</v>
       </c>
     </row>
     <row r="167" spans="1:2">
@@ -1722,7 +1722,7 @@
         <v>43082</v>
       </c>
       <c r="B167">
-        <v>0.3774313</v>
+        <v>0.4025667</v>
       </c>
     </row>
     <row r="168" spans="1:2">
@@ -1730,7 +1730,7 @@
         <v>43083</v>
       </c>
       <c r="B168">
-        <v>0.3805386</v>
+        <v>0.4055569</v>
       </c>
     </row>
     <row r="169" spans="1:2">
@@ -1738,7 +1738,7 @@
         <v>43084</v>
       </c>
       <c r="B169">
-        <v>0.3836175</v>
+        <v>0.4084205</v>
       </c>
     </row>
     <row r="170" spans="1:2">
@@ -1746,7 +1746,7 @@
         <v>43085</v>
       </c>
       <c r="B170">
-        <v>0.3866671</v>
+        <v>0.4111594</v>
       </c>
     </row>
     <row r="171" spans="1:2">
@@ -1754,7 +1754,7 @@
         <v>43086</v>
       </c>
       <c r="B171">
-        <v>0.3896865</v>
+        <v>0.413776</v>
       </c>
     </row>
     <row r="172" spans="1:2">
@@ -1762,7 +1762,7 @@
         <v>43087</v>
       </c>
       <c r="B172">
-        <v>0.3926747</v>
+        <v>0.4162727</v>
       </c>
     </row>
     <row r="173" spans="1:2">
@@ -1770,7 +1770,7 @@
         <v>43088</v>
       </c>
       <c r="B173">
-        <v>0.3956309</v>
+        <v>0.4186523</v>
       </c>
     </row>
     <row r="174" spans="1:2">
@@ -1778,7 +1778,7 @@
         <v>43089</v>
       </c>
       <c r="B174">
-        <v>0.398554</v>
+        <v>0.4209177</v>
       </c>
     </row>
     <row r="175" spans="1:2">
@@ -1786,7 +1786,7 @@
         <v>43090</v>
       </c>
       <c r="B175">
-        <v>0.4014433</v>
+        <v>0.4230721</v>
       </c>
     </row>
     <row r="176" spans="1:2">
@@ -1794,7 +1794,7 @@
         <v>43091</v>
       </c>
       <c r="B176">
-        <v>0.4042977</v>
+        <v>0.4251188</v>
       </c>
     </row>
     <row r="177" spans="1:2">
@@ -1802,7 +1802,7 @@
         <v>43092</v>
       </c>
       <c r="B177">
-        <v>0.4071164</v>
+        <v>0.4270613</v>
       </c>
     </row>
     <row r="178" spans="1:2">
@@ -1810,7 +1810,7 @@
         <v>43093</v>
       </c>
       <c r="B178">
-        <v>0.4098985</v>
+        <v>0.428903</v>
       </c>
     </row>
     <row r="179" spans="1:2">
@@ -1818,7 +1818,7 @@
         <v>43094</v>
       </c>
       <c r="B179">
-        <v>0.4126431</v>
+        <v>0.4306476</v>
       </c>
     </row>
     <row r="180" spans="1:2">
@@ -1826,7 +1826,7 @@
         <v>43095</v>
       </c>
       <c r="B180">
-        <v>0.4153493</v>
+        <v>0.4322987</v>
       </c>
     </row>
     <row r="181" spans="1:2">
@@ -1834,7 +1834,7 @@
         <v>43096</v>
       </c>
       <c r="B181">
-        <v>0.4180161</v>
+        <v>0.43386</v>
       </c>
     </row>
     <row r="182" spans="1:2">
@@ -1842,7 +1842,7 @@
         <v>43097</v>
       </c>
       <c r="B182">
-        <v>0.4206428</v>
+        <v>0.435335</v>
       </c>
     </row>
     <row r="183" spans="1:2">
@@ -1850,7 +1850,7 @@
         <v>43098</v>
       </c>
       <c r="B183">
-        <v>0.4232283</v>
+        <v>0.4367276</v>
       </c>
     </row>
     <row r="184" spans="1:2">
@@ -1858,7 +1858,7 @@
         <v>43099</v>
       </c>
       <c r="B184">
-        <v>0.4257719</v>
+        <v>0.4380412</v>
       </c>
     </row>
     <row r="185" spans="1:2">
@@ -1866,7 +1866,7 @@
         <v>43100</v>
       </c>
       <c r="B185">
-        <v>0.4282726</v>
+        <v>0.4392796</v>
       </c>
     </row>
     <row r="186" spans="1:2">
@@ -1874,7 +1874,7 @@
         <v>43101</v>
       </c>
       <c r="B186">
-        <v>0.4307296</v>
+        <v>0.4404461</v>
       </c>
     </row>
     <row r="187" spans="1:2">
@@ -1882,7 +1882,7 @@
         <v>43102</v>
       </c>
       <c r="B187">
-        <v>0.433142</v>
+        <v>0.4415444</v>
       </c>
     </row>
     <row r="188" spans="1:2">
@@ -1890,7 +1890,7 @@
         <v>43103</v>
       </c>
       <c r="B188">
-        <v>0.4355089</v>
+        <v>0.4425778</v>
       </c>
     </row>
     <row r="189" spans="1:2">
@@ -1898,7 +1898,7 @@
         <v>43104</v>
       </c>
       <c r="B189">
-        <v>0.4378293</v>
+        <v>0.4435496</v>
       </c>
     </row>
     <row r="190" spans="1:2">
@@ -1906,7 +1906,7 @@
         <v>43105</v>
       </c>
       <c r="B190">
-        <v>0.4401026</v>
+        <v>0.4444632</v>
       </c>
     </row>
     <row r="191" spans="1:2">
@@ -1914,7 +1914,7 @@
         <v>43106</v>
       </c>
       <c r="B191">
-        <v>0.4423277</v>
+        <v>0.4453215</v>
       </c>
     </row>
     <row r="192" spans="1:2">
@@ -1922,7 +1922,7 @@
         <v>43107</v>
       </c>
       <c r="B192">
-        <v>0.4445039</v>
+        <v>0.4461278</v>
       </c>
     </row>
     <row r="193" spans="1:2">
@@ -1930,7 +1930,7 @@
         <v>43108</v>
       </c>
       <c r="B193">
-        <v>0.4466303</v>
+        <v>0.4468849</v>
       </c>
     </row>
     <row r="194" spans="1:2">
@@ -1938,7 +1938,7 @@
         <v>43109</v>
       </c>
       <c r="B194">
-        <v>0.4487059</v>
+        <v>0.4475958</v>
       </c>
     </row>
     <row r="195" spans="1:2">
@@ -1946,7 +1946,7 @@
         <v>43110</v>
       </c>
       <c r="B195">
-        <v>0.45073</v>
+        <v>0.4482632</v>
       </c>
     </row>
     <row r="196" spans="1:2">
@@ -1954,7 +1954,7 @@
         <v>43111</v>
       </c>
       <c r="B196">
-        <v>0.4527017</v>
+        <v>0.4488898</v>
       </c>
     </row>
     <row r="197" spans="1:2">
@@ -1962,7 +1962,7 @@
         <v>43112</v>
       </c>
       <c r="B197">
-        <v>0.4546202</v>
+        <v>0.4494782</v>
       </c>
     </row>
     <row r="198" spans="1:2">
@@ -1970,7 +1970,7 @@
         <v>43113</v>
       </c>
       <c r="B198">
-        <v>0.4564845</v>
+        <v>0.4500308</v>
       </c>
     </row>
     <row r="199" spans="1:2">
@@ -1978,7 +1978,7 @@
         <v>43114</v>
       </c>
       <c r="B199">
-        <v>0.4582939</v>
+        <v>0.4505501</v>
       </c>
     </row>
     <row r="200" spans="1:2">
@@ -1986,7 +1986,7 @@
         <v>43115</v>
       </c>
       <c r="B200">
-        <v>0.4600475</v>
+        <v>0.4510382</v>
       </c>
     </row>
     <row r="201" spans="1:2">
@@ -1994,7 +1994,7 @@
         <v>43116</v>
       </c>
       <c r="B201">
-        <v>0.4617445</v>
+        <v>0.4514973</v>
       </c>
     </row>
     <row r="202" spans="1:2">
@@ -2002,7 +2002,7 @@
         <v>43117</v>
       </c>
       <c r="B202">
-        <v>0.463384</v>
+        <v>0.4519295</v>
       </c>
     </row>
     <row r="203" spans="1:2">
@@ -2010,7 +2010,7 @@
         <v>43118</v>
       </c>
       <c r="B203">
-        <v>0.4649652</v>
+        <v>0.4523368</v>
       </c>
     </row>
     <row r="204" spans="1:2">
@@ -2018,7 +2018,7 @@
         <v>43119</v>
       </c>
       <c r="B204">
-        <v>0.4664873</v>
+        <v>0.4527209</v>
       </c>
     </row>
     <row r="205" spans="1:2">
@@ -2026,7 +2026,7 @@
         <v>43120</v>
       </c>
       <c r="B205">
-        <v>0.4679494</v>
+        <v>0.4530837</v>
       </c>
     </row>
     <row r="206" spans="1:2">
@@ -2034,7 +2034,7 @@
         <v>43121</v>
       </c>
       <c r="B206">
-        <v>0.4693507</v>
+        <v>0.4534267</v>
       </c>
     </row>
     <row r="207" spans="1:2">
@@ -2042,7 +2042,7 @@
         <v>43122</v>
       </c>
       <c r="B207">
-        <v>0.4706904</v>
+        <v>0.4537514</v>
       </c>
     </row>
     <row r="208" spans="1:2">
@@ -2050,7 +2050,7 @@
         <v>43123</v>
       </c>
       <c r="B208">
-        <v>0.4719677</v>
+        <v>0.4540594</v>
       </c>
     </row>
     <row r="209" spans="1:2">
@@ -2058,7 +2058,7 @@
         <v>43124</v>
       </c>
       <c r="B209">
-        <v>0.4731817</v>
+        <v>0.4543518</v>
       </c>
     </row>
     <row r="210" spans="1:2">
@@ -2066,7 +2066,7 @@
         <v>43125</v>
       </c>
       <c r="B210">
-        <v>0.4743316</v>
+        <v>0.4546299</v>
       </c>
     </row>
     <row r="211" spans="1:2">
@@ -2074,7 +2074,7 @@
         <v>43126</v>
       </c>
       <c r="B211">
-        <v>0.4754167</v>
+        <v>0.4548948</v>
       </c>
     </row>
     <row r="212" spans="1:2">
@@ -2082,7 +2082,7 @@
         <v>43127</v>
       </c>
       <c r="B212">
-        <v>0.4764361</v>
+        <v>0.4551474</v>
       </c>
     </row>
     <row r="213" spans="1:2">
@@ -2090,7 +2090,7 @@
         <v>43128</v>
       </c>
       <c r="B213">
-        <v>0.477389</v>
+        <v>0.4553886</v>
       </c>
     </row>
     <row r="214" spans="1:2">
@@ -2098,7 +2098,7 @@
         <v>43129</v>
       </c>
       <c r="B214">
-        <v>0.4782745</v>
+        <v>0.4556191</v>
       </c>
     </row>
     <row r="215" spans="1:2">
@@ -2106,7 +2106,7 @@
         <v>43130</v>
       </c>
       <c r="B215">
-        <v>0.479092</v>
+        <v>0.4558395</v>
       </c>
     </row>
     <row r="216" spans="1:2">
@@ -2114,7 +2114,7 @@
         <v>43131</v>
       </c>
       <c r="B216">
-        <v>0.4798406</v>
+        <v>0.4560503</v>
       </c>
     </row>
     <row r="217" spans="1:2">
@@ -2122,7 +2122,7 @@
         <v>43132</v>
       </c>
       <c r="B217">
-        <v>0.4805195</v>
+        <v>0.4562519</v>
       </c>
     </row>
     <row r="218" spans="1:2">
@@ -2130,7 +2130,7 @@
         <v>43133</v>
       </c>
       <c r="B218">
-        <v>0.4811278</v>
+        <v>0.4564445</v>
       </c>
     </row>
     <row r="219" spans="1:2">
@@ -2138,7 +2138,7 @@
         <v>43134</v>
       </c>
       <c r="B219">
-        <v>0.4816649</v>
+        <v>0.4566282</v>
       </c>
     </row>
     <row r="220" spans="1:2">
@@ -2146,7 +2146,7 @@
         <v>43135</v>
       </c>
       <c r="B220">
-        <v>0.48213</v>
+        <v>0.4568031</v>
       </c>
     </row>
     <row r="221" spans="1:2">
@@ -2154,7 +2154,7 @@
         <v>43136</v>
       </c>
       <c r="B221">
-        <v>0.4825221</v>
+        <v>0.456969</v>
       </c>
     </row>
     <row r="222" spans="1:2">
@@ -2162,7 +2162,7 @@
         <v>43137</v>
       </c>
       <c r="B222">
-        <v>0.4828406</v>
+        <v>0.4571256</v>
       </c>
     </row>
     <row r="223" spans="1:2">
@@ -2170,7 +2170,7 @@
         <v>43138</v>
       </c>
       <c r="B223">
-        <v>0.4830847</v>
+        <v>0.4572725</v>
       </c>
     </row>
     <row r="224" spans="1:2">
@@ -2178,7 +2178,7 @@
         <v>43139</v>
       </c>
       <c r="B224">
-        <v>0.4832537</v>
+        <v>0.4574093</v>
       </c>
     </row>
     <row r="225" spans="1:2">
@@ -2186,7 +2186,7 @@
         <v>43140</v>
       </c>
       <c r="B225">
-        <v>0.4833466</v>
+        <v>0.4575354</v>
       </c>
     </row>
     <row r="226" spans="1:2">
@@ -2194,7 +2194,7 @@
         <v>43141</v>
       </c>
       <c r="B226">
-        <v>0.4833628</v>
+        <v>0.4576498</v>
       </c>
     </row>
     <row r="227" spans="1:2">
@@ -2202,7 +2202,7 @@
         <v>43142</v>
       </c>
       <c r="B227">
-        <v>0.4833015</v>
+        <v>0.4577518</v>
       </c>
     </row>
     <row r="228" spans="1:2">
@@ -2210,7 +2210,7 @@
         <v>43143</v>
       </c>
       <c r="B228">
-        <v>0.4831619</v>
+        <v>0.4578403</v>
       </c>
     </row>
     <row r="229" spans="1:2">
@@ -2218,7 +2218,7 @@
         <v>43144</v>
       </c>
       <c r="B229">
-        <v>0.4829432</v>
+        <v>0.4579143</v>
       </c>
     </row>
     <row r="230" spans="1:2">
@@ -2226,7 +2226,7 @@
         <v>43145</v>
       </c>
       <c r="B230">
-        <v>0.4826448</v>
+        <v>0.4579724</v>
       </c>
     </row>
     <row r="231" spans="1:2">
@@ -2234,7 +2234,7 @@
         <v>43146</v>
       </c>
       <c r="B231">
-        <v>0.4822657</v>
+        <v>0.4580133</v>
       </c>
     </row>
     <row r="232" spans="1:2">
@@ -2242,7 +2242,7 @@
         <v>43147</v>
       </c>
       <c r="B232">
-        <v>0.4818054</v>
+        <v>0.4580356</v>
       </c>
     </row>
     <row r="233" spans="1:2">
@@ -2250,7 +2250,7 @@
         <v>43148</v>
       </c>
       <c r="B233">
-        <v>0.481263</v>
+        <v>0.4580377</v>
       </c>
     </row>
     <row r="234" spans="1:2">
@@ -2258,7 +2258,7 @@
         <v>43149</v>
       </c>
       <c r="B234">
-        <v>0.4806378</v>
+        <v>0.458018</v>
       </c>
     </row>
     <row r="235" spans="1:2">
@@ -2266,7 +2266,7 @@
         <v>43150</v>
       </c>
       <c r="B235">
-        <v>0.479929</v>
+        <v>0.4579747</v>
       </c>
     </row>
     <row r="236" spans="1:2">
@@ -2274,7 +2274,7 @@
         <v>43151</v>
       </c>
       <c r="B236">
-        <v>0.4791359</v>
+        <v>0.4579059</v>
       </c>
     </row>
     <row r="237" spans="1:2">
@@ -2282,7 +2282,7 @@
         <v>43152</v>
       </c>
       <c r="B237">
-        <v>0.4782578</v>
+        <v>0.4578099</v>
       </c>
     </row>
     <row r="238" spans="1:2">
@@ -2290,7 +2290,7 @@
         <v>43153</v>
       </c>
       <c r="B238">
-        <v>0.4772938</v>
+        <v>0.4576845</v>
       </c>
     </row>
     <row r="239" spans="1:2">
@@ -2298,7 +2298,7 @@
         <v>43154</v>
       </c>
       <c r="B239">
-        <v>0.4762434</v>
+        <v>0.4575277</v>
       </c>
     </row>
     <row r="240" spans="1:2">
@@ -2306,7 +2306,7 @@
         <v>43155</v>
       </c>
       <c r="B240">
-        <v>0.4751056</v>
+        <v>0.4573376</v>
       </c>
     </row>
     <row r="241" spans="1:2">
@@ -2314,7 +2314,7 @@
         <v>43156</v>
       </c>
       <c r="B241">
-        <v>0.4738799</v>
+        <v>0.4571117</v>
       </c>
     </row>
     <row r="242" spans="1:2">
@@ -2322,7 +2322,7 @@
         <v>43157</v>
       </c>
       <c r="B242">
-        <v>0.4725655</v>
+        <v>0.4568481</v>
       </c>
     </row>
     <row r="243" spans="1:2">
@@ -2330,7 +2330,7 @@
         <v>43158</v>
       </c>
       <c r="B243">
-        <v>0.4711616</v>
+        <v>0.4565444</v>
       </c>
     </row>
     <row r="244" spans="1:2">
@@ -2338,7 +2338,7 @@
         <v>43159</v>
       </c>
       <c r="B244">
-        <v>0.4696675</v>
+        <v>0.4561984</v>
       </c>
     </row>
     <row r="245" spans="1:2">
@@ -2346,7 +2346,7 @@
         <v>43160</v>
       </c>
       <c r="B245">
-        <v>0.4680826</v>
+        <v>0.4558076</v>
       </c>
     </row>
     <row r="246" spans="1:2">
@@ -2354,7 +2354,7 @@
         <v>43161</v>
       </c>
       <c r="B246">
-        <v>0.466406</v>
+        <v>0.4553698</v>
       </c>
     </row>
     <row r="247" spans="1:2">
@@ -2362,7 +2362,7 @@
         <v>43162</v>
       </c>
       <c r="B247">
-        <v>0.4646372</v>
+        <v>0.4548827</v>
       </c>
     </row>
     <row r="248" spans="1:2">
@@ -2370,7 +2370,7 @@
         <v>43163</v>
       </c>
       <c r="B248">
-        <v>0.4627753</v>
+        <v>0.4543437</v>
       </c>
     </row>
     <row r="249" spans="1:2">
@@ -2378,7 +2378,7 @@
         <v>43164</v>
       </c>
       <c r="B249">
-        <v>0.4608196</v>
+        <v>0.4537504</v>
       </c>
     </row>
     <row r="250" spans="1:2">
@@ -2386,7 +2386,7 @@
         <v>43165</v>
       </c>
       <c r="B250">
-        <v>0.4587695</v>
+        <v>0.4531004</v>
       </c>
     </row>
     <row r="251" spans="1:2">
@@ -2394,7 +2394,7 @@
         <v>43166</v>
       </c>
       <c r="B251">
-        <v>0.4566243</v>
+        <v>0.4523913</v>
       </c>
     </row>
     <row r="252" spans="1:2">
@@ -2402,7 +2402,7 @@
         <v>43167</v>
       </c>
       <c r="B252">
-        <v>0.4543832</v>
+        <v>0.4516203</v>
       </c>
     </row>
     <row r="253" spans="1:2">
@@ -2410,7 +2410,7 @@
         <v>43168</v>
       </c>
       <c r="B253">
-        <v>0.4520455</v>
+        <v>0.4507851</v>
       </c>
     </row>
     <row r="254" spans="1:2">
@@ -2418,7 +2418,7 @@
         <v>43169</v>
       </c>
       <c r="B254">
-        <v>0.4496107</v>
+        <v>0.4498829</v>
       </c>
     </row>
     <row r="255" spans="1:2">
@@ -2426,7 +2426,7 @@
         <v>43170</v>
       </c>
       <c r="B255">
-        <v>0.4470778</v>
+        <v>0.4489111</v>
       </c>
     </row>
     <row r="256" spans="1:2">
@@ -2434,7 +2434,7 @@
         <v>43171</v>
       </c>
       <c r="B256">
-        <v>0.4444464</v>
+        <v>0.4478669</v>
       </c>
     </row>
     <row r="257" spans="1:2">
@@ -2442,7 +2442,7 @@
         <v>43172</v>
       </c>
       <c r="B257">
-        <v>0.4417156</v>
+        <v>0.4467476</v>
       </c>
     </row>
     <row r="258" spans="1:2">
@@ -2450,7 +2450,7 @@
         <v>43173</v>
       </c>
       <c r="B258">
-        <v>0.4388849</v>
+        <v>0.4455501</v>
       </c>
     </row>
     <row r="259" spans="1:2">
@@ -2458,7 +2458,7 @@
         <v>43174</v>
       </c>
       <c r="B259">
-        <v>0.4359534</v>
+        <v>0.4442714</v>
       </c>
     </row>
     <row r="260" spans="1:2">
@@ -2466,7 +2466,7 @@
         <v>43175</v>
       </c>
       <c r="B260">
-        <v>0.4329206</v>
+        <v>0.4429085</v>
       </c>
     </row>
     <row r="261" spans="1:2">
@@ -2474,7 +2474,7 @@
         <v>43176</v>
       </c>
       <c r="B261">
-        <v>0.4297858</v>
+        <v>0.441458</v>
       </c>
     </row>
     <row r="262" spans="1:2">
@@ -2482,7 +2482,7 @@
         <v>43177</v>
       </c>
       <c r="B262">
-        <v>0.4265482</v>
+        <v>0.4399164</v>
       </c>
     </row>
     <row r="263" spans="1:2">
@@ -2490,7 +2490,7 @@
         <v>43178</v>
       </c>
       <c r="B263">
-        <v>0.4232073</v>
+        <v>0.4382803</v>
       </c>
     </row>
     <row r="264" spans="1:2">
@@ -2498,7 +2498,7 @@
         <v>43179</v>
       </c>
       <c r="B264">
-        <v>0.4197623</v>
+        <v>0.4365457</v>
       </c>
     </row>
     <row r="265" spans="1:2">
@@ -2506,7 +2506,7 @@
         <v>43180</v>
       </c>
       <c r="B265">
-        <v>0.4162126</v>
+        <v>0.4347088</v>
       </c>
     </row>
     <row r="266" spans="1:2">
@@ -2514,7 +2514,7 @@
         <v>43181</v>
       </c>
       <c r="B266">
-        <v>0.4125576</v>
+        <v>0.4327652</v>
       </c>
     </row>
     <row r="267" spans="1:2">
@@ -2522,7 +2522,7 @@
         <v>43182</v>
       </c>
       <c r="B267">
-        <v>0.4087965</v>
+        <v>0.4307107</v>
       </c>
     </row>
     <row r="268" spans="1:2">
@@ -2530,7 +2530,7 @@
         <v>43183</v>
       </c>
       <c r="B268">
-        <v>0.4049287</v>
+        <v>0.4285405</v>
       </c>
     </row>
     <row r="269" spans="1:2">
@@ -2538,7 +2538,7 @@
         <v>43184</v>
       </c>
       <c r="B269">
-        <v>0.4009536</v>
+        <v>0.4262497</v>
       </c>
     </row>
     <row r="270" spans="1:2">
@@ -2546,7 +2546,7 @@
         <v>43185</v>
       </c>
       <c r="B270">
-        <v>0.3968704</v>
+        <v>0.4238332</v>
       </c>
     </row>
     <row r="271" spans="1:2">
@@ -2554,7 +2554,7 @@
         <v>43186</v>
       </c>
       <c r="B271">
-        <v>0.3926787</v>
+        <v>0.4212857</v>
       </c>
     </row>
     <row r="272" spans="1:2">
@@ -2562,7 +2562,7 @@
         <v>43187</v>
       </c>
       <c r="B272">
-        <v>0.3883776</v>
+        <v>0.4186017</v>
       </c>
     </row>
     <row r="273" spans="1:2">
@@ -2570,7 +2570,7 @@
         <v>43188</v>
       </c>
       <c r="B273">
-        <v>0.3839666</v>
+        <v>0.4157753</v>
       </c>
     </row>
     <row r="274" spans="1:2">
@@ -2578,7 +2578,7 @@
         <v>43189</v>
       </c>
       <c r="B274">
-        <v>0.379445</v>
+        <v>0.4128006</v>
       </c>
     </row>
     <row r="275" spans="1:2">
@@ -2586,7 +2586,7 @@
         <v>43190</v>
       </c>
       <c r="B275">
-        <v>0.3748122</v>
+        <v>0.4096716</v>
       </c>
     </row>
     <row r="276" spans="1:2">
@@ -2594,7 +2594,7 @@
         <v>43191</v>
       </c>
       <c r="B276">
-        <v>0.3700676</v>
+        <v>0.4063822</v>
       </c>
     </row>
     <row r="277" spans="1:2">
@@ -2602,7 +2602,7 @@
         <v>43192</v>
       </c>
       <c r="B277">
-        <v>0.3652104</v>
+        <v>0.4029264</v>
       </c>
     </row>
     <row r="278" spans="1:2">
@@ -2610,7 +2610,7 @@
         <v>43193</v>
       </c>
       <c r="B278">
-        <v>0.3602402</v>
+        <v>0.3992981</v>
       </c>
     </row>
     <row r="279" spans="1:2">
@@ -2618,7 +2618,7 @@
         <v>43194</v>
       </c>
       <c r="B279">
-        <v>0.3551562</v>
+        <v>0.3954915</v>
       </c>
     </row>
     <row r="280" spans="1:2">
@@ -2626,7 +2626,7 @@
         <v>43195</v>
       </c>
       <c r="B280">
-        <v>0.3499579</v>
+        <v>0.3915011</v>
       </c>
     </row>
     <row r="281" spans="1:2">
@@ -2634,7 +2634,7 @@
         <v>43196</v>
       </c>
       <c r="B281">
-        <v>0.3446446</v>
+        <v>0.3873219</v>
       </c>
     </row>
     <row r="282" spans="1:2">
@@ -2642,7 +2642,7 @@
         <v>43197</v>
       </c>
       <c r="B282">
-        <v>0.3392156</v>
+        <v>0.3829493</v>
       </c>
     </row>
     <row r="283" spans="1:2">
@@ -2650,7 +2650,7 @@
         <v>43198</v>
       </c>
       <c r="B283">
-        <v>0.3336705</v>
+        <v>0.3783798</v>
       </c>
     </row>
     <row r="284" spans="1:2">
@@ -2658,7 +2658,7 @@
         <v>43199</v>
       </c>
       <c r="B284">
-        <v>0.3280085</v>
+        <v>0.3736103</v>
       </c>
     </row>
     <row r="285" spans="1:2">
@@ -2666,7 +2666,7 @@
         <v>43200</v>
       </c>
       <c r="B285">
-        <v>0.3222291</v>
+        <v>0.3686394</v>
       </c>
     </row>
     <row r="286" spans="1:2">
@@ -2674,7 +2674,7 @@
         <v>43201</v>
       </c>
       <c r="B286">
-        <v>0.3163316</v>
+        <v>0.3634664</v>
       </c>
     </row>
     <row r="287" spans="1:2">
@@ -2682,7 +2682,7 @@
         <v>43202</v>
       </c>
       <c r="B287">
-        <v>0.3103154</v>
+        <v>0.3580927</v>
       </c>
     </row>
     <row r="288" spans="1:2">
@@ -2690,7 +2690,7 @@
         <v>43203</v>
       </c>
       <c r="B288">
-        <v>0.3041801</v>
+        <v>0.3525208</v>
       </c>
     </row>
     <row r="289" spans="1:2">
@@ -2698,7 +2698,7 @@
         <v>43204</v>
       </c>
       <c r="B289">
-        <v>0.2979248</v>
+        <v>0.3467553</v>
       </c>
     </row>
     <row r="290" spans="1:2">
@@ -2706,7 +2706,7 @@
         <v>43205</v>
       </c>
       <c r="B290">
-        <v>0.2915491</v>
+        <v>0.3408028</v>
       </c>
     </row>
     <row r="291" spans="1:2">
@@ -2714,7 +2714,7 @@
         <v>43206</v>
       </c>
       <c r="B291">
-        <v>0.2850523</v>
+        <v>0.334672</v>
       </c>
     </row>
     <row r="292" spans="1:2">
@@ -2722,7 +2722,7 @@
         <v>43207</v>
       </c>
       <c r="B292">
-        <v>0.2784339</v>
+        <v>0.3283735</v>
       </c>
     </row>
     <row r="293" spans="1:2">
@@ -2730,7 +2730,7 @@
         <v>43208</v>
       </c>
       <c r="B293">
-        <v>0.2716933</v>
+        <v>0.3219205</v>
       </c>
     </row>
     <row r="294" spans="1:2">
@@ -2738,7 +2738,7 @@
         <v>43209</v>
       </c>
       <c r="B294">
-        <v>0.2648298</v>
+        <v>0.315328</v>
       </c>
     </row>
     <row r="295" spans="1:2">
@@ -2746,7 +2746,7 @@
         <v>43210</v>
       </c>
       <c r="B295">
-        <v>0.257843</v>
+        <v>0.3086133</v>
       </c>
     </row>
     <row r="296" spans="1:2">
@@ -2754,7 +2754,7 @@
         <v>43211</v>
       </c>
       <c r="B296">
-        <v>0.2507322</v>
+        <v>0.3017956</v>
       </c>
     </row>
     <row r="297" spans="1:2">
@@ -2762,7 +2762,7 @@
         <v>43212</v>
       </c>
       <c r="B297">
-        <v>0.2434968</v>
+        <v>0.294896</v>
       </c>
     </row>
     <row r="298" spans="1:2">
@@ -2770,7 +2770,7 @@
         <v>43213</v>
       </c>
       <c r="B298">
-        <v>0.2361362</v>
+        <v>0.2879367</v>
       </c>
     </row>
     <row r="299" spans="1:2">
@@ -2778,7 +2778,7 @@
         <v>43214</v>
       </c>
       <c r="B299">
-        <v>0.22865</v>
+        <v>0.2809415</v>
       </c>
     </row>
     <row r="300" spans="1:2">
@@ -2786,7 +2786,7 @@
         <v>43215</v>
       </c>
       <c r="B300">
-        <v>0.2210375</v>
+        <v>0.2739348</v>
       </c>
     </row>
     <row r="301" spans="1:2">
@@ -2794,7 +2794,7 @@
         <v>43216</v>
       </c>
       <c r="B301">
-        <v>0.2132982</v>
+        <v>0.2669416</v>
       </c>
     </row>
     <row r="302" spans="1:2">
@@ -2802,7 +2802,7 @@
         <v>43217</v>
       </c>
       <c r="B302">
-        <v>0.2054314</v>
+        <v>0.2599867</v>
       </c>
     </row>
     <row r="303" spans="1:2">
@@ -2810,7 +2810,7 @@
         <v>43218</v>
       </c>
       <c r="B303">
-        <v>0.1974367</v>
+        <v>0.2530949</v>
       </c>
     </row>
     <row r="304" spans="1:2">
@@ -2818,7 +2818,7 @@
         <v>43219</v>
       </c>
       <c r="B304">
-        <v>0.1893135</v>
+        <v>0.2462898</v>
       </c>
     </row>
     <row r="305" spans="1:2">
@@ -2826,7 +2826,7 @@
         <v>43220</v>
       </c>
       <c r="B305">
-        <v>0.1810611</v>
+        <v>0.2395943</v>
       </c>
     </row>
     <row r="306" spans="1:2">
@@ -2834,7 +2834,7 @@
         <v>43221</v>
       </c>
       <c r="B306">
-        <v>0.1726792</v>
+        <v>0.2330295</v>
       </c>
     </row>
     <row r="307" spans="1:2">
@@ -2842,7 +2842,7 @@
         <v>43222</v>
       </c>
       <c r="B307">
-        <v>0.164167</v>
+        <v>0.226615</v>
       </c>
     </row>
     <row r="308" spans="1:2">
@@ -2850,7 +2850,7 @@
         <v>43223</v>
       </c>
       <c r="B308">
-        <v>0.1555241</v>
+        <v>0.2203683</v>
       </c>
     </row>
     <row r="309" spans="1:2">
@@ -2858,7 +2858,7 @@
         <v>43224</v>
       </c>
       <c r="B309">
-        <v>0.14675</v>
+        <v>0.2143046</v>
       </c>
     </row>
     <row r="310" spans="1:2">
@@ -2866,7 +2866,7 @@
         <v>43225</v>
       </c>
       <c r="B310">
-        <v>0.137844</v>
+        <v>0.208437</v>
       </c>
     </row>
     <row r="311" spans="1:2">
@@ -2874,7 +2874,7 @@
         <v>43226</v>
       </c>
       <c r="B311">
-        <v>0.1288056</v>
+        <v>0.2027763</v>
       </c>
     </row>
     <row r="312" spans="1:2">
@@ -2882,7 +2882,7 @@
         <v>43227</v>
       </c>
       <c r="B312">
-        <v>0.1196344</v>
+        <v>0.1973308</v>
       </c>
     </row>
     <row r="313" spans="1:2">
@@ -2890,7 +2890,7 @@
         <v>43228</v>
       </c>
       <c r="B313">
-        <v>0.1103297</v>
+        <v>0.1921068</v>
       </c>
     </row>
     <row r="314" spans="1:2">
@@ -2898,7 +2898,7 @@
         <v>43229</v>
       </c>
       <c r="B314">
-        <v>0.1008911</v>
+        <v>0.1871081</v>
       </c>
     </row>
     <row r="315" spans="1:2">
@@ -2906,7 +2906,7 @@
         <v>43230</v>
       </c>
       <c r="B315">
-        <v>0.09131789999999999</v>
+        <v>0.1823367</v>
       </c>
     </row>
     <row r="316" spans="1:2">
@@ -2914,7 +2914,7 @@
         <v>43231</v>
       </c>
       <c r="B316">
-        <v>0.0816098</v>
+        <v>0.1777926</v>
       </c>
     </row>
     <row r="317" spans="1:2">
@@ -2922,7 +2922,7 @@
         <v>43232</v>
       </c>
       <c r="B317">
-        <v>0.0717661</v>
+        <v>0.1734744</v>
       </c>
     </row>
     <row r="318" spans="1:2">
@@ -2930,7 +2930,7 @@
         <v>43233</v>
       </c>
       <c r="B318">
-        <v>0.0617863</v>
+        <v>0.1693788</v>
       </c>
     </row>
     <row r="319" spans="1:2">
@@ -2938,7 +2938,7 @@
         <v>43234</v>
       </c>
       <c r="B319">
-        <v>0.05167</v>
+        <v>0.1655014</v>
       </c>
     </row>
     <row r="320" spans="1:2">
@@ -2946,7 +2946,7 @@
         <v>43235</v>
       </c>
       <c r="B320">
-        <v>0.0414165</v>
+        <v>0.1618368</v>
       </c>
     </row>
     <row r="321" spans="1:2">
@@ -2954,7 +2954,7 @@
         <v>43236</v>
       </c>
       <c r="B321">
-        <v>0.0310255</v>
+        <v>0.1583787</v>
       </c>
     </row>
     <row r="322" spans="1:2">
@@ -2962,7 +2962,7 @@
         <v>43237</v>
       </c>
       <c r="B322">
-        <v>0.0204964</v>
+        <v>0.1551198</v>
       </c>
     </row>
     <row r="323" spans="1:2">
@@ -2970,7 +2970,7 @@
         <v>43238</v>
       </c>
       <c r="B323">
-        <v>0.0098286</v>
+        <v>0.1520526</v>
       </c>
     </row>
     <row r="324" spans="1:2">
@@ -2978,7 +2978,7 @@
         <v>43239</v>
       </c>
       <c r="B324">
-        <v>0.0098286</v>
+        <v>0.1491689</v>
       </c>
     </row>
     <row r="325" spans="1:2">
@@ -2986,7 +2986,7 @@
         <v>43240</v>
       </c>
       <c r="B325">
-        <v>0.0098286</v>
+        <v>0.1464606</v>
       </c>
     </row>
     <row r="326" spans="1:2">
@@ -2994,7 +2994,7 @@
         <v>43241</v>
       </c>
       <c r="B326">
-        <v>0.0098286</v>
+        <v>0.143919</v>
       </c>
     </row>
     <row r="327" spans="1:2">
@@ -3002,7 +3002,7 @@
         <v>43242</v>
       </c>
       <c r="B327">
-        <v>0.0098286</v>
+        <v>0.1415359</v>
       </c>
     </row>
     <row r="328" spans="1:2">
@@ -3010,7 +3010,7 @@
         <v>43243</v>
       </c>
       <c r="B328">
-        <v>0.0098286</v>
+        <v>0.1393027</v>
       </c>
     </row>
     <row r="329" spans="1:2">
@@ -3018,7 +3018,7 @@
         <v>43244</v>
       </c>
       <c r="B329">
-        <v>0.0098286</v>
+        <v>0.1372111</v>
       </c>
     </row>
     <row r="330" spans="1:2">
@@ -3026,7 +3026,7 @@
         <v>43245</v>
       </c>
       <c r="B330">
-        <v>0.0098286</v>
+        <v>0.135253</v>
       </c>
     </row>
     <row r="331" spans="1:2">
@@ -3034,7 +3034,7 @@
         <v>43246</v>
       </c>
       <c r="B331">
-        <v>0.0098286</v>
+        <v>0.1334205</v>
       </c>
     </row>
     <row r="332" spans="1:2">
@@ -3042,7 +3042,7 @@
         <v>43247</v>
       </c>
       <c r="B332">
-        <v>0.0098286</v>
+        <v>0.1317062</v>
       </c>
     </row>
     <row r="333" spans="1:2">
@@ -3050,7 +3050,7 @@
         <v>43248</v>
       </c>
       <c r="B333">
-        <v>0.0098286</v>
+        <v>0.1301025</v>
       </c>
     </row>
     <row r="334" spans="1:2">
@@ -3058,7 +3058,7 @@
         <v>43249</v>
       </c>
       <c r="B334">
-        <v>0.0098286</v>
+        <v>0.1286027</v>
       </c>
     </row>
     <row r="335" spans="1:2">
@@ -3066,7 +3066,7 @@
         <v>43250</v>
       </c>
       <c r="B335">
-        <v>0.0098286</v>
+        <v>0.1271999</v>
       </c>
     </row>
     <row r="336" spans="1:2">
@@ -3074,7 +3074,7 @@
         <v>43251</v>
       </c>
       <c r="B336">
-        <v>0.0098286</v>
+        <v>0.125888</v>
       </c>
     </row>
     <row r="337" spans="1:2">
@@ -3082,7 +3082,7 @@
         <v>43252</v>
       </c>
       <c r="B337">
-        <v>0.0098286</v>
+        <v>0.124661</v>
       </c>
     </row>
     <row r="338" spans="1:2">
@@ -3090,7 +3090,7 @@
         <v>43253</v>
       </c>
       <c r="B338">
-        <v>0.0098286</v>
+        <v>0.1235132</v>
       </c>
     </row>
     <row r="339" spans="1:2">
@@ -3098,7 +3098,7 @@
         <v>43254</v>
       </c>
       <c r="B339">
-        <v>0.0098286</v>
+        <v>0.1224393</v>
       </c>
     </row>
     <row r="340" spans="1:2">
@@ -3106,7 +3106,7 @@
         <v>43255</v>
       </c>
       <c r="B340">
-        <v>0.0098286</v>
+        <v>0.1214343</v>
       </c>
     </row>
     <row r="341" spans="1:2">
@@ -3114,7 +3114,7 @@
         <v>43256</v>
       </c>
       <c r="B341">
-        <v>0.0098286</v>
+        <v>0.1204937</v>
       </c>
     </row>
     <row r="342" spans="1:2">
@@ -3122,7 +3122,7 @@
         <v>43257</v>
       </c>
       <c r="B342">
-        <v>0.0098286</v>
+        <v>0.1196129</v>
       </c>
     </row>
     <row r="343" spans="1:2">
@@ -3130,7 +3130,7 @@
         <v>43258</v>
       </c>
       <c r="B343">
-        <v>0.0098286</v>
+        <v>0.118788</v>
       </c>
     </row>
     <row r="344" spans="1:2">
@@ -3138,7 +3138,7 @@
         <v>43259</v>
       </c>
       <c r="B344">
-        <v>0.0098286</v>
+        <v>0.1180151</v>
       </c>
     </row>
     <row r="345" spans="1:2">
@@ -3146,7 +3146,7 @@
         <v>43260</v>
       </c>
       <c r="B345">
-        <v>0.0098286</v>
+        <v>0.1172906</v>
       </c>
     </row>
     <row r="346" spans="1:2">
@@ -3154,7 +3154,7 @@
         <v>43261</v>
       </c>
       <c r="B346">
-        <v>0.0098286</v>
+        <v>0.1166113</v>
       </c>
     </row>
     <row r="347" spans="1:2">
@@ -3162,7 +3162,7 @@
         <v>43262</v>
       </c>
       <c r="B347">
-        <v>0.0098286</v>
+        <v>0.115974</v>
       </c>
     </row>
     <row r="348" spans="1:2">
@@ -3170,7 +3170,7 @@
         <v>43263</v>
       </c>
       <c r="B348">
-        <v>0.0098286</v>
+        <v>0.1153759</v>
       </c>
     </row>
     <row r="349" spans="1:2">
@@ -3178,7 +3178,7 @@
         <v>43264</v>
       </c>
       <c r="B349">
-        <v>0.0098286</v>
+        <v>0.1148143</v>
       </c>
     </row>
     <row r="350" spans="1:2">
@@ -3186,7 +3186,7 @@
         <v>43265</v>
       </c>
       <c r="B350">
-        <v>0.0098286</v>
+        <v>0.1142868</v>
       </c>
     </row>
     <row r="351" spans="1:2">
@@ -3194,7 +3194,7 @@
         <v>43266</v>
       </c>
       <c r="B351">
-        <v>0.0098286</v>
+        <v>0.113791</v>
       </c>
     </row>
     <row r="352" spans="1:2">
@@ -3202,7 +3202,7 @@
         <v>43267</v>
       </c>
       <c r="B352">
-        <v>0.0098286</v>
+        <v>0.1133247</v>
       </c>
     </row>
     <row r="353" spans="1:2">
@@ -3210,7 +3210,7 @@
         <v>43268</v>
       </c>
       <c r="B353">
-        <v>0.0098286</v>
+        <v>0.1128861</v>
       </c>
     </row>
     <row r="354" spans="1:2">
@@ -3218,7 +3218,7 @@
         <v>43269</v>
       </c>
       <c r="B354">
-        <v>0.0098286</v>
+        <v>0.1124732</v>
       </c>
     </row>
     <row r="355" spans="1:2">
@@ -3226,7 +3226,7 @@
         <v>43270</v>
       </c>
       <c r="B355">
-        <v>0.0098286</v>
+        <v>0.1120844</v>
       </c>
     </row>
     <row r="356" spans="1:2">
@@ -3234,7 +3234,7 @@
         <v>43271</v>
       </c>
       <c r="B356">
-        <v>0.0098286</v>
+        <v>0.111718</v>
       </c>
     </row>
     <row r="357" spans="1:2">
@@ -3242,7 +3242,7 @@
         <v>43272</v>
       </c>
       <c r="B357">
-        <v>0.0098286</v>
+        <v>0.1113726</v>
       </c>
     </row>
     <row r="358" spans="1:2">
@@ -3250,7 +3250,7 @@
         <v>43273</v>
       </c>
       <c r="B358">
-        <v>0.0098286</v>
+        <v>0.1110467</v>
       </c>
     </row>
     <row r="359" spans="1:2">
@@ -3258,7 +3258,7 @@
         <v>43274</v>
       </c>
       <c r="B359">
-        <v>0.0098286</v>
+        <v>0.1107392</v>
       </c>
     </row>
     <row r="360" spans="1:2">
@@ -3266,7 +3266,7 @@
         <v>43275</v>
       </c>
       <c r="B360">
-        <v>0.0098286</v>
+        <v>0.1104489</v>
       </c>
     </row>
     <row r="361" spans="1:2">
@@ -3274,7 +3274,7 @@
         <v>43276</v>
       </c>
       <c r="B361">
-        <v>0.0098286</v>
+        <v>0.1101745</v>
       </c>
     </row>
     <row r="362" spans="1:2">
@@ -3282,7 +3282,7 @@
         <v>43277</v>
       </c>
       <c r="B362">
-        <v>0.0098286</v>
+        <v>0.1099152</v>
       </c>
     </row>
     <row r="363" spans="1:2">
@@ -3290,7 +3290,7 @@
         <v>43278</v>
       </c>
       <c r="B363">
-        <v>0.0098286</v>
+        <v>0.10967</v>
       </c>
     </row>
     <row r="364" spans="1:2">
@@ -3298,7 +3298,7 @@
         <v>43279</v>
       </c>
       <c r="B364">
-        <v>0.0098286</v>
+        <v>0.109438</v>
       </c>
     </row>
     <row r="365" spans="1:2">
@@ -3306,7 +3306,7 @@
         <v>43280</v>
       </c>
       <c r="B365">
-        <v>0.0098286</v>
+        <v>0.1092183</v>
       </c>
     </row>
     <row r="366" spans="1:2">
@@ -3314,7 +3314,7 @@
         <v>43281</v>
       </c>
       <c r="B366">
-        <v>0.0098286</v>
+        <v>0.1090103</v>
       </c>
     </row>
     <row r="367" spans="1:2">
@@ -3322,7 +3322,7 @@
         <v>43282</v>
       </c>
       <c r="B367">
-        <v>0.0098286</v>
+        <v>0.1088131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>